<commit_message>
Add FET for NASA RMC motor controller, create TDFN-8-5x6 footprint
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16822" uniqueCount="6880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16833" uniqueCount="6886">
   <si>
     <t>Part Number</t>
   </si>
@@ -20671,6 +20671,24 @@
   </si>
   <si>
     <t>IRF540NPBF</t>
+  </si>
+  <si>
+    <t>XSTR-00049</t>
+  </si>
+  <si>
+    <t>XSTR, MOSFET N-Channel, 40V 100A TDFN-8</t>
+  </si>
+  <si>
+    <t>83W</t>
+  </si>
+  <si>
+    <t>BSC027N04LS</t>
+  </si>
+  <si>
+    <t>TDFN-8-5x6</t>
+  </si>
+  <si>
+    <t>n-mosfet-SSSGD</t>
   </si>
 </sst>
 </file>
@@ -43671,10 +43689,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45536,6 +45554,44 @@
       </c>
       <c r="L50" s="8">
         <v>0.95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>6880</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6881</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2101</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4647</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6882</v>
+      </c>
+      <c r="F51" t="s">
+        <v>4650</v>
+      </c>
+      <c r="G51" t="s">
+        <v>2496</v>
+      </c>
+      <c r="H51" t="s">
+        <v>2299</v>
+      </c>
+      <c r="I51" t="s">
+        <v>6883</v>
+      </c>
+      <c r="J51" t="s">
+        <v>6884</v>
+      </c>
+      <c r="K51" t="s">
+        <v>6885</v>
+      </c>
+      <c r="L51" s="8">
+        <v>1.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many updates, including the Raspberry Pi 4 Compute Module
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16833" uniqueCount="6886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16884" uniqueCount="6915">
   <si>
     <t>Part Number</t>
   </si>
@@ -20689,6 +20689,93 @@
   </si>
   <si>
     <t>n-mosfet-SSSGD</t>
+  </si>
+  <si>
+    <t>CONN-00100</t>
+  </si>
+  <si>
+    <t>Terminal Blk, 4 Pos, 16A, 5.08mm Pitch, Screwless, Horizontal, 12-24AWG</t>
+  </si>
+  <si>
+    <t>TE_CONN_1986712-4</t>
+  </si>
+  <si>
+    <t>1986712-4</t>
+  </si>
+  <si>
+    <t>IFACE-00031</t>
+  </si>
+  <si>
+    <t>IC, RS-232 Transceiver, Dual Channel, SOIC-16</t>
+  </si>
+  <si>
+    <t>Maxim Integrated</t>
+  </si>
+  <si>
+    <t>MAX232CSE+</t>
+  </si>
+  <si>
+    <t>MAX232</t>
+  </si>
+  <si>
+    <t>CONN-00101</t>
+  </si>
+  <si>
+    <t>Header, 18x1, 0.1", Vertical</t>
+  </si>
+  <si>
+    <t>conn-18x1_0</t>
+  </si>
+  <si>
+    <t>TSW-118-07-G-S</t>
+  </si>
+  <si>
+    <t>HDDR_18x1_0</t>
+  </si>
+  <si>
+    <t>CAP-00583</t>
+  </si>
+  <si>
+    <t>T491D227K016AT</t>
+  </si>
+  <si>
+    <t>CHIP_2917_KEMET_T491D</t>
+  </si>
+  <si>
+    <t>T495X227K016ATE100</t>
+  </si>
+  <si>
+    <t>CAP-00584</t>
+  </si>
+  <si>
+    <t>ANLG-00079</t>
+  </si>
+  <si>
+    <t>IC, 7 NPN Darlington Array, 50V 500mA</t>
+  </si>
+  <si>
+    <t>ULN2003AD</t>
+  </si>
+  <si>
+    <t>ULN200xA</t>
+  </si>
+  <si>
+    <t>MISC-00060</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Foundation</t>
+  </si>
+  <si>
+    <t>RPI_CM4</t>
+  </si>
+  <si>
+    <t>RPI_CM4_3MM</t>
+  </si>
+  <si>
+    <t>CM4004032</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4 Compute Module, CM4, 4GB DDR4, 32 GB eMMC</t>
   </si>
 </sst>
 </file>
@@ -42319,10 +42406,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43681,6 +43768,29 @@
         <v>0.13</v>
       </c>
     </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>6909</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6914</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6910</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6913</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6912</v>
+      </c>
+      <c r="F62" t="s">
+        <v>6911</v>
+      </c>
+      <c r="G62" s="8">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -43691,8 +43801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48493,10 +48603,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J102" sqref="J102"/>
+    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51742,6 +51852,73 @@
         <v>1.64</v>
       </c>
     </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>6886</v>
+      </c>
+      <c r="B102" t="s">
+        <v>6887</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2383</v>
+      </c>
+      <c r="D102">
+        <v>4</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102" t="s">
+        <v>6681</v>
+      </c>
+      <c r="G102" t="s">
+        <v>2979</v>
+      </c>
+      <c r="H102" t="s">
+        <v>6889</v>
+      </c>
+      <c r="I102" t="s">
+        <v>6888</v>
+      </c>
+      <c r="J102" t="s">
+        <v>2957</v>
+      </c>
+      <c r="K102" s="8">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>6895</v>
+      </c>
+      <c r="B103" t="s">
+        <v>6896</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D103">
+        <v>18</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="G103" t="s">
+        <v>4738</v>
+      </c>
+      <c r="H103" t="s">
+        <v>6898</v>
+      </c>
+      <c r="I103" t="s">
+        <v>6899</v>
+      </c>
+      <c r="J103" t="s">
+        <v>6897</v>
+      </c>
+      <c r="K103" s="8">
+        <v>1.66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -51750,10 +51927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K584"/>
+  <dimension ref="A1:K586"/>
   <sheetViews>
-    <sheetView topLeftCell="A559" workbookViewId="0">
-      <selection activeCell="I585" sqref="I585"/>
+    <sheetView topLeftCell="A575" workbookViewId="0">
+      <selection activeCell="K587" sqref="K587"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -71133,6 +71310,78 @@
       </c>
       <c r="K584" s="8">
         <v>0.32</v>
+      </c>
+    </row>
+    <row r="585" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A585" t="s">
+        <v>6900</v>
+      </c>
+      <c r="B585" t="str">
+        <f>CONCATENATE("CAP",", ",C585,", ",D585,", ",E585,", ",F585,", 2917")</f>
+        <v>CAP, 220uF, ±10%, 16V, Tantalum, 2917</v>
+      </c>
+      <c r="C585" t="s">
+        <v>1824</v>
+      </c>
+      <c r="D585" t="s">
+        <v>4345</v>
+      </c>
+      <c r="E585" t="s">
+        <v>19</v>
+      </c>
+      <c r="F585" t="s">
+        <v>4971</v>
+      </c>
+      <c r="G585" t="s">
+        <v>4806</v>
+      </c>
+      <c r="H585" t="s">
+        <v>6901</v>
+      </c>
+      <c r="I585" t="s">
+        <v>6902</v>
+      </c>
+      <c r="J585" t="s">
+        <v>2080</v>
+      </c>
+      <c r="K585" s="8">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="586" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A586" t="s">
+        <v>6904</v>
+      </c>
+      <c r="B586" t="str">
+        <f>CONCATENATE("CAP",", ",C586,", ",D586,", ",E586,", ",F586,", 100mOhm, 2917")</f>
+        <v>CAP, 220uF, ±10%, 16V, Tantalum, 100mOhm, 2917</v>
+      </c>
+      <c r="C586" t="s">
+        <v>1824</v>
+      </c>
+      <c r="D586" t="s">
+        <v>4345</v>
+      </c>
+      <c r="E586" t="s">
+        <v>19</v>
+      </c>
+      <c r="F586" t="s">
+        <v>4971</v>
+      </c>
+      <c r="G586" t="s">
+        <v>4806</v>
+      </c>
+      <c r="H586" t="s">
+        <v>6903</v>
+      </c>
+      <c r="I586" t="s">
+        <v>5490</v>
+      </c>
+      <c r="J586" t="s">
+        <v>2080</v>
+      </c>
+      <c r="K586" s="8">
+        <v>2.57</v>
       </c>
     </row>
   </sheetData>
@@ -75992,10 +76241,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76720,6 +76969,29 @@
       </c>
       <c r="G32" s="8">
         <v>4.05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>6890</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6891</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6892</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6893</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5505</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6894</v>
+      </c>
+      <c r="G33" s="8">
+        <v>2.92</v>
       </c>
     </row>
   </sheetData>
@@ -79385,10 +79657,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -81204,6 +81476,29 @@
       </c>
       <c r="G80" s="8">
         <v>4.01</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>6905</v>
+      </c>
+      <c r="B81" t="s">
+        <v>6906</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6907</v>
+      </c>
+      <c r="E81" t="s">
+        <v>5505</v>
+      </c>
+      <c r="F81" t="s">
+        <v>6908</v>
+      </c>
+      <c r="G81" s="8">
+        <v>0.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to various things
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16884" uniqueCount="6915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16904" uniqueCount="6928">
   <si>
     <t>Part Number</t>
   </si>
@@ -20776,6 +20776,45 @@
   </si>
   <si>
     <t>Raspberry Pi 4 Compute Module, CM4, 4GB DDR4, 32 GB eMMC</t>
+  </si>
+  <si>
+    <t>M2012TXG41-DC</t>
+  </si>
+  <si>
+    <t>CONN-00102</t>
+  </si>
+  <si>
+    <t>Terminal Blk Header, 2 Pos, 5.08mm, 12A, Right-Angle</t>
+  </si>
+  <si>
+    <t>PHOENIX_1757242</t>
+  </si>
+  <si>
+    <t>CONN-00103</t>
+  </si>
+  <si>
+    <t>USB-A Jack x1, USB 3.x, Vertical, Thru-Hole</t>
+  </si>
+  <si>
+    <t>AMPHENOL_GSB412137CHR</t>
+  </si>
+  <si>
+    <t>usb_a_3.0_x1</t>
+  </si>
+  <si>
+    <t>GSB412137CHR</t>
+  </si>
+  <si>
+    <t>ANLG-00080</t>
+  </si>
+  <si>
+    <t>IC, DAC, 8-bit, Rail-Rail Output, SPI, 2.7~5.5V</t>
+  </si>
+  <si>
+    <t>DAC081</t>
+  </si>
+  <si>
+    <t>DAC081S101CIMK</t>
   </si>
 </sst>
 </file>
@@ -42408,8 +42447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42654,7 +42693,7 @@
         <v>4478</v>
       </c>
       <c r="E11" t="s">
-        <v>4478</v>
+        <v>6915</v>
       </c>
       <c r="F11" t="s">
         <v>4479</v>
@@ -48603,10 +48642,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51917,6 +51956,73 @@
       </c>
       <c r="K103" s="8">
         <v>1.66</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>6916</v>
+      </c>
+      <c r="B104" t="s">
+        <v>6917</v>
+      </c>
+      <c r="C104" t="s">
+        <v>2383</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104" t="s">
+        <v>6729</v>
+      </c>
+      <c r="G104" t="s">
+        <v>2381</v>
+      </c>
+      <c r="H104">
+        <v>1757242</v>
+      </c>
+      <c r="I104" t="s">
+        <v>6918</v>
+      </c>
+      <c r="J104" t="s">
+        <v>2391</v>
+      </c>
+      <c r="K104" s="8">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>6919</v>
+      </c>
+      <c r="B105" t="s">
+        <v>6920</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5801</v>
+      </c>
+      <c r="D105">
+        <v>9</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="G105" t="s">
+        <v>2908</v>
+      </c>
+      <c r="H105" t="s">
+        <v>6923</v>
+      </c>
+      <c r="I105" t="s">
+        <v>6921</v>
+      </c>
+      <c r="J105" t="s">
+        <v>6922</v>
+      </c>
+      <c r="K105" s="8">
+        <v>1.59</v>
       </c>
     </row>
   </sheetData>
@@ -79657,10 +79763,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -81499,6 +81605,29 @@
       </c>
       <c r="G81" s="8">
         <v>0.49</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>6924</v>
+      </c>
+      <c r="B82" t="s">
+        <v>6925</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6927</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6213</v>
+      </c>
+      <c r="F82" t="s">
+        <v>6926</v>
+      </c>
+      <c r="G82" s="8">
+        <v>1.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Late October updates, including updates for NASA RMC BMS
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16904" uniqueCount="6928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16975" uniqueCount="6964">
   <si>
     <t>Part Number</t>
   </si>
@@ -20815,6 +20815,114 @@
   </si>
   <si>
     <t>DAC081S101CIMK</t>
+  </si>
+  <si>
+    <t>V40PWM10C-M3/I</t>
+  </si>
+  <si>
+    <t>schottky_dual_KAA</t>
+  </si>
+  <si>
+    <t>DPAK_SLIM</t>
+  </si>
+  <si>
+    <t>0.89V</t>
+  </si>
+  <si>
+    <t>DIO-00081</t>
+  </si>
+  <si>
+    <t>Dio, Schottky Array, Dual, Common Cathode, 100V 20A, SLIM DPAK</t>
+  </si>
+  <si>
+    <t>XSTR-00050</t>
+  </si>
+  <si>
+    <t>XSTR, MOSFET P-Channel, 80V 110A, D2PAK</t>
+  </si>
+  <si>
+    <t>110A</t>
+  </si>
+  <si>
+    <t>SUM110P08-11L-E3</t>
+  </si>
+  <si>
+    <t>BZX585-C16,115</t>
+  </si>
+  <si>
+    <t>DIO-00082</t>
+  </si>
+  <si>
+    <t>Dio, Zener, 16V 300mW, SOD-523</t>
+  </si>
+  <si>
+    <t>MAG-00132</t>
+  </si>
+  <si>
+    <t>Xfmr, 2:1 Center-Tapped, 388uH, SMD</t>
+  </si>
+  <si>
+    <t>388uH</t>
+  </si>
+  <si>
+    <t>160mA</t>
+  </si>
+  <si>
+    <t>189mOhm</t>
+  </si>
+  <si>
+    <t>WURTH_750315228</t>
+  </si>
+  <si>
+    <t>xfmr_ct</t>
+  </si>
+  <si>
+    <t>PWREG-00064</t>
+  </si>
+  <si>
+    <t>2.25 ~ 5.5V</t>
+  </si>
+  <si>
+    <t>Xfmr Driver</t>
+  </si>
+  <si>
+    <t>SN6505</t>
+  </si>
+  <si>
+    <t>SN6505B</t>
+  </si>
+  <si>
+    <t>IC, 1A Transformer Driver, Push-Pull, Soft-Start Enabled</t>
+  </si>
+  <si>
+    <t>DIO-00083</t>
+  </si>
+  <si>
+    <t>LED, Green, SMD Right-Angle, Low-Current, Kingbright HELI2 Series</t>
+  </si>
+  <si>
+    <t>102.5mW</t>
+  </si>
+  <si>
+    <t>25mA</t>
+  </si>
+  <si>
+    <t>APA2107LZGCK</t>
+  </si>
+  <si>
+    <t>APA2107</t>
+  </si>
+  <si>
+    <t>CAP-00585</t>
+  </si>
+  <si>
+    <t>Knowles Novacap</t>
+  </si>
+  <si>
+    <t>LS1808N101K302NTM</t>
+  </si>
+  <si>
+    <t>250VAC</t>
   </si>
 </sst>
 </file>
@@ -43838,10 +43946,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45743,6 +45851,44 @@
         <v>1.19</v>
       </c>
     </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>6934</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6935</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4646</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6936</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2297</v>
+      </c>
+      <c r="F52" t="s">
+        <v>6355</v>
+      </c>
+      <c r="G52" t="s">
+        <v>4979</v>
+      </c>
+      <c r="H52" t="s">
+        <v>5581</v>
+      </c>
+      <c r="I52" t="s">
+        <v>6937</v>
+      </c>
+      <c r="J52" t="s">
+        <v>5381</v>
+      </c>
+      <c r="K52" t="s">
+        <v>5707</v>
+      </c>
+      <c r="L52" s="8">
+        <v>4.43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -45751,10 +45897,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView topLeftCell="C64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K83" sqref="K83"/>
+    <sheetView topLeftCell="C67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M86" sqref="M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48631,6 +48777,120 @@
       </c>
       <c r="M82" s="8">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>6932</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>6933</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>6931</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>4601</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>2431</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>6928</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>6930</v>
+      </c>
+      <c r="L83" s="2" t="s">
+        <v>6929</v>
+      </c>
+      <c r="M83" s="8">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>6939</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>6940</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>4545</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>4744</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>2134</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>2939</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>2131</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>4826</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>6938</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>2184</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>2130</v>
+      </c>
+      <c r="M84" s="8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>6954</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>6955</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>5158</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>2945</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>6956</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>6957</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>2497</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>4632</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>6958</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>6959</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>2502</v>
+      </c>
+      <c r="M85" s="8">
+        <v>0.51</v>
       </c>
     </row>
   </sheetData>
@@ -52033,10 +52293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K586"/>
+  <dimension ref="A1:K587"/>
   <sheetViews>
-    <sheetView topLeftCell="A575" workbookViewId="0">
-      <selection activeCell="K587" sqref="K587"/>
+    <sheetView tabSelected="1" topLeftCell="A575" workbookViewId="0">
+      <selection activeCell="B588" sqref="B588"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -71490,6 +71750,42 @@
         <v>2.57</v>
       </c>
     </row>
+    <row r="587" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A587" t="s">
+        <v>6960</v>
+      </c>
+      <c r="B587" t="str">
+        <f>CONCATENATE("CAP",", ",C587,", ",D587,", ",E587,", ",F587,", X2/Y3, 1808")</f>
+        <v>CAP, 100pF, ±5%, 250VAC, C0G, X2/Y3, 1808</v>
+      </c>
+      <c r="C587" t="s">
+        <v>2799</v>
+      </c>
+      <c r="D587" t="s">
+        <v>6231</v>
+      </c>
+      <c r="E587" t="s">
+        <v>6963</v>
+      </c>
+      <c r="F587" t="s">
+        <v>2614</v>
+      </c>
+      <c r="G587" t="s">
+        <v>6961</v>
+      </c>
+      <c r="H587" t="s">
+        <v>6962</v>
+      </c>
+      <c r="I587" t="s">
+        <v>4808</v>
+      </c>
+      <c r="J587" t="s">
+        <v>23</v>
+      </c>
+      <c r="K587" s="8">
+        <v>0.78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -71498,10 +71794,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N133"/>
+  <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="L134" sqref="L134"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76045,6 +76341,38 @@
       </c>
       <c r="M133" s="8">
         <v>4.18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>6941</v>
+      </c>
+      <c r="B134" t="s">
+        <v>6942</v>
+      </c>
+      <c r="C134" t="s">
+        <v>6943</v>
+      </c>
+      <c r="E134" t="s">
+        <v>6944</v>
+      </c>
+      <c r="H134" t="s">
+        <v>6945</v>
+      </c>
+      <c r="I134" t="s">
+        <v>2421</v>
+      </c>
+      <c r="J134">
+        <v>750315228</v>
+      </c>
+      <c r="K134" t="s">
+        <v>6946</v>
+      </c>
+      <c r="L134" t="s">
+        <v>6947</v>
+      </c>
+      <c r="M134" s="8">
+        <v>2.4</v>
       </c>
     </row>
   </sheetData>
@@ -77427,10 +77755,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -79755,6 +80083,41 @@
         <v>1.57</v>
       </c>
     </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>6948</v>
+      </c>
+      <c r="B66" t="s">
+        <v>6953</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6949</v>
+      </c>
+      <c r="E66" t="s">
+        <v>70</v>
+      </c>
+      <c r="G66" t="s">
+        <v>6950</v>
+      </c>
+      <c r="H66" t="s">
+        <v>73</v>
+      </c>
+      <c r="I66" t="s">
+        <v>2288</v>
+      </c>
+      <c r="J66" t="s">
+        <v>6952</v>
+      </c>
+      <c r="K66" t="s">
+        <v>2559</v>
+      </c>
+      <c r="L66" t="s">
+        <v>6951</v>
+      </c>
+      <c r="M66" s="8">
+        <v>2.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -79765,7 +80128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add WS2812B, 4-pin 5050 LED footprint, and a few other parts
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17000" uniqueCount="6973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17014" uniqueCount="6983">
   <si>
     <t>Part Number</t>
   </si>
@@ -19059,9 +19059,6 @@
     <t>PTC Fuse (Polyfuse), 24V 500mA Hold, 1A Trip, 100ms</t>
   </si>
   <si>
-    <t>PTC RESET FUSE 24V 500MA 1206</t>
-  </si>
-  <si>
     <t>ANLG-00064</t>
   </si>
   <si>
@@ -20950,6 +20947,39 @@
   </si>
   <si>
     <t>C4520C0G3F100F085KA</t>
+  </si>
+  <si>
+    <t>0ZCJ0050AF2E</t>
+  </si>
+  <si>
+    <t>CONN-00104</t>
+  </si>
+  <si>
+    <t>Barrier Block, 2-Pos, 30A 600V, 11.12mm Pitch</t>
+  </si>
+  <si>
+    <t>8PCV-02-006</t>
+  </si>
+  <si>
+    <t>TE_CONN_8PCV-02-006</t>
+  </si>
+  <si>
+    <t>MISC-00061</t>
+  </si>
+  <si>
+    <t>WS2812B</t>
+  </si>
+  <si>
+    <t>5050_4</t>
+  </si>
+  <si>
+    <t>ws2812b</t>
+  </si>
+  <si>
+    <t>World Semi</t>
+  </si>
+  <si>
+    <t>WS2812B, Intelligent RGB LED Chip, 3.5~5.3V, 5x5mm (5050) SMD</t>
   </si>
 </sst>
 </file>
@@ -21322,8 +21352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A704" workbookViewId="0">
-      <selection activeCell="B730" sqref="B730"/>
+    <sheetView topLeftCell="A700" workbookViewId="0">
+      <selection activeCell="K709" sqref="K709"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21454,7 +21484,7 @@
         <v>2612</v>
       </c>
       <c r="H4" t="s">
-        <v>2373</v>
+        <v>2440</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
@@ -21483,7 +21513,7 @@
         <v>2372</v>
       </c>
       <c r="H5" t="s">
-        <v>2373</v>
+        <v>2440</v>
       </c>
       <c r="I5" t="s">
         <v>12</v>
@@ -41524,7 +41554,7 @@
         <v>5969</v>
       </c>
       <c r="H710" t="s">
-        <v>2373</v>
+        <v>2440</v>
       </c>
       <c r="I710" t="s">
         <v>12</v>
@@ -41855,7 +41885,7 @@
     </row>
     <row r="721" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A721" t="s">
-        <v>6599</v>
+        <v>6598</v>
       </c>
       <c r="B721" t="s">
         <v>6338</v>
@@ -41887,25 +41917,25 @@
     </row>
     <row r="722" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A722" t="s">
-        <v>6628</v>
+        <v>6627</v>
       </c>
       <c r="B722" t="s">
-        <v>6600</v>
+        <v>6599</v>
       </c>
       <c r="C722">
         <v>0</v>
       </c>
       <c r="D722" t="s">
-        <v>6603</v>
+        <v>6602</v>
       </c>
       <c r="E722" s="12" t="s">
-        <v>6601</v>
+        <v>6600</v>
       </c>
       <c r="F722" t="s">
         <v>2300</v>
       </c>
       <c r="G722" t="s">
-        <v>6602</v>
+        <v>6601</v>
       </c>
       <c r="H722" t="s">
         <v>11</v>
@@ -41919,10 +41949,10 @@
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A723" t="s">
-        <v>6643</v>
+        <v>6642</v>
       </c>
       <c r="B723" t="s">
-        <v>6629</v>
+        <v>6628</v>
       </c>
       <c r="C723" t="s">
         <v>279</v>
@@ -41937,7 +41967,7 @@
         <v>2300</v>
       </c>
       <c r="G723" t="s">
-        <v>6630</v>
+        <v>6629</v>
       </c>
       <c r="H723" t="s">
         <v>35</v>
@@ -41951,10 +41981,10 @@
     </row>
     <row r="724" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A724" t="s">
-        <v>6655</v>
+        <v>6654</v>
       </c>
       <c r="B724" t="s">
-        <v>6644</v>
+        <v>6643</v>
       </c>
       <c r="C724">
         <v>100</v>
@@ -41969,7 +41999,7 @@
         <v>2367</v>
       </c>
       <c r="G724" t="s">
-        <v>6645</v>
+        <v>6644</v>
       </c>
       <c r="H724" t="s">
         <v>5524</v>
@@ -41983,10 +42013,10 @@
     </row>
     <row r="725" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A725" t="s">
-        <v>6714</v>
+        <v>6713</v>
       </c>
       <c r="B725" t="s">
-        <v>6656</v>
+        <v>6655</v>
       </c>
       <c r="C725">
         <v>100</v>
@@ -42001,7 +42031,7 @@
         <v>2367</v>
       </c>
       <c r="G725" t="s">
-        <v>6657</v>
+        <v>6656</v>
       </c>
       <c r="H725" t="s">
         <v>5607</v>
@@ -42015,10 +42045,10 @@
     </row>
     <row r="726" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A726" t="s">
+        <v>6714</v>
+      </c>
+      <c r="B726" t="s">
         <v>6715</v>
-      </c>
-      <c r="B726" t="s">
-        <v>6716</v>
       </c>
       <c r="C726" t="s">
         <v>200</v>
@@ -42027,13 +42057,13 @@
         <v>0.01</v>
       </c>
       <c r="E726" s="12" t="s">
-        <v>6601</v>
+        <v>6600</v>
       </c>
       <c r="F726" t="s">
         <v>2611</v>
       </c>
       <c r="G726" t="s">
-        <v>6717</v>
+        <v>6716</v>
       </c>
       <c r="H726" t="s">
         <v>11</v>
@@ -42047,10 +42077,10 @@
     </row>
     <row r="727" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A727" t="s">
-        <v>6760</v>
+        <v>6759</v>
       </c>
       <c r="B727" t="s">
-        <v>6764</v>
+        <v>6763</v>
       </c>
       <c r="C727" t="s">
         <v>900</v>
@@ -42059,16 +42089,16 @@
         <v>0.1</v>
       </c>
       <c r="E727" s="12" t="s">
-        <v>6761</v>
+        <v>6760</v>
       </c>
       <c r="F727" t="s">
         <v>4889</v>
       </c>
       <c r="G727" t="s">
-        <v>6763</v>
+        <v>6762</v>
       </c>
       <c r="H727" t="s">
-        <v>6762</v>
+        <v>6761</v>
       </c>
       <c r="I727" t="s">
         <v>2343</v>
@@ -42079,10 +42109,10 @@
     </row>
     <row r="728" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A728" t="s">
+        <v>6805</v>
+      </c>
+      <c r="B728" t="s">
         <v>6806</v>
-      </c>
-      <c r="B728" t="s">
-        <v>6807</v>
       </c>
       <c r="C728">
         <v>0.5</v>
@@ -42097,10 +42127,10 @@
         <v>2611</v>
       </c>
       <c r="G728" t="s">
+        <v>6807</v>
+      </c>
+      <c r="H728" t="s">
         <v>6808</v>
-      </c>
-      <c r="H728" t="s">
-        <v>6809</v>
       </c>
       <c r="I728" t="s">
         <v>12</v>
@@ -42111,10 +42141,10 @@
     </row>
     <row r="729" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A729" t="s">
+        <v>6809</v>
+      </c>
+      <c r="B729" t="s">
         <v>6810</v>
-      </c>
-      <c r="B729" t="s">
-        <v>6811</v>
       </c>
       <c r="C729">
         <v>10</v>
@@ -42126,7 +42156,7 @@
         <v>5250</v>
       </c>
       <c r="H729" t="s">
-        <v>6812</v>
+        <v>6811</v>
       </c>
       <c r="I729" t="s">
         <v>12</v>
@@ -42580,10 +42610,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42828,7 +42858,7 @@
         <v>4477</v>
       </c>
       <c r="E11" t="s">
-        <v>6914</v>
+        <v>6913</v>
       </c>
       <c r="F11" t="s">
         <v>4478</v>
@@ -43769,7 +43799,7 @@
         <v>5947</v>
       </c>
       <c r="D54" t="s">
-        <v>6342</v>
+        <v>6972</v>
       </c>
       <c r="E54" t="s">
         <v>1471</v>
@@ -43783,22 +43813,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>6378</v>
+      </c>
+      <c r="B55" t="s">
         <v>6379</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>6380</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>6381</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
+        <v>6381</v>
+      </c>
+      <c r="F55" t="s">
         <v>6382</v>
-      </c>
-      <c r="E55" t="s">
-        <v>6382</v>
-      </c>
-      <c r="F55" t="s">
-        <v>6383</v>
       </c>
       <c r="G55" s="8">
         <v>13.68</v>
@@ -43806,22 +43836,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>6492</v>
+      </c>
+      <c r="B56" t="s">
         <v>6493</v>
-      </c>
-      <c r="B56" t="s">
-        <v>6494</v>
       </c>
       <c r="C56" t="s">
         <v>2287</v>
       </c>
       <c r="D56" t="s">
-        <v>6495</v>
+        <v>6494</v>
       </c>
       <c r="E56" t="s">
         <v>2558</v>
       </c>
       <c r="F56" t="s">
-        <v>6496</v>
+        <v>6495</v>
       </c>
       <c r="G56" s="8">
         <v>0.61</v>
@@ -43829,22 +43859,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>6585</v>
+      </c>
+      <c r="B57" t="s">
         <v>6586</v>
-      </c>
-      <c r="B57" t="s">
-        <v>6587</v>
       </c>
       <c r="C57" t="s">
         <v>2465</v>
       </c>
       <c r="D57" t="s">
+        <v>6587</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6589</v>
+      </c>
+      <c r="F57" t="s">
         <v>6588</v>
-      </c>
-      <c r="E57" t="s">
-        <v>6590</v>
-      </c>
-      <c r="F57" t="s">
-        <v>6589</v>
       </c>
       <c r="G57" s="8">
         <v>0.81</v>
@@ -43852,16 +43882,16 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>6621</v>
+      </c>
+      <c r="B58" t="s">
         <v>6622</v>
-      </c>
-      <c r="B58" t="s">
-        <v>6623</v>
       </c>
       <c r="C58" t="s">
         <v>4552</v>
       </c>
       <c r="D58" t="s">
-        <v>6624</v>
+        <v>6623</v>
       </c>
       <c r="E58" t="s">
         <v>4325</v>
@@ -43875,16 +43905,16 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>6703</v>
+        <v>6702</v>
       </c>
       <c r="B59" t="s">
-        <v>6705</v>
+        <v>6704</v>
       </c>
       <c r="C59" t="s">
         <v>1381</v>
       </c>
       <c r="D59" t="s">
-        <v>6704</v>
+        <v>6703</v>
       </c>
       <c r="E59" t="s">
         <v>4325</v>
@@ -43898,22 +43928,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>6782</v>
+      </c>
+      <c r="B60" t="s">
         <v>6783</v>
-      </c>
-      <c r="B60" t="s">
-        <v>6784</v>
       </c>
       <c r="C60" t="s">
         <v>4263</v>
       </c>
       <c r="D60" t="s">
-        <v>6785</v>
+        <v>6784</v>
       </c>
       <c r="E60" t="s">
-        <v>6785</v>
+        <v>6784</v>
       </c>
       <c r="F60" t="s">
-        <v>6785</v>
+        <v>6784</v>
       </c>
       <c r="G60" s="8">
         <v>6.32</v>
@@ -43921,19 +43951,19 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>6856</v>
+        <v>6855</v>
       </c>
       <c r="B61" t="s">
-        <v>6859</v>
+        <v>6858</v>
       </c>
       <c r="C61" t="s">
         <v>2978</v>
       </c>
       <c r="D61" t="s">
-        <v>6858</v>
+        <v>6857</v>
       </c>
       <c r="E61" t="s">
-        <v>6857</v>
+        <v>6856</v>
       </c>
       <c r="F61" t="s">
         <v>6010</v>
@@ -43944,25 +43974,48 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>6907</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6912</v>
+      </c>
+      <c r="C62" t="s">
         <v>6908</v>
       </c>
-      <c r="B62" t="s">
-        <v>6913</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
+        <v>6911</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6910</v>
+      </c>
+      <c r="F62" t="s">
         <v>6909</v>
-      </c>
-      <c r="D62" t="s">
-        <v>6912</v>
-      </c>
-      <c r="E62" t="s">
-        <v>6911</v>
-      </c>
-      <c r="F62" t="s">
-        <v>6910</v>
       </c>
       <c r="G62" s="8">
         <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>6977</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6982</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6981</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6978</v>
+      </c>
+      <c r="E63" t="s">
+        <v>6979</v>
+      </c>
+      <c r="F63" t="s">
+        <v>6980</v>
+      </c>
+      <c r="G63" s="8">
+        <v>0.10489999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -43975,7 +44028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -45538,10 +45591,10 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>6352</v>
+        <v>6351</v>
       </c>
       <c r="B43" t="s">
-        <v>6358</v>
+        <v>6357</v>
       </c>
       <c r="C43" t="s">
         <v>946</v>
@@ -45550,10 +45603,10 @@
         <v>5481</v>
       </c>
       <c r="E43" t="s">
+        <v>6352</v>
+      </c>
+      <c r="F43" t="s">
         <v>6353</v>
-      </c>
-      <c r="F43" t="s">
-        <v>6354</v>
       </c>
       <c r="G43" t="s">
         <v>2093</v>
@@ -45562,13 +45615,13 @@
         <v>2091</v>
       </c>
       <c r="I43" t="s">
-        <v>6355</v>
+        <v>6354</v>
       </c>
       <c r="J43" t="s">
         <v>2413</v>
       </c>
       <c r="K43" t="s">
-        <v>6356</v>
+        <v>6355</v>
       </c>
       <c r="L43" s="8">
         <v>0.87</v>
@@ -45576,13 +45629,13 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>6357</v>
+        <v>6356</v>
       </c>
       <c r="B44" t="s">
+        <v>6358</v>
+      </c>
+      <c r="C44" t="s">
         <v>6359</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6360</v>
       </c>
       <c r="D44" t="s">
         <v>1225</v>
@@ -45597,10 +45650,10 @@
         <v>6122</v>
       </c>
       <c r="H44" t="s">
-        <v>6362</v>
+        <v>6361</v>
       </c>
       <c r="I44" t="s">
-        <v>6361</v>
+        <v>6360</v>
       </c>
       <c r="J44" t="s">
         <v>6124</v>
@@ -45614,16 +45667,16 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>6362</v>
+      </c>
+      <c r="B45" t="s">
         <v>6363</v>
-      </c>
-      <c r="B45" t="s">
-        <v>6364</v>
       </c>
       <c r="C45" t="s">
         <v>5716</v>
       </c>
       <c r="D45" t="s">
-        <v>6365</v>
+        <v>6364</v>
       </c>
       <c r="E45" t="s">
         <v>2948</v>
@@ -45638,7 +45691,7 @@
         <v>5580</v>
       </c>
       <c r="I45" t="s">
-        <v>6366</v>
+        <v>6365</v>
       </c>
       <c r="J45" t="s">
         <v>4800</v>
@@ -45652,10 +45705,10 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>6692</v>
+      </c>
+      <c r="B46" t="s">
         <v>6693</v>
-      </c>
-      <c r="B46" t="s">
-        <v>6694</v>
       </c>
       <c r="C46" t="s">
         <v>2120</v>
@@ -45664,7 +45717,7 @@
         <v>2106</v>
       </c>
       <c r="E46" t="s">
-        <v>6695</v>
+        <v>6694</v>
       </c>
       <c r="F46" t="s">
         <v>4649</v>
@@ -45673,10 +45726,10 @@
         <v>4978</v>
       </c>
       <c r="H46" t="s">
-        <v>6362</v>
+        <v>6361</v>
       </c>
       <c r="I46" t="s">
-        <v>6696</v>
+        <v>6695</v>
       </c>
       <c r="J46" t="s">
         <v>6124</v>
@@ -45690,19 +45743,19 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>6697</v>
+        <v>6696</v>
       </c>
       <c r="B47" t="s">
-        <v>6702</v>
+        <v>6701</v>
       </c>
       <c r="C47" t="s">
         <v>2120</v>
       </c>
       <c r="D47" t="s">
-        <v>6701</v>
+        <v>6700</v>
       </c>
       <c r="E47" t="s">
-        <v>6700</v>
+        <v>6699</v>
       </c>
       <c r="F47" t="s">
         <v>4649</v>
@@ -45711,16 +45764,16 @@
         <v>2251</v>
       </c>
       <c r="H47" t="s">
-        <v>6362</v>
+        <v>6361</v>
       </c>
       <c r="I47" t="s">
-        <v>6699</v>
+        <v>6698</v>
       </c>
       <c r="J47" t="s">
         <v>6124</v>
       </c>
       <c r="K47" t="s">
-        <v>6698</v>
+        <v>6697</v>
       </c>
       <c r="L47" s="8">
         <v>0.32</v>
@@ -45728,22 +45781,22 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>6709</v>
+        <v>6708</v>
       </c>
       <c r="B48" t="s">
-        <v>6708</v>
+        <v>6707</v>
       </c>
       <c r="C48" t="s">
         <v>2100</v>
       </c>
       <c r="D48" t="s">
-        <v>6707</v>
+        <v>6706</v>
       </c>
       <c r="E48" t="s">
         <v>2296</v>
       </c>
       <c r="F48" t="s">
-        <v>6354</v>
+        <v>6353</v>
       </c>
       <c r="G48" t="s">
         <v>2255</v>
@@ -45752,13 +45805,13 @@
         <v>5580</v>
       </c>
       <c r="I48" t="s">
-        <v>6706</v>
+        <v>6705</v>
       </c>
       <c r="J48" t="s">
         <v>5380</v>
       </c>
       <c r="K48" t="s">
-        <v>6356</v>
+        <v>6355</v>
       </c>
       <c r="L48" s="8">
         <v>2.81</v>
@@ -45766,10 +45819,10 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>6828</v>
+      </c>
+      <c r="B49" t="s">
         <v>6829</v>
-      </c>
-      <c r="B49" t="s">
-        <v>6830</v>
       </c>
       <c r="C49" t="s">
         <v>1836</v>
@@ -45784,13 +45837,13 @@
         <v>2236</v>
       </c>
       <c r="G49" t="s">
-        <v>6831</v>
+        <v>6830</v>
       </c>
       <c r="H49" t="s">
         <v>2091</v>
       </c>
       <c r="I49" t="s">
-        <v>6832</v>
+        <v>6831</v>
       </c>
       <c r="J49" t="s">
         <v>5246</v>
@@ -45804,31 +45857,31 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>6872</v>
+      </c>
+      <c r="B50" t="s">
         <v>6873</v>
-      </c>
-      <c r="B50" t="s">
-        <v>6874</v>
       </c>
       <c r="C50" t="s">
         <v>944</v>
       </c>
       <c r="D50" t="s">
+        <v>6874</v>
+      </c>
+      <c r="E50" t="s">
         <v>6875</v>
-      </c>
-      <c r="E50" t="s">
-        <v>6876</v>
       </c>
       <c r="F50" t="s">
         <v>4649</v>
       </c>
       <c r="G50" t="s">
-        <v>6877</v>
+        <v>6876</v>
       </c>
       <c r="H50" t="s">
         <v>2298</v>
       </c>
       <c r="I50" t="s">
-        <v>6878</v>
+        <v>6877</v>
       </c>
       <c r="J50" t="s">
         <v>4542</v>
@@ -45842,10 +45895,10 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>6878</v>
+      </c>
+      <c r="B51" t="s">
         <v>6879</v>
-      </c>
-      <c r="B51" t="s">
-        <v>6880</v>
       </c>
       <c r="C51" t="s">
         <v>2100</v>
@@ -45854,7 +45907,7 @@
         <v>4646</v>
       </c>
       <c r="E51" t="s">
-        <v>6881</v>
+        <v>6880</v>
       </c>
       <c r="F51" t="s">
         <v>4649</v>
@@ -45866,13 +45919,13 @@
         <v>2298</v>
       </c>
       <c r="I51" t="s">
+        <v>6881</v>
+      </c>
+      <c r="J51" t="s">
         <v>6882</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>6883</v>
-      </c>
-      <c r="K51" t="s">
-        <v>6884</v>
       </c>
       <c r="L51" s="8">
         <v>1.19</v>
@@ -45880,22 +45933,22 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>6932</v>
+      </c>
+      <c r="B52" t="s">
         <v>6933</v>
-      </c>
-      <c r="B52" t="s">
-        <v>6934</v>
       </c>
       <c r="C52" t="s">
         <v>4645</v>
       </c>
       <c r="D52" t="s">
-        <v>6935</v>
+        <v>6934</v>
       </c>
       <c r="E52" t="s">
         <v>2296</v>
       </c>
       <c r="F52" t="s">
-        <v>6354</v>
+        <v>6353</v>
       </c>
       <c r="G52" t="s">
         <v>4978</v>
@@ -45904,13 +45957,13 @@
         <v>5580</v>
       </c>
       <c r="I52" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="J52" t="s">
         <v>5380</v>
       </c>
       <c r="K52" t="s">
-        <v>6356</v>
+        <v>6355</v>
       </c>
       <c r="L52" s="8">
         <v>4.43</v>
@@ -47406,7 +47459,7 @@
         <v>4499</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>6484</v>
+        <v>6483</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>2501</v>
@@ -47730,7 +47783,7 @@
         <v>5159</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>6484</v>
+        <v>6483</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>2501</v>
@@ -47768,7 +47821,7 @@
         <v>5164</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>6484</v>
+        <v>6483</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>2501</v>
@@ -48336,19 +48389,19 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
+        <v>6366</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>6367</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>6368</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>6369</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>6370</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>6371</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>2130</v>
@@ -48357,7 +48410,7 @@
         <v>5149</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>6372</v>
+        <v>6371</v>
       </c>
       <c r="K69" s="2" t="s">
         <v>2104</v>
@@ -48371,13 +48424,13 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
+        <v>6413</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>6474</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>6414</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>6475</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>6415</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>2106</v>
@@ -48389,13 +48442,13 @@
         <v>2287</v>
       </c>
       <c r="J70" s="2" t="s">
+        <v>6415</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>6417</v>
+      </c>
+      <c r="L70" s="2" t="s">
         <v>6416</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>6418</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>6417</v>
       </c>
       <c r="M70" s="8">
         <v>0.56000000000000005</v>
@@ -48403,16 +48456,16 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>6429</v>
+        <v>6428</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>6433</v>
+        <v>6432</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>4544</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>6430</v>
+        <v>6429</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>2111</v>
@@ -48424,13 +48477,13 @@
         <v>50</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>6431</v>
+        <v>6430</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>2558</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>6432</v>
+        <v>6431</v>
       </c>
       <c r="M71" s="8">
         <v>0.73</v>
@@ -48438,10 +48491,10 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>6476</v>
+        <v>6475</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>6479</v>
+        <v>6478</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>4827</v>
@@ -48450,7 +48503,7 @@
         <v>4765</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>6370</v>
+        <v>6369</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>2133</v>
@@ -48462,13 +48515,13 @@
         <v>5149</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>6478</v>
+        <v>6477</v>
       </c>
       <c r="K72" s="2" t="s">
         <v>2181</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>6477</v>
+        <v>6476</v>
       </c>
       <c r="M72" s="8">
         <v>0.16</v>
@@ -48476,13 +48529,13 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
+        <v>6508</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>6509</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>6510</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>6511</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>944</v>
@@ -48497,7 +48550,7 @@
         <v>2091</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>6512</v>
+        <v>6511</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>2104</v>
@@ -48511,10 +48564,10 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
+        <v>6556</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>6557</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>6558</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>4827</v>
@@ -48538,7 +48591,7 @@
         <v>2091</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>6559</v>
+        <v>6558</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>2104</v>
@@ -48552,13 +48605,13 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
+        <v>6603</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>6604</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>6605</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>6606</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>944</v>
@@ -48573,7 +48626,7 @@
         <v>2091</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>6607</v>
+        <v>6606</v>
       </c>
       <c r="K75" s="2" t="s">
         <v>5586</v>
@@ -48587,13 +48640,13 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
+        <v>6607</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>6608</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>6609</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>6610</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>2120</v>
@@ -48608,7 +48661,7 @@
         <v>2430</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>6611</v>
+        <v>6610</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>5586</v>
@@ -48622,13 +48675,13 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
+        <v>6709</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>6710</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>6711</v>
-      </c>
       <c r="D77" s="2" t="s">
-        <v>6430</v>
+        <v>6429</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>70</v>
@@ -48640,13 +48693,13 @@
         <v>5149</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>6712</v>
+        <v>6711</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>6124</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>6713</v>
+        <v>6712</v>
       </c>
       <c r="M77" s="8">
         <v>0.35</v>
@@ -48654,34 +48707,34 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>6736</v>
+        <v>6735</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>6743</v>
+        <v>6742</v>
       </c>
       <c r="C78" s="2" t="s">
+        <v>6740</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>6741</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>6742</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>4660</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>6740</v>
+        <v>6739</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>6739</v>
+        <v>6738</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>6738</v>
+        <v>6737</v>
       </c>
       <c r="K78" t="s">
-        <v>6744</v>
+        <v>6743</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>6737</v>
+        <v>6736</v>
       </c>
       <c r="M78" s="8">
         <v>3.68</v>
@@ -48689,13 +48742,13 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>6805</v>
+        <v>6804</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>6804</v>
+        <v>6803</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>6803</v>
+        <v>6802</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>944</v>
@@ -48710,10 +48763,10 @@
         <v>5149</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>6802</v>
+        <v>6801</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>6865</v>
+        <v>6864</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>2097</v>
@@ -48724,10 +48777,10 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
+        <v>6823</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>6824</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>6825</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>2172</v>
@@ -48736,7 +48789,7 @@
         <v>2130</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>6864</v>
+        <v>6863</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>2129</v>
@@ -48744,10 +48797,10 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
+        <v>6825</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>6826</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>6827</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>5457</v>
@@ -48765,10 +48818,10 @@
         <v>2091</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>6828</v>
+        <v>6827</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>6863</v>
+        <v>6862</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>2097</v>
@@ -48779,16 +48832,16 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
+        <v>6868</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>6869</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>6870</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>2506</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>6871</v>
+        <v>6870</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>2507</v>
@@ -48797,7 +48850,7 @@
         <v>2496</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>6872</v>
+        <v>6871</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>2501</v>
@@ -48808,13 +48861,13 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
+        <v>6930</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>6931</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>6932</v>
-      </c>
       <c r="C83" s="2" t="s">
-        <v>6930</v>
+        <v>6929</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>944</v>
@@ -48829,13 +48882,13 @@
         <v>2430</v>
       </c>
       <c r="J83" s="2" t="s">
+        <v>6926</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>6928</v>
+      </c>
+      <c r="L83" s="2" t="s">
         <v>6927</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>6929</v>
-      </c>
-      <c r="L83" s="2" t="s">
-        <v>6928</v>
       </c>
       <c r="M83" s="8">
         <v>1.37</v>
@@ -48843,10 +48896,10 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
+        <v>6937</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>6938</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>6939</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>4544</v>
@@ -48870,7 +48923,7 @@
         <v>4825</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>6937</v>
+        <v>6936</v>
       </c>
       <c r="K84" s="2" t="s">
         <v>2183</v>
@@ -48884,10 +48937,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
+        <v>6952</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>6953</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>6954</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>5157</v>
@@ -48896,10 +48949,10 @@
         <v>2944</v>
       </c>
       <c r="F85" s="2" t="s">
+        <v>6954</v>
+      </c>
+      <c r="G85" s="2" t="s">
         <v>6955</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>6956</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>2496</v>
@@ -48908,10 +48961,10 @@
         <v>4631</v>
       </c>
       <c r="J85" s="2" t="s">
+        <v>6956</v>
+      </c>
+      <c r="K85" s="2" t="s">
         <v>6957</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>6958</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>2501</v>
@@ -48922,10 +48975,10 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>6969</v>
+        <v>6968</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>6968</v>
+        <v>6967</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>6079</v>
@@ -48943,7 +48996,7 @@
         <v>4500</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>6967</v>
+        <v>6966</v>
       </c>
       <c r="K86" s="2" t="s">
         <v>2098</v>
@@ -48964,10 +49017,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
     <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I106" sqref="I106"/>
+      <selection activeCell="I107" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51589,10 +51642,10 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>6438</v>
+        <v>6437</v>
       </c>
       <c r="B83" t="s">
-        <v>6437</v>
+        <v>6436</v>
       </c>
       <c r="C83" t="s">
         <v>5800</v>
@@ -51610,13 +51663,13 @@
         <v>2907</v>
       </c>
       <c r="H83" t="s">
+        <v>6433</v>
+      </c>
+      <c r="I83" t="s">
         <v>6434</v>
       </c>
-      <c r="I83" t="s">
+      <c r="J83" t="s">
         <v>6435</v>
-      </c>
-      <c r="J83" t="s">
-        <v>6436</v>
       </c>
       <c r="K83" s="8">
         <v>2.15</v>
@@ -51624,10 +51677,10 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>6446</v>
+      </c>
+      <c r="B84" t="s">
         <v>6447</v>
-      </c>
-      <c r="B84" t="s">
-        <v>6448</v>
       </c>
       <c r="C84" t="s">
         <v>5800</v>
@@ -51639,16 +51692,16 @@
         <v>1</v>
       </c>
       <c r="G84" t="s">
+        <v>6448</v>
+      </c>
+      <c r="H84" t="s">
         <v>6449</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
+        <v>6449</v>
+      </c>
+      <c r="J84" t="s">
         <v>6450</v>
-      </c>
-      <c r="I84" t="s">
-        <v>6450</v>
-      </c>
-      <c r="J84" t="s">
-        <v>6451</v>
       </c>
       <c r="K84" s="8">
         <v>10.26</v>
@@ -51656,19 +51709,19 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>6488</v>
+        <v>6487</v>
       </c>
       <c r="B85" t="s">
+        <v>6484</v>
+      </c>
+      <c r="G85" t="s">
         <v>6485</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>6486</v>
       </c>
-      <c r="H85" t="s">
-        <v>6487</v>
-      </c>
       <c r="I85" t="s">
-        <v>6487</v>
+        <v>6486</v>
       </c>
       <c r="J85" t="s">
         <v>6307</v>
@@ -51679,10 +51732,10 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>6534</v>
+        <v>6533</v>
       </c>
       <c r="B86" t="s">
-        <v>6538</v>
+        <v>6537</v>
       </c>
       <c r="C86" t="s">
         <v>6315</v>
@@ -51700,13 +51753,13 @@
         <v>2978</v>
       </c>
       <c r="H86" t="s">
+        <v>6534</v>
+      </c>
+      <c r="I86" t="s">
         <v>6535</v>
       </c>
-      <c r="I86" t="s">
+      <c r="J86" t="s">
         <v>6536</v>
-      </c>
-      <c r="J86" t="s">
-        <v>6537</v>
       </c>
       <c r="K86" s="8">
         <v>7.49</v>
@@ -51714,10 +51767,10 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>6538</v>
+      </c>
+      <c r="B87" t="s">
         <v>6539</v>
-      </c>
-      <c r="B87" t="s">
-        <v>6540</v>
       </c>
       <c r="C87" t="s">
         <v>5478</v>
@@ -51735,13 +51788,13 @@
         <v>2978</v>
       </c>
       <c r="H87" t="s">
+        <v>6540</v>
+      </c>
+      <c r="I87" t="s">
         <v>6541</v>
       </c>
-      <c r="I87" t="s">
-        <v>6542</v>
-      </c>
       <c r="J87" t="s">
-        <v>6537</v>
+        <v>6536</v>
       </c>
       <c r="K87" s="8">
         <v>5.17</v>
@@ -51749,10 +51802,10 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>6581</v>
+      </c>
+      <c r="B88" t="s">
         <v>6582</v>
-      </c>
-      <c r="B88" t="s">
-        <v>6583</v>
       </c>
       <c r="C88" t="s">
         <v>5800</v>
@@ -51761,10 +51814,10 @@
         <v>2978</v>
       </c>
       <c r="H88" t="s">
+        <v>6583</v>
+      </c>
+      <c r="I88" t="s">
         <v>6584</v>
-      </c>
-      <c r="I88" t="s">
-        <v>6585</v>
       </c>
       <c r="J88" t="s">
         <v>4740</v>
@@ -51775,10 +51828,10 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
+        <v>6613</v>
+      </c>
+      <c r="B89" t="s">
         <v>6614</v>
-      </c>
-      <c r="B89" t="s">
-        <v>6615</v>
       </c>
       <c r="C89" t="s">
         <v>2396</v>
@@ -51793,10 +51846,10 @@
         <v>2388</v>
       </c>
       <c r="H89" s="11" t="s">
-        <v>6613</v>
+        <v>6612</v>
       </c>
       <c r="I89" t="s">
-        <v>6612</v>
+        <v>6611</v>
       </c>
       <c r="J89" t="s">
         <v>2956</v>
@@ -51807,10 +51860,10 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>6616</v>
+        <v>6615</v>
       </c>
       <c r="B90" t="s">
-        <v>6620</v>
+        <v>6619</v>
       </c>
       <c r="C90" t="s">
         <v>5511</v>
@@ -51819,13 +51872,13 @@
         <v>2978</v>
       </c>
       <c r="H90" t="s">
-        <v>6619</v>
+        <v>6618</v>
       </c>
       <c r="I90" t="s">
-        <v>6618</v>
+        <v>6617</v>
       </c>
       <c r="J90" t="s">
-        <v>6617</v>
+        <v>6616</v>
       </c>
       <c r="K90" s="8">
         <v>1.33</v>
@@ -51833,10 +51886,10 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>6645</v>
+      </c>
+      <c r="B91" t="s">
         <v>6646</v>
-      </c>
-      <c r="B91" t="s">
-        <v>6647</v>
       </c>
       <c r="C91" t="s">
         <v>2396</v>
@@ -51848,16 +51901,16 @@
         <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>6648</v>
+        <v>6647</v>
       </c>
       <c r="G91" t="s">
         <v>2978</v>
       </c>
       <c r="H91" t="s">
+        <v>6648</v>
+      </c>
+      <c r="I91" t="s">
         <v>6649</v>
-      </c>
-      <c r="I91" t="s">
-        <v>6650</v>
       </c>
       <c r="J91" t="s">
         <v>2446</v>
@@ -51868,10 +51921,10 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>6654</v>
+        <v>6653</v>
       </c>
       <c r="B92" t="s">
-        <v>6653</v>
+        <v>6652</v>
       </c>
       <c r="C92" t="s">
         <v>5478</v>
@@ -51883,16 +51936,16 @@
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>6648</v>
+        <v>6647</v>
       </c>
       <c r="G92" t="s">
         <v>2978</v>
       </c>
       <c r="H92" t="s">
-        <v>6652</v>
+        <v>6651</v>
       </c>
       <c r="I92" t="s">
-        <v>6651</v>
+        <v>6650</v>
       </c>
       <c r="J92" t="s">
         <v>2446</v>
@@ -51903,10 +51956,10 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>6672</v>
+        <v>6671</v>
       </c>
       <c r="B93" t="s">
-        <v>6676</v>
+        <v>6675</v>
       </c>
       <c r="C93" t="s">
         <v>5511</v>
@@ -51921,13 +51974,13 @@
         <v>2388</v>
       </c>
       <c r="H93" s="11" t="s">
-        <v>6675</v>
+        <v>6674</v>
       </c>
       <c r="I93" t="s">
-        <v>6674</v>
+        <v>6673</v>
       </c>
       <c r="J93" t="s">
-        <v>6673</v>
+        <v>6672</v>
       </c>
       <c r="K93" s="8">
         <v>2.02</v>
@@ -51935,13 +51988,13 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>6676</v>
+      </c>
+      <c r="B94" t="s">
         <v>6677</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>6678</v>
-      </c>
-      <c r="C94" t="s">
-        <v>6679</v>
       </c>
       <c r="D94">
         <v>35</v>
@@ -51950,19 +52003,19 @@
         <v>1</v>
       </c>
       <c r="F94" t="s">
-        <v>6680</v>
+        <v>6679</v>
       </c>
       <c r="G94" t="s">
         <v>2978</v>
       </c>
       <c r="H94" t="s">
+        <v>6680</v>
+      </c>
+      <c r="I94" t="s">
         <v>6681</v>
       </c>
-      <c r="I94" t="s">
+      <c r="J94" t="s">
         <v>6682</v>
-      </c>
-      <c r="J94" t="s">
-        <v>6683</v>
       </c>
       <c r="K94" s="8">
         <v>11.45</v>
@@ -51970,10 +52023,10 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>6688</v>
+        <v>6687</v>
       </c>
       <c r="B95" t="s">
-        <v>6684</v>
+        <v>6683</v>
       </c>
       <c r="C95" t="s">
         <v>2396</v>
@@ -51985,19 +52038,19 @@
         <v>1</v>
       </c>
       <c r="F95" t="s">
-        <v>6680</v>
+        <v>6679</v>
       </c>
       <c r="G95" t="s">
         <v>2978</v>
       </c>
       <c r="H95" t="s">
+        <v>6684</v>
+      </c>
+      <c r="I95" t="s">
         <v>6685</v>
       </c>
-      <c r="I95" t="s">
+      <c r="J95" t="s">
         <v>6686</v>
-      </c>
-      <c r="J95" t="s">
-        <v>6687</v>
       </c>
       <c r="K95" s="8">
         <v>11.68</v>
@@ -52005,10 +52058,10 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>6717</v>
+      </c>
+      <c r="B96" t="s">
         <v>6718</v>
-      </c>
-      <c r="B96" t="s">
-        <v>6719</v>
       </c>
       <c r="C96" t="s">
         <v>2382</v>
@@ -52026,10 +52079,10 @@
         <v>2978</v>
       </c>
       <c r="H96" t="s">
+        <v>6719</v>
+      </c>
+      <c r="I96" t="s">
         <v>6720</v>
-      </c>
-      <c r="I96" t="s">
-        <v>6721</v>
       </c>
       <c r="J96" t="s">
         <v>2383</v>
@@ -52040,10 +52093,10 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>6725</v>
+        <v>6724</v>
       </c>
       <c r="B97" t="s">
-        <v>6722</v>
+        <v>6721</v>
       </c>
       <c r="C97" t="s">
         <v>2382</v>
@@ -52061,10 +52114,10 @@
         <v>2978</v>
       </c>
       <c r="H97" t="s">
+        <v>6722</v>
+      </c>
+      <c r="I97" t="s">
         <v>6723</v>
-      </c>
-      <c r="I97" t="s">
-        <v>6724</v>
       </c>
       <c r="J97" t="s">
         <v>2956</v>
@@ -52075,10 +52128,10 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
+        <v>6725</v>
+      </c>
+      <c r="B98" t="s">
         <v>6726</v>
-      </c>
-      <c r="B98" t="s">
-        <v>6727</v>
       </c>
       <c r="C98" t="s">
         <v>2382</v>
@@ -52090,16 +52143,16 @@
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>6728</v>
+        <v>6727</v>
       </c>
       <c r="G98" t="s">
         <v>2380</v>
       </c>
       <c r="H98" s="11" t="s">
+        <v>6728</v>
+      </c>
+      <c r="I98" t="s">
         <v>6729</v>
-      </c>
-      <c r="I98" t="s">
-        <v>6730</v>
       </c>
       <c r="J98" t="s">
         <v>2956</v>
@@ -52110,10 +52163,10 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
+        <v>6744</v>
+      </c>
+      <c r="B99" t="s">
         <v>6745</v>
-      </c>
-      <c r="B99" t="s">
-        <v>6746</v>
       </c>
       <c r="C99" t="s">
         <v>2382</v>
@@ -52134,7 +52187,7 @@
         <v>1991105</v>
       </c>
       <c r="I99" t="s">
-        <v>6747</v>
+        <v>6746</v>
       </c>
       <c r="J99" t="s">
         <v>2383</v>
@@ -52145,13 +52198,13 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>6773</v>
+        <v>6772</v>
       </c>
       <c r="B100" t="s">
-        <v>6772</v>
+        <v>6771</v>
       </c>
       <c r="C100" t="s">
-        <v>6679</v>
+        <v>6678</v>
       </c>
       <c r="D100">
         <v>3</v>
@@ -52166,10 +52219,10 @@
         <v>2978</v>
       </c>
       <c r="H100" t="s">
-        <v>6771</v>
+        <v>6770</v>
       </c>
       <c r="I100" t="s">
-        <v>6770</v>
+        <v>6769</v>
       </c>
       <c r="J100" t="s">
         <v>2383</v>
@@ -52180,10 +52233,10 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>6860</v>
+        <v>6859</v>
       </c>
       <c r="B101" t="s">
-        <v>6862</v>
+        <v>6861</v>
       </c>
       <c r="C101" t="s">
         <v>6217</v>
@@ -52201,7 +52254,7 @@
         <v>6218</v>
       </c>
       <c r="H101" t="s">
-        <v>6861</v>
+        <v>6860</v>
       </c>
       <c r="I101" t="s">
         <v>6220</v>
@@ -52215,10 +52268,10 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>6884</v>
+      </c>
+      <c r="B102" t="s">
         <v>6885</v>
-      </c>
-      <c r="B102" t="s">
-        <v>6886</v>
       </c>
       <c r="C102" t="s">
         <v>2382</v>
@@ -52230,16 +52283,16 @@
         <v>1</v>
       </c>
       <c r="F102" t="s">
-        <v>6680</v>
+        <v>6679</v>
       </c>
       <c r="G102" t="s">
         <v>2978</v>
       </c>
       <c r="H102" t="s">
-        <v>6888</v>
+        <v>6887</v>
       </c>
       <c r="I102" t="s">
-        <v>6887</v>
+        <v>6886</v>
       </c>
       <c r="J102" t="s">
         <v>2956</v>
@@ -52250,10 +52303,10 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>6893</v>
+      </c>
+      <c r="B103" t="s">
         <v>6894</v>
-      </c>
-      <c r="B103" t="s">
-        <v>6895</v>
       </c>
       <c r="C103" t="s">
         <v>2396</v>
@@ -52268,13 +52321,13 @@
         <v>4737</v>
       </c>
       <c r="H103" t="s">
+        <v>6896</v>
+      </c>
+      <c r="I103" t="s">
         <v>6897</v>
       </c>
-      <c r="I103" t="s">
-        <v>6898</v>
-      </c>
       <c r="J103" t="s">
-        <v>6896</v>
+        <v>6895</v>
       </c>
       <c r="K103" s="8">
         <v>1.66</v>
@@ -52282,10 +52335,10 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>6914</v>
+      </c>
+      <c r="B104" t="s">
         <v>6915</v>
-      </c>
-      <c r="B104" t="s">
-        <v>6916</v>
       </c>
       <c r="C104" t="s">
         <v>2382</v>
@@ -52297,7 +52350,7 @@
         <v>1</v>
       </c>
       <c r="F104" t="s">
-        <v>6728</v>
+        <v>6727</v>
       </c>
       <c r="G104" t="s">
         <v>2380</v>
@@ -52306,7 +52359,7 @@
         <v>1757242</v>
       </c>
       <c r="I104" t="s">
-        <v>6917</v>
+        <v>6916</v>
       </c>
       <c r="J104" t="s">
         <v>2390</v>
@@ -52317,10 +52370,10 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
+        <v>6917</v>
+      </c>
+      <c r="B105" t="s">
         <v>6918</v>
-      </c>
-      <c r="B105" t="s">
-        <v>6919</v>
       </c>
       <c r="C105" t="s">
         <v>5800</v>
@@ -52335,16 +52388,51 @@
         <v>2907</v>
       </c>
       <c r="H105" t="s">
-        <v>6922</v>
+        <v>6921</v>
       </c>
       <c r="I105" t="s">
+        <v>6919</v>
+      </c>
+      <c r="J105" t="s">
         <v>6920</v>
-      </c>
-      <c r="J105" t="s">
-        <v>6921</v>
       </c>
       <c r="K105" s="8">
         <v>1.59</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>6973</v>
+      </c>
+      <c r="B106" t="s">
+        <v>6974</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2387</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106" t="s">
+        <v>4660</v>
+      </c>
+      <c r="G106" t="s">
+        <v>2978</v>
+      </c>
+      <c r="H106" t="s">
+        <v>6975</v>
+      </c>
+      <c r="I106" t="s">
+        <v>6976</v>
+      </c>
+      <c r="J106" t="s">
+        <v>2390</v>
+      </c>
+      <c r="K106" s="8">
+        <v>1.84</v>
       </c>
     </row>
   </sheetData>
@@ -71274,7 +71362,7 @@
     </row>
     <row r="572" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
-        <v>6527</v>
+        <v>6526</v>
       </c>
       <c r="B572" t="str">
         <f>CONCATENATE("CAP",", ",C572,", ",D572,", ",E572,", ",F572,", 1812")</f>
@@ -71287,7 +71375,7 @@
         <v>4344</v>
       </c>
       <c r="E572" t="s">
-        <v>6528</v>
+        <v>6527</v>
       </c>
       <c r="F572" t="s">
         <v>20</v>
@@ -71296,7 +71384,7 @@
         <v>4971</v>
       </c>
       <c r="H572" t="s">
-        <v>6529</v>
+        <v>6528</v>
       </c>
       <c r="I572" t="s">
         <v>5946</v>
@@ -71310,7 +71398,7 @@
     </row>
     <row r="573" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
-        <v>6543</v>
+        <v>6542</v>
       </c>
       <c r="B573" t="str">
         <f>CONCATENATE("CAP ARR x4",", ",C573,", ",D573,", ",E573,", ",F573,", 1812")</f>
@@ -71332,13 +71420,13 @@
         <v>4805</v>
       </c>
       <c r="H573" t="s">
-        <v>6546</v>
+        <v>6545</v>
       </c>
       <c r="I573" t="s">
+        <v>6543</v>
+      </c>
+      <c r="J573" t="s">
         <v>6544</v>
-      </c>
-      <c r="J573" t="s">
-        <v>6545</v>
       </c>
       <c r="K573" s="8">
         <v>0.46</v>
@@ -71346,14 +71434,14 @@
     </row>
     <row r="574" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
-        <v>6780</v>
+        <v>6779</v>
       </c>
       <c r="B574" t="str">
         <f>CONCATENATE("CAP",", ",C574,", ",D574,", ",E574,", ",F574,"")</f>
         <v>CAP, 0.01uF, ±20%, 305VAC, Film X2</v>
       </c>
       <c r="C574" t="s">
-        <v>6781</v>
+        <v>6780</v>
       </c>
       <c r="D574" t="s">
         <v>4327</v>
@@ -71368,7 +71456,7 @@
         <v>1381</v>
       </c>
       <c r="H574" t="s">
-        <v>6782</v>
+        <v>6781</v>
       </c>
       <c r="I574" t="s">
         <v>6142</v>
@@ -71382,7 +71470,7 @@
     </row>
     <row r="575" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
-        <v>6791</v>
+        <v>6790</v>
       </c>
       <c r="B575" t="str">
         <f>CONCATENATE("CAP",", ",C575,", ",D575,", ",E575,", ",F575,", Thru-Hole 0.2in spacing")</f>
@@ -71404,10 +71492,10 @@
         <v>4805</v>
       </c>
       <c r="H575" t="s">
-        <v>6793</v>
+        <v>6792</v>
       </c>
       <c r="I575" t="s">
-        <v>6792</v>
+        <v>6791</v>
       </c>
       <c r="J575" t="s">
         <v>23</v>
@@ -71418,7 +71506,7 @@
     </row>
     <row r="576" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A576" t="s">
-        <v>6796</v>
+        <v>6795</v>
       </c>
       <c r="B576" t="str">
         <f>CONCATENATE("CAP",", ",C576,", ",D576,", ",E576,", ",F576,", Thru-Hole 0.2in spacing")</f>
@@ -71440,10 +71528,10 @@
         <v>4805</v>
       </c>
       <c r="H576" t="s">
+        <v>6793</v>
+      </c>
+      <c r="I576" t="s">
         <v>6794</v>
-      </c>
-      <c r="I576" t="s">
-        <v>6795</v>
       </c>
       <c r="J576" t="s">
         <v>23</v>
@@ -71454,7 +71542,7 @@
     </row>
     <row r="577" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
-        <v>6813</v>
+        <v>6812</v>
       </c>
       <c r="B577" t="str">
         <f>CONCATENATE("CAP",", ",C577,", ",D577,", ",E577,", ",F577,", Thru-Hole 0.2in spacing")</f>
@@ -71476,10 +71564,10 @@
         <v>4805</v>
       </c>
       <c r="H577" t="s">
-        <v>6814</v>
+        <v>6813</v>
       </c>
       <c r="I577" t="s">
-        <v>6795</v>
+        <v>6794</v>
       </c>
       <c r="J577" t="s">
         <v>23</v>
@@ -71490,7 +71578,7 @@
     </row>
     <row r="578" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
-        <v>6815</v>
+        <v>6814</v>
       </c>
       <c r="B578" t="str">
         <f>CONCATENATE("CAP",", ",C578,", ",D578,", ",E578,", ",F578,", Radial/Can")</f>
@@ -71512,10 +71600,10 @@
         <v>1555</v>
       </c>
       <c r="H578" t="s">
-        <v>6817</v>
+        <v>6816</v>
       </c>
       <c r="I578" t="s">
-        <v>6816</v>
+        <v>6815</v>
       </c>
       <c r="J578" t="s">
         <v>2079</v>
@@ -71526,7 +71614,7 @@
     </row>
     <row r="579" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
-        <v>6818</v>
+        <v>6817</v>
       </c>
       <c r="B579" t="str">
         <f>CONCATENATE("CAP",", ",C579,", ",D579,", ",E579,", ",F579,", Radial/Can")</f>
@@ -71545,10 +71633,10 @@
         <v>1842</v>
       </c>
       <c r="G579" t="s">
+        <v>6818</v>
+      </c>
+      <c r="H579" t="s">
         <v>6819</v>
-      </c>
-      <c r="H579" t="s">
-        <v>6820</v>
       </c>
       <c r="I579" t="s">
         <v>5678</v>
@@ -71562,7 +71650,7 @@
     </row>
     <row r="580" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
-        <v>6821</v>
+        <v>6820</v>
       </c>
       <c r="B580" t="str">
         <f>CONCATENATE("CAP",", ",C580,", ",D580,", ",E580,", ",F580,", Thru-Hole 0.2in spacing")</f>
@@ -71584,10 +71672,10 @@
         <v>4805</v>
       </c>
       <c r="H580" t="s">
-        <v>6823</v>
+        <v>6822</v>
       </c>
       <c r="I580" t="s">
-        <v>6822</v>
+        <v>6821</v>
       </c>
       <c r="J580" t="s">
         <v>23</v>
@@ -71598,7 +71686,7 @@
     </row>
     <row r="581" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
-        <v>6840</v>
+        <v>6839</v>
       </c>
       <c r="B581" t="str">
         <f>CONCATENATE("CAP",", ",C581,", ",D581,", ",E581,", ",F581,", Thru-Hole 0.2in spacing")</f>
@@ -71620,10 +71708,10 @@
         <v>4805</v>
       </c>
       <c r="H581" t="s">
-        <v>6841</v>
+        <v>6840</v>
       </c>
       <c r="I581" t="s">
-        <v>6792</v>
+        <v>6791</v>
       </c>
       <c r="J581" t="s">
         <v>23</v>
@@ -71634,7 +71722,7 @@
     </row>
     <row r="582" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
-        <v>6846</v>
+        <v>6845</v>
       </c>
       <c r="B582" t="str">
         <f>CONCATENATE("CAP",", ",C582,", ",D582,", ",E582,", ",F582,", Thru-Hole 0.2in spacing")</f>
@@ -71656,10 +71744,10 @@
         <v>4805</v>
       </c>
       <c r="H582" t="s">
-        <v>6845</v>
+        <v>6844</v>
       </c>
       <c r="I582" t="s">
-        <v>6795</v>
+        <v>6794</v>
       </c>
       <c r="J582" t="s">
         <v>23</v>
@@ -71670,7 +71758,7 @@
     </row>
     <row r="583" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
-        <v>6853</v>
+        <v>6852</v>
       </c>
       <c r="B583" t="str">
         <f>CONCATENATE("CAP",", ",C583,", ",D583,", ",E583,", ",F583,", Thru-Hole 0.2in spacing")</f>
@@ -71692,10 +71780,10 @@
         <v>4805</v>
       </c>
       <c r="H583" t="s">
+        <v>6853</v>
+      </c>
+      <c r="I583" t="s">
         <v>6854</v>
-      </c>
-      <c r="I583" t="s">
-        <v>6855</v>
       </c>
       <c r="J583" t="s">
         <v>23</v>
@@ -71706,7 +71794,7 @@
     </row>
     <row r="584" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
-        <v>6866</v>
+        <v>6865</v>
       </c>
       <c r="B584" t="str">
         <f>CONCATENATE("CAP",", ",C584,", ",D584,", ",E584,", ",F584,", Thru-Hole 0.2in spacing")</f>
@@ -71728,10 +71816,10 @@
         <v>4805</v>
       </c>
       <c r="H584" t="s">
+        <v>6866</v>
+      </c>
+      <c r="I584" t="s">
         <v>6867</v>
-      </c>
-      <c r="I584" t="s">
-        <v>6868</v>
       </c>
       <c r="J584" t="s">
         <v>23</v>
@@ -71742,7 +71830,7 @@
     </row>
     <row r="585" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
-        <v>6899</v>
+        <v>6898</v>
       </c>
       <c r="B585" t="str">
         <f>CONCATENATE("CAP",", ",C585,", ",D585,", ",E585,", ",F585,", 2917")</f>
@@ -71764,10 +71852,10 @@
         <v>4805</v>
       </c>
       <c r="H585" t="s">
+        <v>6899</v>
+      </c>
+      <c r="I585" t="s">
         <v>6900</v>
-      </c>
-      <c r="I585" t="s">
-        <v>6901</v>
       </c>
       <c r="J585" t="s">
         <v>2079</v>
@@ -71778,7 +71866,7 @@
     </row>
     <row r="586" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
-        <v>6903</v>
+        <v>6902</v>
       </c>
       <c r="B586" t="str">
         <f>CONCATENATE("CAP",", ",C586,", ",D586,", ",E586,", ",F586,", 100mOhm, 2917")</f>
@@ -71800,7 +71888,7 @@
         <v>4805</v>
       </c>
       <c r="H586" t="s">
-        <v>6902</v>
+        <v>6901</v>
       </c>
       <c r="I586" t="s">
         <v>5489</v>
@@ -71814,7 +71902,7 @@
     </row>
     <row r="587" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
-        <v>6959</v>
+        <v>6958</v>
       </c>
       <c r="B587" t="str">
         <f>CONCATENATE("CAP",", ",C587,", ",D587,", ",E587,", ",F587,", X2/Y3, 1808")</f>
@@ -71827,16 +71915,16 @@
         <v>6230</v>
       </c>
       <c r="E587" t="s">
-        <v>6962</v>
+        <v>6961</v>
       </c>
       <c r="F587" t="s">
         <v>2613</v>
       </c>
       <c r="G587" t="s">
+        <v>6959</v>
+      </c>
+      <c r="H587" t="s">
         <v>6960</v>
-      </c>
-      <c r="H587" t="s">
-        <v>6961</v>
       </c>
       <c r="I587" t="s">
         <v>4807</v>
@@ -71850,7 +71938,7 @@
     </row>
     <row r="588" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
-        <v>6970</v>
+        <v>6969</v>
       </c>
       <c r="B588" t="str">
         <f>CONCATENATE("CAP",", ",C588,", ",D588,", ",E588,", ",F588,", X2/Y3, 1808")</f>
@@ -71860,10 +71948,10 @@
         <v>2794</v>
       </c>
       <c r="D588" t="s">
-        <v>6971</v>
+        <v>6970</v>
       </c>
       <c r="E588" t="s">
-        <v>6528</v>
+        <v>6527</v>
       </c>
       <c r="F588" t="s">
         <v>2613</v>
@@ -71872,7 +71960,7 @@
         <v>1381</v>
       </c>
       <c r="H588" t="s">
-        <v>6972</v>
+        <v>6971</v>
       </c>
       <c r="I588" t="s">
         <v>4807</v>
@@ -75991,10 +76079,10 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
+        <v>6393</v>
+      </c>
+      <c r="B121" t="s">
         <v>6394</v>
-      </c>
-      <c r="B121" t="s">
-        <v>6395</v>
       </c>
       <c r="C121" t="s">
         <v>1286</v>
@@ -76003,19 +76091,19 @@
         <v>1283</v>
       </c>
       <c r="E121" t="s">
+        <v>6395</v>
+      </c>
+      <c r="H121" t="s">
         <v>6396</v>
-      </c>
-      <c r="H121" t="s">
-        <v>6397</v>
       </c>
       <c r="I121" t="s">
         <v>21</v>
       </c>
       <c r="J121" t="s">
-        <v>6399</v>
+        <v>6398</v>
       </c>
       <c r="K121" t="s">
-        <v>6398</v>
+        <v>6397</v>
       </c>
       <c r="L121" t="s">
         <v>1382</v>
@@ -76026,10 +76114,10 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>6399</v>
+      </c>
+      <c r="B122" t="s">
         <v>6400</v>
-      </c>
-      <c r="B122" t="s">
-        <v>6401</v>
       </c>
       <c r="E122" t="s">
         <v>1229</v>
@@ -76047,10 +76135,10 @@
         <v>21</v>
       </c>
       <c r="J122" t="s">
+        <v>6401</v>
+      </c>
+      <c r="K122" t="s">
         <v>6402</v>
-      </c>
-      <c r="K122" t="s">
-        <v>6403</v>
       </c>
       <c r="L122" t="s">
         <v>36</v>
@@ -76061,10 +76149,10 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>6451</v>
+      </c>
+      <c r="B123" t="s">
         <v>6452</v>
-      </c>
-      <c r="B123" t="s">
-        <v>6453</v>
       </c>
       <c r="F123">
         <v>90</v>
@@ -76073,19 +76161,19 @@
         <v>37</v>
       </c>
       <c r="H123" t="s">
-        <v>6454</v>
+        <v>6453</v>
       </c>
       <c r="I123" t="s">
         <v>21</v>
       </c>
       <c r="J123" t="s">
+        <v>6454</v>
+      </c>
+      <c r="K123" t="s">
         <v>6455</v>
       </c>
-      <c r="K123" t="s">
+      <c r="L123" t="s">
         <v>6456</v>
-      </c>
-      <c r="L123" t="s">
-        <v>6457</v>
       </c>
       <c r="M123" s="8">
         <v>0.53</v>
@@ -76093,10 +76181,10 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>6480</v>
+        <v>6479</v>
       </c>
       <c r="B124" t="s">
-        <v>6483</v>
+        <v>6482</v>
       </c>
       <c r="E124" t="s">
         <v>2119</v>
@@ -76108,7 +76196,7 @@
         <v>37</v>
       </c>
       <c r="H124" t="s">
-        <v>6481</v>
+        <v>6480</v>
       </c>
       <c r="I124" t="s">
         <v>2420</v>
@@ -76117,7 +76205,7 @@
         <v>742792114</v>
       </c>
       <c r="K124" t="s">
-        <v>6482</v>
+        <v>6481</v>
       </c>
       <c r="L124" t="s">
         <v>36</v>
@@ -76128,10 +76216,10 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>6522</v>
+      </c>
+      <c r="B125" t="s">
         <v>6523</v>
-      </c>
-      <c r="B125" t="s">
-        <v>6524</v>
       </c>
       <c r="C125" t="s">
         <v>1290</v>
@@ -76140,7 +76228,7 @@
         <v>5833</v>
       </c>
       <c r="E125" t="s">
-        <v>6525</v>
+        <v>6524</v>
       </c>
       <c r="H125" t="s">
         <v>5024</v>
@@ -76152,7 +76240,7 @@
         <v>744043100</v>
       </c>
       <c r="K125" t="s">
-        <v>6526</v>
+        <v>6525</v>
       </c>
       <c r="L125" t="s">
         <v>1382</v>
@@ -76163,10 +76251,10 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>6590</v>
+      </c>
+      <c r="B126" t="s">
         <v>6591</v>
-      </c>
-      <c r="B126" t="s">
-        <v>6592</v>
       </c>
       <c r="C126" t="s">
         <v>1220</v>
@@ -76178,7 +76266,7 @@
         <v>5984</v>
       </c>
       <c r="G126" t="s">
-        <v>6593</v>
+        <v>6592</v>
       </c>
       <c r="H126" t="s">
         <v>5827</v>
@@ -76187,10 +76275,10 @@
         <v>21</v>
       </c>
       <c r="J126" t="s">
-        <v>6594</v>
+        <v>6593</v>
       </c>
       <c r="K126" t="s">
-        <v>6398</v>
+        <v>6397</v>
       </c>
       <c r="L126" t="s">
         <v>1382</v>
@@ -76201,10 +76289,10 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>6624</v>
+      </c>
+      <c r="B127" t="s">
         <v>6625</v>
-      </c>
-      <c r="B127" t="s">
-        <v>6626</v>
       </c>
       <c r="E127" t="s">
         <v>2119</v>
@@ -76216,16 +76304,16 @@
         <v>37</v>
       </c>
       <c r="H127" t="s">
-        <v>6481</v>
+        <v>6480</v>
       </c>
       <c r="I127" t="s">
         <v>2355</v>
       </c>
       <c r="J127" t="s">
-        <v>6627</v>
+        <v>6626</v>
       </c>
       <c r="K127" t="s">
-        <v>6403</v>
+        <v>6402</v>
       </c>
       <c r="L127" t="s">
         <v>36</v>
@@ -76236,10 +76324,10 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
+        <v>6630</v>
+      </c>
+      <c r="B128" t="s">
         <v>6631</v>
-      </c>
-      <c r="B128" t="s">
-        <v>6632</v>
       </c>
       <c r="E128" t="s">
         <v>1229</v>
@@ -76251,16 +76339,16 @@
         <v>37</v>
       </c>
       <c r="H128" t="s">
-        <v>6633</v>
+        <v>6632</v>
       </c>
       <c r="I128" t="s">
         <v>21</v>
       </c>
       <c r="J128" t="s">
-        <v>6635</v>
+        <v>6634</v>
       </c>
       <c r="K128" t="s">
-        <v>6634</v>
+        <v>6633</v>
       </c>
       <c r="L128" t="s">
         <v>36</v>
@@ -76271,10 +76359,10 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
+        <v>6635</v>
+      </c>
+      <c r="B129" t="s">
         <v>6636</v>
-      </c>
-      <c r="B129" t="s">
-        <v>6637</v>
       </c>
       <c r="E129" t="s">
         <v>1237</v>
@@ -76286,16 +76374,16 @@
         <v>37</v>
       </c>
       <c r="H129" t="s">
-        <v>6638</v>
+        <v>6637</v>
       </c>
       <c r="I129" t="s">
         <v>21</v>
       </c>
       <c r="J129" t="s">
-        <v>6639</v>
+        <v>6638</v>
       </c>
       <c r="K129" t="s">
-        <v>6634</v>
+        <v>6633</v>
       </c>
       <c r="L129" t="s">
         <v>36</v>
@@ -76306,10 +76394,10 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>6640</v>
+      </c>
+      <c r="B130" t="s">
         <v>6641</v>
-      </c>
-      <c r="B130" t="s">
-        <v>6642</v>
       </c>
       <c r="E130" t="s">
         <v>2119</v>
@@ -76327,10 +76415,10 @@
         <v>21</v>
       </c>
       <c r="J130" t="s">
-        <v>6640</v>
+        <v>6639</v>
       </c>
       <c r="K130" t="s">
-        <v>6634</v>
+        <v>6633</v>
       </c>
       <c r="L130" t="s">
         <v>36</v>
@@ -76341,10 +76429,10 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>6735</v>
+        <v>6734</v>
       </c>
       <c r="B131" t="s">
-        <v>6734</v>
+        <v>6733</v>
       </c>
       <c r="C131" t="s">
         <v>1290</v>
@@ -76353,16 +76441,16 @@
         <v>1283</v>
       </c>
       <c r="E131" t="s">
-        <v>6733</v>
+        <v>6732</v>
       </c>
       <c r="H131" t="s">
-        <v>6732</v>
+        <v>6731</v>
       </c>
       <c r="I131" t="s">
         <v>4889</v>
       </c>
       <c r="J131" t="s">
-        <v>6731</v>
+        <v>6730</v>
       </c>
       <c r="K131" t="s">
         <v>5828</v>
@@ -76376,10 +76464,10 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
+        <v>6764</v>
+      </c>
+      <c r="B132" t="s">
         <v>6765</v>
-      </c>
-      <c r="B132" t="s">
-        <v>6766</v>
       </c>
       <c r="C132" t="s">
         <v>1290</v>
@@ -76391,16 +76479,16 @@
         <v>4600</v>
       </c>
       <c r="H132" t="s">
-        <v>6767</v>
+        <v>6766</v>
       </c>
       <c r="I132" t="s">
         <v>4889</v>
       </c>
       <c r="J132" t="s">
+        <v>6767</v>
+      </c>
+      <c r="K132" t="s">
         <v>6768</v>
-      </c>
-      <c r="K132" t="s">
-        <v>6769</v>
       </c>
       <c r="L132" t="s">
         <v>1382</v>
@@ -76411,28 +76499,28 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>6774</v>
+        <v>6773</v>
       </c>
       <c r="B133" t="s">
-        <v>6779</v>
+        <v>6778</v>
       </c>
       <c r="C133" t="s">
-        <v>6778</v>
+        <v>6777</v>
       </c>
       <c r="E133" t="s">
         <v>4600</v>
       </c>
       <c r="H133" t="s">
-        <v>6777</v>
+        <v>6776</v>
       </c>
       <c r="I133" t="s">
         <v>2420</v>
       </c>
       <c r="J133" t="s">
+        <v>6774</v>
+      </c>
+      <c r="K133" t="s">
         <v>6775</v>
-      </c>
-      <c r="K133" t="s">
-        <v>6776</v>
       </c>
       <c r="L133" t="s">
         <v>4899</v>
@@ -76443,19 +76531,19 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
+        <v>6939</v>
+      </c>
+      <c r="B134" t="s">
         <v>6940</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>6941</v>
       </c>
-      <c r="C134" t="s">
+      <c r="E134" t="s">
         <v>6942</v>
       </c>
-      <c r="E134" t="s">
+      <c r="H134" t="s">
         <v>6943</v>
-      </c>
-      <c r="H134" t="s">
-        <v>6944</v>
       </c>
       <c r="I134" t="s">
         <v>2420</v>
@@ -76464,10 +76552,10 @@
         <v>750315228</v>
       </c>
       <c r="K134" t="s">
+        <v>6944</v>
+      </c>
+      <c r="L134" t="s">
         <v>6945</v>
-      </c>
-      <c r="L134" t="s">
-        <v>6946</v>
       </c>
       <c r="M134" s="8">
         <v>2.4</v>
@@ -76747,22 +76835,22 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6384</v>
+        <v>6383</v>
       </c>
       <c r="B14" t="s">
-        <v>6387</v>
+        <v>6386</v>
       </c>
       <c r="C14" t="s">
         <v>2287</v>
       </c>
       <c r="D14" t="s">
+        <v>6384</v>
+      </c>
+      <c r="E14" t="s">
         <v>6385</v>
       </c>
-      <c r="E14" t="s">
-        <v>6386</v>
-      </c>
       <c r="F14" t="s">
-        <v>6385</v>
+        <v>6384</v>
       </c>
     </row>
   </sheetData>
@@ -76933,7 +77021,7 @@
         <v>4253</v>
       </c>
       <c r="E7" t="s">
-        <v>6790</v>
+        <v>6789</v>
       </c>
       <c r="F7" t="s">
         <v>4253</v>
@@ -77367,22 +77455,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>6403</v>
+      </c>
+      <c r="B27" t="s">
         <v>6404</v>
-      </c>
-      <c r="B27" t="s">
-        <v>6405</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
       </c>
       <c r="D27" t="s">
+        <v>6405</v>
+      </c>
+      <c r="E27" t="s">
         <v>6406</v>
       </c>
-      <c r="E27" t="s">
-        <v>6407</v>
-      </c>
       <c r="F27" t="s">
-        <v>6621</v>
+        <v>6620</v>
       </c>
       <c r="G27" s="8">
         <v>1.56</v>
@@ -77390,22 +77478,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>6424</v>
+        <v>6423</v>
       </c>
       <c r="B28" t="s">
-        <v>6428</v>
+        <v>6427</v>
       </c>
       <c r="C28" t="s">
         <v>2331</v>
       </c>
       <c r="D28" t="s">
+        <v>6424</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6426</v>
+      </c>
+      <c r="F28" t="s">
         <v>6425</v>
-      </c>
-      <c r="E28" t="s">
-        <v>6427</v>
-      </c>
-      <c r="F28" t="s">
-        <v>6426</v>
       </c>
       <c r="G28" s="8">
         <v>0.94</v>
@@ -77413,22 +77501,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>6457</v>
+      </c>
+      <c r="B29" t="s">
         <v>6458</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>6459</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>6460</v>
-      </c>
-      <c r="D29" t="s">
-        <v>6461</v>
       </c>
       <c r="E29" t="s">
         <v>2716</v>
       </c>
       <c r="F29" t="s">
-        <v>6462</v>
+        <v>6461</v>
       </c>
       <c r="G29" s="8">
         <v>3.71</v>
@@ -77436,22 +77524,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>6467</v>
+        <v>6466</v>
       </c>
       <c r="B30" t="s">
-        <v>6463</v>
+        <v>6462</v>
       </c>
       <c r="C30" t="s">
         <v>2287</v>
       </c>
       <c r="D30" t="s">
+        <v>6463</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6465</v>
+      </c>
+      <c r="F30" t="s">
         <v>6464</v>
-      </c>
-      <c r="E30" t="s">
-        <v>6466</v>
-      </c>
-      <c r="F30" t="s">
-        <v>6465</v>
       </c>
       <c r="G30" s="8">
         <v>0.51</v>
@@ -77459,10 +77547,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>6665</v>
+        <v>6664</v>
       </c>
       <c r="B31" t="s">
-        <v>6667</v>
+        <v>6666</v>
       </c>
       <c r="C31" t="s">
         <v>4313</v>
@@ -77474,7 +77562,7 @@
         <v>5642</v>
       </c>
       <c r="F31" t="s">
-        <v>6666</v>
+        <v>6665</v>
       </c>
       <c r="G31" s="8">
         <v>6.69</v>
@@ -77482,22 +77570,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>6689</v>
+        <v>6688</v>
       </c>
       <c r="B32" t="s">
-        <v>6692</v>
+        <v>6691</v>
       </c>
       <c r="C32" t="s">
         <v>2287</v>
       </c>
       <c r="D32" t="s">
-        <v>6691</v>
+        <v>6690</v>
       </c>
       <c r="E32" t="s">
         <v>4469</v>
       </c>
       <c r="F32" t="s">
-        <v>6690</v>
+        <v>6689</v>
       </c>
       <c r="G32" s="8">
         <v>4.05</v>
@@ -77505,22 +77593,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>6888</v>
+      </c>
+      <c r="B33" t="s">
         <v>6889</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>6890</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>6891</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6892</v>
       </c>
       <c r="E33" t="s">
         <v>5504</v>
       </c>
       <c r="F33" t="s">
-        <v>6893</v>
+        <v>6892</v>
       </c>
       <c r="G33" s="8">
         <v>2.92</v>
@@ -77623,7 +77711,7 @@
         <v>84</v>
       </c>
       <c r="J2" t="s">
-        <v>6966</v>
+        <v>6965</v>
       </c>
       <c r="K2" t="s">
         <v>85</v>
@@ -79652,16 +79740,16 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>6387</v>
+      </c>
+      <c r="B51" t="s">
         <v>6388</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>6389</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>6390</v>
-      </c>
-      <c r="D51" t="s">
-        <v>6391</v>
       </c>
       <c r="E51" t="s">
         <v>1225</v>
@@ -79676,13 +79764,13 @@
         <v>2287</v>
       </c>
       <c r="J51" t="s">
-        <v>6392</v>
+        <v>6391</v>
       </c>
       <c r="K51" t="s">
         <v>4469</v>
       </c>
       <c r="L51" t="s">
-        <v>6393</v>
+        <v>6392</v>
       </c>
       <c r="M51" s="8">
         <v>1.1299999999999999</v>
@@ -79690,22 +79778,22 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>6418</v>
+      </c>
+      <c r="B52" t="s">
         <v>6419</v>
-      </c>
-      <c r="B52" t="s">
-        <v>6420</v>
       </c>
       <c r="I52" t="s">
         <v>2287</v>
       </c>
       <c r="J52" t="s">
+        <v>6420</v>
+      </c>
+      <c r="K52" t="s">
+        <v>6422</v>
+      </c>
+      <c r="L52" t="s">
         <v>6421</v>
-      </c>
-      <c r="K52" t="s">
-        <v>6423</v>
-      </c>
-      <c r="L52" t="s">
-        <v>6422</v>
       </c>
       <c r="M52" s="8">
         <v>5.4</v>
@@ -79713,22 +79801,22 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>6438</v>
+      </c>
+      <c r="B53" t="s">
         <v>6439</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>6440</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>6441</v>
-      </c>
-      <c r="D53" t="s">
-        <v>6442</v>
       </c>
       <c r="E53" t="s">
         <v>70</v>
       </c>
       <c r="G53" t="s">
-        <v>6443</v>
+        <v>6442</v>
       </c>
       <c r="H53" t="s">
         <v>2519</v>
@@ -79737,13 +79825,13 @@
         <v>2287</v>
       </c>
       <c r="J53" t="s">
-        <v>6446</v>
+        <v>6445</v>
       </c>
       <c r="K53" t="s">
-        <v>6445</v>
+        <v>6444</v>
       </c>
       <c r="L53" t="s">
-        <v>6444</v>
+        <v>6443</v>
       </c>
       <c r="M53" s="8">
         <v>4.55</v>
@@ -79751,34 +79839,34 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>6467</v>
+      </c>
+      <c r="B54" t="s">
         <v>6468</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>6469</v>
       </c>
-      <c r="C54" t="s">
-        <v>6470</v>
-      </c>
       <c r="D54" t="s">
-        <v>6470</v>
+        <v>6469</v>
       </c>
       <c r="E54" t="s">
         <v>70</v>
       </c>
       <c r="G54" t="s">
-        <v>6471</v>
+        <v>6470</v>
       </c>
       <c r="I54" t="s">
         <v>2287</v>
       </c>
       <c r="J54" t="s">
+        <v>6471</v>
+      </c>
+      <c r="K54" t="s">
         <v>6472</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>6473</v>
-      </c>
-      <c r="L54" t="s">
-        <v>6474</v>
       </c>
       <c r="M54" s="8">
         <v>1.56</v>
@@ -79786,10 +79874,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>6488</v>
+      </c>
+      <c r="B55" t="s">
         <v>6489</v>
-      </c>
-      <c r="B55" t="s">
-        <v>6490</v>
       </c>
       <c r="E55" t="s">
         <v>2111</v>
@@ -79801,13 +79889,13 @@
         <v>2287</v>
       </c>
       <c r="J55" t="s">
-        <v>6491</v>
+        <v>6490</v>
       </c>
       <c r="K55" t="s">
         <v>4469</v>
       </c>
       <c r="L55" t="s">
-        <v>6492</v>
+        <v>6491</v>
       </c>
       <c r="M55" s="8">
         <v>1.92</v>
@@ -79815,16 +79903,16 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>6496</v>
+      </c>
+      <c r="B56" t="s">
         <v>6497</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>6498</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>6499</v>
-      </c>
-      <c r="D56" t="s">
-        <v>6500</v>
       </c>
       <c r="E56" t="s">
         <v>2119</v>
@@ -79836,13 +79924,13 @@
         <v>2287</v>
       </c>
       <c r="J56" t="s">
-        <v>6501</v>
+        <v>6500</v>
       </c>
       <c r="K56" t="s">
         <v>2558</v>
       </c>
       <c r="L56" t="s">
-        <v>6502</v>
+        <v>6501</v>
       </c>
       <c r="M56" s="8">
         <v>0.89</v>
@@ -79850,16 +79938,16 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>6502</v>
+      </c>
+      <c r="B57" t="s">
         <v>6503</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>6504</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>6505</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6506</v>
       </c>
       <c r="E57" t="s">
         <v>2119</v>
@@ -79874,13 +79962,13 @@
         <v>2287</v>
       </c>
       <c r="J57" t="s">
-        <v>6507</v>
+        <v>6506</v>
       </c>
       <c r="K57" t="s">
         <v>4698</v>
       </c>
       <c r="L57" t="s">
-        <v>6508</v>
+        <v>6507</v>
       </c>
       <c r="M57" s="8">
         <v>4.3099999999999996</v>
@@ -79888,13 +79976,13 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>6516</v>
+      </c>
+      <c r="B58" t="s">
         <v>6517</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>6518</v>
-      </c>
-      <c r="C58" t="s">
-        <v>6519</v>
       </c>
       <c r="D58" t="s">
         <v>2944</v>
@@ -79909,16 +79997,16 @@
         <v>2519</v>
       </c>
       <c r="I58" t="s">
+        <v>6519</v>
+      </c>
+      <c r="J58" t="s">
         <v>6520</v>
       </c>
-      <c r="J58" t="s">
+      <c r="K58" t="s">
         <v>6521</v>
       </c>
-      <c r="K58" t="s">
-        <v>6522</v>
-      </c>
       <c r="L58" t="s">
-        <v>6522</v>
+        <v>6521</v>
       </c>
       <c r="M58" s="8">
         <v>5.71</v>
@@ -79926,13 +80014,13 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>6533</v>
+        <v>6532</v>
       </c>
       <c r="B59" t="s">
-        <v>6530</v>
+        <v>6529</v>
       </c>
       <c r="C59" t="s">
-        <v>6519</v>
+        <v>6518</v>
       </c>
       <c r="D59" t="s">
         <v>2944</v>
@@ -79947,16 +80035,16 @@
         <v>2519</v>
       </c>
       <c r="I59" t="s">
-        <v>6520</v>
+        <v>6519</v>
       </c>
       <c r="J59" t="s">
+        <v>6530</v>
+      </c>
+      <c r="K59" t="s">
         <v>6531</v>
       </c>
-      <c r="K59" t="s">
-        <v>6532</v>
-      </c>
       <c r="L59" t="s">
-        <v>6532</v>
+        <v>6531</v>
       </c>
       <c r="M59" s="8">
         <v>3.41</v>
@@ -79964,13 +80052,13 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6552</v>
+        <v>6551</v>
       </c>
       <c r="B60" t="s">
-        <v>6551</v>
+        <v>6550</v>
       </c>
       <c r="C60" t="s">
-        <v>6550</v>
+        <v>6549</v>
       </c>
       <c r="D60" t="s">
         <v>2170</v>
@@ -79988,13 +80076,13 @@
         <v>21</v>
       </c>
       <c r="J60" t="s">
-        <v>6549</v>
+        <v>6548</v>
       </c>
       <c r="K60" t="s">
+        <v>6546</v>
+      </c>
+      <c r="L60" t="s">
         <v>6547</v>
-      </c>
-      <c r="L60" t="s">
-        <v>6548</v>
       </c>
       <c r="M60" s="8">
         <v>32</v>
@@ -80002,16 +80090,16 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>6575</v>
+        <v>6574</v>
       </c>
       <c r="B61" t="s">
+        <v>6576</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>6578</v>
+      </c>
+      <c r="D61" s="11" t="s">
         <v>6577</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>6579</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>6578</v>
       </c>
       <c r="E61" t="s">
         <v>70</v>
@@ -80026,13 +80114,13 @@
         <v>2287</v>
       </c>
       <c r="J61" t="s">
+        <v>6579</v>
+      </c>
+      <c r="K61" t="s">
+        <v>6575</v>
+      </c>
+      <c r="L61" t="s">
         <v>6580</v>
-      </c>
-      <c r="K61" t="s">
-        <v>6576</v>
-      </c>
-      <c r="L61" t="s">
-        <v>6581</v>
       </c>
       <c r="M61" s="8">
         <v>1.58</v>
@@ -80040,16 +80128,16 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>6750</v>
+        <v>6749</v>
       </c>
       <c r="B62" t="s">
-        <v>6752</v>
+        <v>6751</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>6579</v>
+        <v>6578</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>6578</v>
+        <v>6577</v>
       </c>
       <c r="E62" t="s">
         <v>2938</v>
@@ -80064,13 +80152,13 @@
         <v>2091</v>
       </c>
       <c r="J62" t="s">
-        <v>6753</v>
+        <v>6752</v>
       </c>
       <c r="K62" t="s">
         <v>4469</v>
       </c>
       <c r="L62" t="s">
-        <v>6754</v>
+        <v>6753</v>
       </c>
       <c r="M62" s="8">
         <v>0.79</v>
@@ -80078,16 +80166,16 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>6751</v>
+        <v>6750</v>
       </c>
       <c r="B63" t="s">
-        <v>6755</v>
+        <v>6754</v>
       </c>
       <c r="C63" t="s">
+        <v>6757</v>
+      </c>
+      <c r="D63" t="s">
         <v>6758</v>
-      </c>
-      <c r="D63" t="s">
-        <v>6759</v>
       </c>
       <c r="E63" t="s">
         <v>2938</v>
@@ -80102,13 +80190,13 @@
         <v>2091</v>
       </c>
       <c r="J63" t="s">
-        <v>6756</v>
+        <v>6755</v>
       </c>
       <c r="K63" t="s">
         <v>4469</v>
       </c>
       <c r="L63" t="s">
-        <v>6757</v>
+        <v>6756</v>
       </c>
       <c r="M63" s="8">
         <v>0.37</v>
@@ -80116,19 +80204,19 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>6785</v>
+      </c>
+      <c r="B64" t="s">
         <v>6786</v>
       </c>
-      <c r="B64" t="s">
-        <v>6787</v>
-      </c>
       <c r="C64" t="s">
-        <v>6519</v>
+        <v>6518</v>
       </c>
       <c r="D64" t="s">
         <v>4765</v>
       </c>
       <c r="E64" t="s">
-        <v>6788</v>
+        <v>6787</v>
       </c>
       <c r="G64" t="s">
         <v>5071</v>
@@ -80137,16 +80225,16 @@
         <v>2519</v>
       </c>
       <c r="I64" t="s">
-        <v>6520</v>
+        <v>6519</v>
       </c>
       <c r="J64" t="s">
-        <v>6789</v>
+        <v>6788</v>
       </c>
       <c r="K64" t="s">
-        <v>6522</v>
+        <v>6521</v>
       </c>
       <c r="L64" t="s">
-        <v>6522</v>
+        <v>6521</v>
       </c>
       <c r="M64" s="8">
         <v>5.71</v>
@@ -80154,16 +80242,16 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>6797</v>
+      </c>
+      <c r="B65" t="s">
         <v>6798</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>6799</v>
       </c>
-      <c r="C65" t="s">
+      <c r="G65" t="s">
         <v>6800</v>
-      </c>
-      <c r="G65" t="s">
-        <v>6801</v>
       </c>
       <c r="H65" t="s">
         <v>73</v>
@@ -80172,7 +80260,7 @@
         <v>2287</v>
       </c>
       <c r="J65" t="s">
-        <v>6797</v>
+        <v>6796</v>
       </c>
       <c r="K65" t="s">
         <v>5331</v>
@@ -80186,19 +80274,19 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>6946</v>
+      </c>
+      <c r="B66" t="s">
+        <v>6951</v>
+      </c>
+      <c r="C66" t="s">
         <v>6947</v>
-      </c>
-      <c r="B66" t="s">
-        <v>6952</v>
-      </c>
-      <c r="C66" t="s">
-        <v>6948</v>
       </c>
       <c r="E66" t="s">
         <v>70</v>
       </c>
       <c r="G66" t="s">
-        <v>6949</v>
+        <v>6948</v>
       </c>
       <c r="H66" t="s">
         <v>73</v>
@@ -80207,13 +80295,13 @@
         <v>2287</v>
       </c>
       <c r="J66" t="s">
-        <v>6951</v>
+        <v>6950</v>
       </c>
       <c r="K66" t="s">
         <v>2558</v>
       </c>
       <c r="L66" t="s">
-        <v>6950</v>
+        <v>6949</v>
       </c>
       <c r="M66" s="8">
         <v>2.7</v>
@@ -81705,19 +81793,19 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>6343</v>
+        <v>6342</v>
       </c>
       <c r="B66" t="s">
-        <v>6345</v>
+        <v>6344</v>
       </c>
       <c r="C66" t="s">
         <v>4313</v>
       </c>
       <c r="D66" t="s">
-        <v>6344</v>
+        <v>6343</v>
       </c>
       <c r="E66" t="s">
-        <v>6346</v>
+        <v>6345</v>
       </c>
       <c r="F66" t="s">
         <v>4714</v>
@@ -81728,22 +81816,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>6347</v>
+        <v>6346</v>
       </c>
       <c r="B67" t="s">
-        <v>6351</v>
+        <v>6350</v>
       </c>
       <c r="C67" t="s">
         <v>2287</v>
       </c>
       <c r="D67" t="s">
-        <v>6350</v>
+        <v>6349</v>
       </c>
       <c r="E67" t="s">
-        <v>6349</v>
+        <v>6348</v>
       </c>
       <c r="F67" t="s">
-        <v>6348</v>
+        <v>6347</v>
       </c>
       <c r="G67" s="8">
         <v>2.7</v>
@@ -81751,22 +81839,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>6372</v>
+      </c>
+      <c r="B68" t="s">
         <v>6373</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>6374</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
+        <v>6377</v>
+      </c>
+      <c r="E68" t="s">
         <v>6375</v>
       </c>
-      <c r="D68" t="s">
-        <v>6378</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>6376</v>
-      </c>
-      <c r="F68" t="s">
-        <v>6377</v>
       </c>
       <c r="G68" s="8">
         <v>8.4499999999999993</v>
@@ -81774,22 +81862,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>6559</v>
+      </c>
+      <c r="B69" t="s">
         <v>6560</v>
-      </c>
-      <c r="B69" t="s">
-        <v>6561</v>
       </c>
       <c r="C69" t="s">
         <v>2091</v>
       </c>
       <c r="D69" t="s">
+        <v>6561</v>
+      </c>
+      <c r="E69" t="s">
         <v>6562</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>6563</v>
-      </c>
-      <c r="F69" t="s">
-        <v>6564</v>
       </c>
       <c r="G69" s="8">
         <v>1.32</v>
@@ -81797,16 +81885,16 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>6564</v>
+      </c>
+      <c r="B70" t="s">
         <v>6565</v>
-      </c>
-      <c r="B70" t="s">
-        <v>6566</v>
       </c>
       <c r="C70" t="s">
         <v>2287</v>
       </c>
       <c r="D70" t="s">
-        <v>6567</v>
+        <v>6566</v>
       </c>
       <c r="E70" t="s">
         <v>4469</v>
@@ -81820,16 +81908,16 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>6568</v>
+        <v>6567</v>
       </c>
       <c r="B71" t="s">
-        <v>6570</v>
+        <v>6569</v>
       </c>
       <c r="C71" t="s">
         <v>2091</v>
       </c>
       <c r="D71" t="s">
-        <v>6569</v>
+        <v>6568</v>
       </c>
       <c r="E71" t="s">
         <v>5189</v>
@@ -81843,22 +81931,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>6570</v>
+      </c>
+      <c r="B72" t="s">
         <v>6571</v>
-      </c>
-      <c r="B72" t="s">
-        <v>6572</v>
       </c>
       <c r="C72" t="s">
         <v>4313</v>
       </c>
       <c r="D72" t="s">
+        <v>6572</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6562</v>
+      </c>
+      <c r="F72" t="s">
         <v>6573</v>
-      </c>
-      <c r="E72" t="s">
-        <v>6563</v>
-      </c>
-      <c r="F72" t="s">
-        <v>6574</v>
       </c>
       <c r="G72" s="8">
         <v>4.3499999999999996</v>
@@ -81866,22 +81954,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>6657</v>
+      </c>
+      <c r="B73" t="s">
         <v>6658</v>
       </c>
-      <c r="B73" t="s">
-        <v>6659</v>
-      </c>
       <c r="C73" t="s">
-        <v>6375</v>
+        <v>6374</v>
       </c>
       <c r="D73" t="s">
-        <v>6661</v>
+        <v>6660</v>
       </c>
       <c r="E73" t="s">
         <v>4469</v>
       </c>
       <c r="F73" t="s">
-        <v>6660</v>
+        <v>6659</v>
       </c>
       <c r="G73" s="8">
         <v>7.61</v>
@@ -81889,22 +81977,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>6661</v>
+      </c>
+      <c r="B74" t="s">
         <v>6662</v>
-      </c>
-      <c r="B74" t="s">
-        <v>6663</v>
       </c>
       <c r="C74" t="s">
         <v>2430</v>
       </c>
       <c r="D74" t="s">
-        <v>6664</v>
+        <v>6663</v>
       </c>
       <c r="E74" t="s">
         <v>5504</v>
       </c>
       <c r="F74" t="s">
-        <v>6664</v>
+        <v>6663</v>
       </c>
       <c r="G74" s="8">
         <v>1.77</v>
@@ -81912,22 +82000,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>6667</v>
+      </c>
+      <c r="B75" t="s">
         <v>6668</v>
-      </c>
-      <c r="B75" t="s">
-        <v>6669</v>
       </c>
       <c r="C75" t="s">
         <v>2287</v>
       </c>
       <c r="D75" t="s">
-        <v>6670</v>
+        <v>6669</v>
       </c>
       <c r="E75" t="s">
         <v>4509</v>
       </c>
       <c r="F75" t="s">
-        <v>6671</v>
+        <v>6670</v>
       </c>
       <c r="G75" s="8">
         <v>8.27</v>
@@ -81935,16 +82023,16 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>6747</v>
+      </c>
+      <c r="B76" t="s">
         <v>6748</v>
-      </c>
-      <c r="B76" t="s">
-        <v>6749</v>
       </c>
       <c r="C76" t="s">
         <v>4313</v>
       </c>
       <c r="D76" t="s">
-        <v>6573</v>
+        <v>6572</v>
       </c>
       <c r="E76" t="s">
         <v>4469</v>
@@ -81958,22 +82046,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>6832</v>
+      </c>
+      <c r="B77" t="s">
         <v>6833</v>
-      </c>
-      <c r="B77" t="s">
-        <v>6834</v>
       </c>
       <c r="C77" t="s">
         <v>4313</v>
       </c>
       <c r="D77" t="s">
-        <v>6835</v>
+        <v>6834</v>
       </c>
       <c r="E77" t="s">
         <v>5331</v>
       </c>
       <c r="F77" t="s">
-        <v>6836</v>
+        <v>6835</v>
       </c>
       <c r="G77" s="8">
         <v>5.96</v>
@@ -81981,16 +82069,16 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>6837</v>
+        <v>6836</v>
       </c>
       <c r="B78" t="s">
-        <v>6839</v>
+        <v>6838</v>
       </c>
       <c r="C78" t="s">
         <v>2287</v>
       </c>
       <c r="D78" t="s">
-        <v>6838</v>
+        <v>6837</v>
       </c>
       <c r="E78" t="s">
         <v>5356</v>
@@ -82004,16 +82092,16 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>6846</v>
+      </c>
+      <c r="B79" t="s">
         <v>6847</v>
-      </c>
-      <c r="B79" t="s">
-        <v>6848</v>
       </c>
       <c r="C79" t="s">
         <v>2287</v>
       </c>
       <c r="D79" t="s">
-        <v>6849</v>
+        <v>6848</v>
       </c>
       <c r="E79" t="s">
         <v>5209</v>
@@ -82027,16 +82115,16 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>6850</v>
+        <v>6849</v>
       </c>
       <c r="B80" t="s">
-        <v>6852</v>
+        <v>6851</v>
       </c>
       <c r="C80" t="s">
         <v>2287</v>
       </c>
       <c r="D80" t="s">
-        <v>6851</v>
+        <v>6850</v>
       </c>
       <c r="E80" t="s">
         <v>5331</v>
@@ -82050,22 +82138,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>6903</v>
+      </c>
+      <c r="B81" t="s">
         <v>6904</v>
-      </c>
-      <c r="B81" t="s">
-        <v>6905</v>
       </c>
       <c r="C81" t="s">
         <v>2287</v>
       </c>
       <c r="D81" t="s">
-        <v>6906</v>
+        <v>6905</v>
       </c>
       <c r="E81" t="s">
         <v>5504</v>
       </c>
       <c r="F81" t="s">
-        <v>6907</v>
+        <v>6906</v>
       </c>
       <c r="G81" s="8">
         <v>0.49</v>
@@ -82073,22 +82161,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>6922</v>
+      </c>
+      <c r="B82" t="s">
         <v>6923</v>
-      </c>
-      <c r="B82" t="s">
-        <v>6924</v>
       </c>
       <c r="C82" t="s">
         <v>2287</v>
       </c>
       <c r="D82" t="s">
-        <v>6926</v>
+        <v>6925</v>
       </c>
       <c r="E82" t="s">
         <v>6212</v>
       </c>
       <c r="F82" t="s">
-        <v>6925</v>
+        <v>6924</v>
       </c>
       <c r="G82" s="8">
         <v>1.45</v>
@@ -82096,16 +82184,16 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>6962</v>
+      </c>
+      <c r="B83" t="s">
         <v>6963</v>
-      </c>
-      <c r="B83" t="s">
-        <v>6964</v>
       </c>
       <c r="C83" t="s">
         <v>2287</v>
       </c>
       <c r="D83" t="s">
-        <v>6965</v>
+        <v>6964</v>
       </c>
       <c r="E83" t="s">
         <v>4469</v>
@@ -83001,22 +83089,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>6407</v>
+      </c>
+      <c r="B41" t="s">
         <v>6408</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>6409</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>6410</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>6411</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>6412</v>
-      </c>
-      <c r="F41" t="s">
-        <v>6413</v>
       </c>
       <c r="G41" s="8">
         <v>8.19</v>
@@ -83024,22 +83112,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>6512</v>
+      </c>
+      <c r="B42" t="s">
         <v>6513</v>
-      </c>
-      <c r="B42" t="s">
-        <v>6514</v>
       </c>
       <c r="C42" t="s">
         <v>2287</v>
       </c>
       <c r="D42" t="s">
-        <v>6515</v>
+        <v>6514</v>
       </c>
       <c r="E42" t="s">
         <v>2521</v>
       </c>
       <c r="F42" t="s">
-        <v>6516</v>
+        <v>6515</v>
       </c>
       <c r="G42" s="8">
         <v>0.32</v>
@@ -83047,22 +83135,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>6552</v>
+      </c>
+      <c r="B43" t="s">
         <v>6553</v>
-      </c>
-      <c r="B43" t="s">
-        <v>6554</v>
       </c>
       <c r="C43" t="s">
         <v>2287</v>
       </c>
       <c r="D43" t="s">
-        <v>6555</v>
+        <v>6554</v>
       </c>
       <c r="E43" t="s">
         <v>4299</v>
       </c>
       <c r="F43" t="s">
-        <v>6556</v>
+        <v>6555</v>
       </c>
       <c r="G43" s="8">
         <v>0.39</v>
@@ -83070,22 +83158,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>6594</v>
+      </c>
+      <c r="B44" t="s">
         <v>6595</v>
-      </c>
-      <c r="B44" t="s">
-        <v>6596</v>
       </c>
       <c r="C44" t="s">
         <v>2287</v>
       </c>
       <c r="D44" t="s">
-        <v>6598</v>
+        <v>6597</v>
       </c>
       <c r="E44" t="s">
         <v>2558</v>
       </c>
       <c r="F44" t="s">
-        <v>6597</v>
+        <v>6596</v>
       </c>
       <c r="G44" s="8">
         <v>0.37</v>
@@ -83093,22 +83181,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>6842</v>
+        <v>6841</v>
       </c>
       <c r="B45" t="s">
-        <v>6844</v>
+        <v>6843</v>
       </c>
       <c r="C45" t="s">
         <v>2287</v>
       </c>
       <c r="D45" t="s">
-        <v>6843</v>
+        <v>6842</v>
       </c>
       <c r="E45" t="s">
         <v>5209</v>
       </c>
       <c r="F45" t="s">
-        <v>6556</v>
+        <v>6555</v>
       </c>
       <c r="G45" s="8">
         <v>0.4</v>

</xml_diff>

<commit_message>
Add 7x1 0.1 inch header among other things
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17014" uniqueCount="6983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17021" uniqueCount="6987">
   <si>
     <t>Part Number</t>
   </si>
@@ -20980,6 +20980,18 @@
   </si>
   <si>
     <t>WS2812B, Intelligent RGB LED Chip, 3.5~5.3V, 5x5mm (5050) SMD</t>
+  </si>
+  <si>
+    <t>CONN-00105</t>
+  </si>
+  <si>
+    <t>Header, 7x1, 0.1"</t>
+  </si>
+  <si>
+    <t>TSW-107-07-F-S</t>
+  </si>
+  <si>
+    <t>HDDR_7x1_0</t>
   </si>
 </sst>
 </file>
@@ -42612,7 +42624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
@@ -49017,10 +49029,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L106"/>
+  <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I107" sqref="I107"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52433,6 +52445,38 @@
       </c>
       <c r="K106" s="8">
         <v>1.84</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>6983</v>
+      </c>
+      <c r="B107" t="s">
+        <v>6984</v>
+      </c>
+      <c r="C107" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D107">
+        <v>7</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="G107" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H107" t="s">
+        <v>6985</v>
+      </c>
+      <c r="I107" t="s">
+        <v>6986</v>
+      </c>
+      <c r="J107" t="s">
+        <v>4247</v>
+      </c>
+      <c r="K107" s="8">
+        <v>0.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add several 0.1 inch connectors
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17021" uniqueCount="6987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17070" uniqueCount="7020">
   <si>
     <t>Part Number</t>
   </si>
@@ -20992,6 +20992,105 @@
   </si>
   <si>
     <t>HDDR_7x1_0</t>
+  </si>
+  <si>
+    <t>CONN-00106</t>
+  </si>
+  <si>
+    <t>CONN-00107</t>
+  </si>
+  <si>
+    <t>CONN-00108</t>
+  </si>
+  <si>
+    <t>CONN-00109</t>
+  </si>
+  <si>
+    <t>CONN-00110</t>
+  </si>
+  <si>
+    <t>Header, 5x1, 0.1"</t>
+  </si>
+  <si>
+    <t>TSW-105-07-F-S</t>
+  </si>
+  <si>
+    <t>Header, 9x1, 0.1"</t>
+  </si>
+  <si>
+    <t>TSW-109-07-F-S</t>
+  </si>
+  <si>
+    <t>Header, 11x1, 0.1"</t>
+  </si>
+  <si>
+    <t>Header, 13x1, 0.1"</t>
+  </si>
+  <si>
+    <t>Header, 17x1, 0.1"</t>
+  </si>
+  <si>
+    <t>TSW-111-07-F-S</t>
+  </si>
+  <si>
+    <t>TSW-113-07-F-S</t>
+  </si>
+  <si>
+    <t>TSW-117-07-F-S</t>
+  </si>
+  <si>
+    <t>CONN-00111</t>
+  </si>
+  <si>
+    <t>CONN-00112</t>
+  </si>
+  <si>
+    <t>Header, 19x1, 0.1"</t>
+  </si>
+  <si>
+    <t>Header, 20x1, 0.1"</t>
+  </si>
+  <si>
+    <t>TSW-119-07-F-S</t>
+  </si>
+  <si>
+    <t>TSW-120-07-F-S</t>
+  </si>
+  <si>
+    <t>HDDR_5x1_0</t>
+  </si>
+  <si>
+    <t>HDDR_9x1_0</t>
+  </si>
+  <si>
+    <t>HDDR_11x1_0</t>
+  </si>
+  <si>
+    <t>HDDR_13x1_0</t>
+  </si>
+  <si>
+    <t>HDDR_17x1_0</t>
+  </si>
+  <si>
+    <t>HDDR_19x1_0</t>
+  </si>
+  <si>
+    <t>HDDR_20x1_0</t>
+  </si>
+  <si>
+    <t>conn-11x1_0</t>
+  </si>
+  <si>
+    <t>conn-13x1_0</t>
+  </si>
+  <si>
+    <t>conn-17x1_0</t>
+  </si>
+  <si>
+    <t>conn-19x1_0</t>
+  </si>
+  <si>
+    <t>conn-20x1_0</t>
   </si>
 </sst>
 </file>
@@ -49029,10 +49128,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108"/>
+      <selection activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52477,6 +52576,209 @@
       </c>
       <c r="K107" s="8">
         <v>0.61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>6987</v>
+      </c>
+      <c r="B108" t="s">
+        <v>6992</v>
+      </c>
+      <c r="C108" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D108">
+        <v>5</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+      <c r="G108" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H108" t="s">
+        <v>6993</v>
+      </c>
+      <c r="I108" t="s">
+        <v>7008</v>
+      </c>
+      <c r="J108" t="s">
+        <v>4248</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>6988</v>
+      </c>
+      <c r="B109" t="s">
+        <v>6994</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D109">
+        <v>9</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="G109" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H109" t="s">
+        <v>6995</v>
+      </c>
+      <c r="I109" t="s">
+        <v>7009</v>
+      </c>
+      <c r="J109" t="s">
+        <v>5042</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>6989</v>
+      </c>
+      <c r="B110" t="s">
+        <v>6996</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D110">
+        <v>11</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="G110" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H110" t="s">
+        <v>6999</v>
+      </c>
+      <c r="I110" t="s">
+        <v>7010</v>
+      </c>
+      <c r="J110" t="s">
+        <v>7015</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>6990</v>
+      </c>
+      <c r="B111" t="s">
+        <v>6997</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D111">
+        <v>13</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="G111" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H111" t="s">
+        <v>7000</v>
+      </c>
+      <c r="I111" t="s">
+        <v>7011</v>
+      </c>
+      <c r="J111" t="s">
+        <v>7016</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>6991</v>
+      </c>
+      <c r="B112" t="s">
+        <v>6998</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D112">
+        <v>17</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="G112" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H112" t="s">
+        <v>7001</v>
+      </c>
+      <c r="I112" t="s">
+        <v>7012</v>
+      </c>
+      <c r="J112" t="s">
+        <v>7017</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>7002</v>
+      </c>
+      <c r="B113" t="s">
+        <v>7004</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D113">
+        <v>19</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="G113" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H113" t="s">
+        <v>7006</v>
+      </c>
+      <c r="I113" t="s">
+        <v>7013</v>
+      </c>
+      <c r="J113" t="s">
+        <v>7018</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>7003</v>
+      </c>
+      <c r="B114" t="s">
+        <v>7005</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D114">
+        <v>20</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="G114" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H114" t="s">
+        <v>7007</v>
+      </c>
+      <c r="I114" t="s">
+        <v>7014</v>
+      </c>
+      <c r="J114" t="s">
+        <v>7019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add TUSB7340 and fix that one Phoenix Contact header footprint
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17070" uniqueCount="7020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17085" uniqueCount="7026">
   <si>
     <t>Part Number</t>
   </si>
@@ -21091,6 +21091,24 @@
   </si>
   <si>
     <t>conn-20x1_0</t>
+  </si>
+  <si>
+    <t>CAP-00587</t>
+  </si>
+  <si>
+    <t>CL31A226KAHNNNE</t>
+  </si>
+  <si>
+    <t>IFACE-00032</t>
+  </si>
+  <si>
+    <t>IC, PCIe to USB 3.0 Bridge, PWQFN-100</t>
+  </si>
+  <si>
+    <t>TUSB7340</t>
+  </si>
+  <si>
+    <t>PWQFN-N100-DUAL-ROW</t>
   </si>
 </sst>
 </file>
@@ -49130,7 +49148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
@@ -52789,10 +52807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K588"/>
+  <dimension ref="A1:K589"/>
   <sheetViews>
     <sheetView topLeftCell="A575" workbookViewId="0">
-      <selection activeCell="B589" sqref="B589"/>
+      <selection activeCell="E590" sqref="E590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72316,6 +72334,42 @@
       </c>
       <c r="K588" s="8">
         <v>0.67</v>
+      </c>
+    </row>
+    <row r="589" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A589" t="s">
+        <v>7020</v>
+      </c>
+      <c r="B589" t="str">
+        <f>CONCATENATE("CAP",", ",C589,", ",D589,", ",E589,", ",F589,", 1206")</f>
+        <v>CAP, 22uF, ±10%, 25V, X5R, 1206</v>
+      </c>
+      <c r="C589" t="s">
+        <v>1819</v>
+      </c>
+      <c r="D589" t="s">
+        <v>4344</v>
+      </c>
+      <c r="E589" t="s">
+        <v>27</v>
+      </c>
+      <c r="F589" t="s">
+        <v>4326</v>
+      </c>
+      <c r="G589" t="s">
+        <v>5112</v>
+      </c>
+      <c r="H589" t="s">
+        <v>7021</v>
+      </c>
+      <c r="I589" t="s">
+        <v>1471</v>
+      </c>
+      <c r="J589" t="s">
+        <v>23</v>
+      </c>
+      <c r="K589" s="8">
+        <v>0.41</v>
       </c>
     </row>
   </sheetData>
@@ -77207,10 +77261,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -77958,6 +78012,29 @@
       </c>
       <c r="G33" s="8">
         <v>2.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>7022</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7023</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7024</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7025</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7024</v>
+      </c>
+      <c r="G34" s="8">
+        <v>14.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a few support components for the TUSB7340 among other misc stuff
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17085" uniqueCount="7026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17121" uniqueCount="7045">
   <si>
     <t>Part Number</t>
   </si>
@@ -21109,6 +21109,63 @@
   </si>
   <si>
     <t>PWQFN-N100-DUAL-ROW</t>
+  </si>
+  <si>
+    <t>LOGIC-00044</t>
+  </si>
+  <si>
+    <t>1G86</t>
+  </si>
+  <si>
+    <t>SN74AHC1G86DBVR</t>
+  </si>
+  <si>
+    <t>IC, XOR, Single 2-Input, 1.65~5.5V, SOT-23-5</t>
+  </si>
+  <si>
+    <t>CAP-00588</t>
+  </si>
+  <si>
+    <t>CP_SMD_8x10</t>
+  </si>
+  <si>
+    <t>UCW1V221MNL1GS</t>
+  </si>
+  <si>
+    <t>PWREG-00065</t>
+  </si>
+  <si>
+    <t>1.1V ~ 5.5V</t>
+  </si>
+  <si>
+    <t>0.8V ~ 3.6V</t>
+  </si>
+  <si>
+    <t>TPS74901RGWR</t>
+  </si>
+  <si>
+    <t>VQFN_20_EP</t>
+  </si>
+  <si>
+    <t>TPS74901RGW</t>
+  </si>
+  <si>
+    <t>REG, Linear, Pos Adj 3A, En + Soft-Start, VQFN-20</t>
+  </si>
+  <si>
+    <t>OSC-00007</t>
+  </si>
+  <si>
+    <t>XTAL, 48MHz, 18pF, 20ppm</t>
+  </si>
+  <si>
+    <t>48M</t>
+  </si>
+  <si>
+    <t>ABM8-48.000MHZ-B2-T</t>
+  </si>
+  <si>
+    <t>ABRACON_ABM8</t>
   </si>
 </sst>
 </file>
@@ -52807,10 +52864,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K589"/>
+  <dimension ref="A1:K590"/>
   <sheetViews>
-    <sheetView topLeftCell="A575" workbookViewId="0">
-      <selection activeCell="E590" sqref="E590"/>
+    <sheetView topLeftCell="A581" workbookViewId="0">
+      <selection activeCell="B591" sqref="B591"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72370,6 +72427,42 @@
       </c>
       <c r="K589" s="8">
         <v>0.41</v>
+      </c>
+    </row>
+    <row r="590" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A590" t="s">
+        <v>7030</v>
+      </c>
+      <c r="B590" t="str">
+        <f>CONCATENATE("CAP",", ",C590,", ",D590,", ",E590,", ",F590,", 7000hrs @ 105°C, SMD")</f>
+        <v>CAP, 220uF, ±20%, 35V, Al, 7000hrs @ 105°C, SMD</v>
+      </c>
+      <c r="C590" t="s">
+        <v>1823</v>
+      </c>
+      <c r="D590" t="s">
+        <v>4327</v>
+      </c>
+      <c r="E590" t="s">
+        <v>948</v>
+      </c>
+      <c r="F590" t="s">
+        <v>1842</v>
+      </c>
+      <c r="G590" t="s">
+        <v>1555</v>
+      </c>
+      <c r="H590" t="s">
+        <v>7032</v>
+      </c>
+      <c r="I590" t="s">
+        <v>7031</v>
+      </c>
+      <c r="J590" t="s">
+        <v>2079</v>
+      </c>
+      <c r="K590" s="8">
+        <v>0.71</v>
       </c>
     </row>
   </sheetData>
@@ -77263,7 +77356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -78045,10 +78138,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -78359,6 +78452,44 @@
         <v>0.86</v>
       </c>
     </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7040</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7041</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7042</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E9">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4749</v>
+      </c>
+      <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2917</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7043</v>
+      </c>
+      <c r="J9" t="s">
+        <v>7044</v>
+      </c>
+      <c r="K9" t="s">
+        <v>5774</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0.65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -78367,10 +78498,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -80728,6 +80859,44 @@
       </c>
       <c r="M66" s="8">
         <v>2.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>7033</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7039</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7034</v>
+      </c>
+      <c r="D67" t="s">
+        <v>7035</v>
+      </c>
+      <c r="E67" t="s">
+        <v>2119</v>
+      </c>
+      <c r="G67" t="s">
+        <v>2560</v>
+      </c>
+      <c r="H67" t="s">
+        <v>73</v>
+      </c>
+      <c r="I67" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J67" t="s">
+        <v>7036</v>
+      </c>
+      <c r="K67" t="s">
+        <v>7037</v>
+      </c>
+      <c r="L67" t="s">
+        <v>7038</v>
+      </c>
+      <c r="M67" s="8">
+        <v>3.71</v>
       </c>
     </row>
   </sheetData>
@@ -82636,10 +82805,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -83625,6 +83794,29 @@
         <v>0.4</v>
       </c>
     </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>7026</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7029</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7028</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2521</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7027</v>
+      </c>
+      <c r="G46" s="8">
+        <v>0.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add many parts, Integrated Libraries update
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17121" uniqueCount="7045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17306" uniqueCount="7144">
   <si>
     <t>Part Number</t>
   </si>
@@ -21166,6 +21166,303 @@
   </si>
   <si>
     <t>ABRACON_ABM8</t>
+  </si>
+  <si>
+    <t>DIO-00085</t>
+  </si>
+  <si>
+    <t>LED, WHITE 4000K JR5050 6V (5W)</t>
+  </si>
+  <si>
+    <t>5.77V</t>
+  </si>
+  <si>
+    <t>Cree Inc.</t>
+  </si>
+  <si>
+    <t>JR5050AWT-P-B40EB0000-N0000001</t>
+  </si>
+  <si>
+    <t>CREE-JR5050</t>
+  </si>
+  <si>
+    <t>RES-00728</t>
+  </si>
+  <si>
+    <t>CRCW12061R00FKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 1 OHM 1% 1/4W 1206 100ppm/°C</t>
+  </si>
+  <si>
+    <t>RES-00729</t>
+  </si>
+  <si>
+    <t>RES SMD 2.1 OHM 1% 1/4W 1206 100ppm/°C</t>
+  </si>
+  <si>
+    <t>CRCW12062R10FKEA</t>
+  </si>
+  <si>
+    <t>ANLG-00082</t>
+  </si>
+  <si>
+    <t>IC, VGA, Single-Ended, Linear-in-dB, DC to 100MHz</t>
+  </si>
+  <si>
+    <t>AD8337BCPZ</t>
+  </si>
+  <si>
+    <t>LFCSP-8</t>
+  </si>
+  <si>
+    <t>AD8337</t>
+  </si>
+  <si>
+    <t>MOLEX_0733910070</t>
+  </si>
+  <si>
+    <t>CONN-00113</t>
+  </si>
+  <si>
+    <t>SMA Female Receptacle, 50 Ohm, 18GHz, Thru-Hole</t>
+  </si>
+  <si>
+    <t>MISC-00062</t>
+  </si>
+  <si>
+    <t>Test Point, 1mm Drill, 2mm Pad</t>
+  </si>
+  <si>
+    <t>TP_1x2mm</t>
+  </si>
+  <si>
+    <t>TP_1</t>
+  </si>
+  <si>
+    <t>PWREG-00066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module, AC-DC Isolated, 12V 250mA Output, 85~305VAC </t>
+  </si>
+  <si>
+    <t>RAC03-12SGB</t>
+  </si>
+  <si>
+    <t>RAC03-xGB</t>
+  </si>
+  <si>
+    <t>AC-DC-module-4-pin</t>
+  </si>
+  <si>
+    <t>PWREG-00067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module, AC-DC Isolated, 5V 600mA Output, 85~305VAC </t>
+  </si>
+  <si>
+    <t>RAC03-05SGB</t>
+  </si>
+  <si>
+    <t>DIO-00086</t>
+  </si>
+  <si>
+    <t>MRA4007T3G</t>
+  </si>
+  <si>
+    <t>1000V</t>
+  </si>
+  <si>
+    <t>Dio, Silicon, General Purpose, 1000V 1A, SMA</t>
+  </si>
+  <si>
+    <t>IFACE-00033</t>
+  </si>
+  <si>
+    <t>IC, CANbus Transceiver, Isolated, 2500 VRMS, 8-SOP</t>
+  </si>
+  <si>
+    <t>Ti</t>
+  </si>
+  <si>
+    <t>ISO1050</t>
+  </si>
+  <si>
+    <t>ISO1050DUB</t>
+  </si>
+  <si>
+    <t>SOP-8</t>
+  </si>
+  <si>
+    <t>PWREG-00068</t>
+  </si>
+  <si>
+    <t>Module, DC-DC Isolated, 5V 1W 1kV, Recom Econoline</t>
+  </si>
+  <si>
+    <t>DC-DC-module-generic</t>
+  </si>
+  <si>
+    <t>RECOM_R1SE</t>
+  </si>
+  <si>
+    <t>R1SE-0505-R</t>
+  </si>
+  <si>
+    <t>CONN-00114</t>
+  </si>
+  <si>
+    <t>Screw Terminal, #10-32, 2-Pin, 30A</t>
+  </si>
+  <si>
+    <t>KEYSTONE_1299</t>
+  </si>
+  <si>
+    <t>LOGIC-00045</t>
+  </si>
+  <si>
+    <t>IC, D-Type Flip-Flop, Single w/ CLR Input, SOT-23-6</t>
+  </si>
+  <si>
+    <t>SN74LVC1G175DBVR</t>
+  </si>
+  <si>
+    <t>1G175</t>
+  </si>
+  <si>
+    <t>ANLG-00083</t>
+  </si>
+  <si>
+    <t>IC, Current Monitor, High/Low-Side, 8-VSSOP</t>
+  </si>
+  <si>
+    <t>INA301A3IDGKR</t>
+  </si>
+  <si>
+    <t>INA301</t>
+  </si>
+  <si>
+    <t>PWREG-00069</t>
+  </si>
+  <si>
+    <t>IC, PFC Controller, CCM 250kHz, 8-SOIC</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>UCC28180</t>
+  </si>
+  <si>
+    <t>UCC28180DR</t>
+  </si>
+  <si>
+    <t>MAG-00133</t>
+  </si>
+  <si>
+    <t>Ind, 330uH, 6.1A (11.2A sat.), 0.074 Ohm</t>
+  </si>
+  <si>
+    <t>330uH</t>
+  </si>
+  <si>
+    <t>74mOhm</t>
+  </si>
+  <si>
+    <t>BOURNS_1140-331K-RC</t>
+  </si>
+  <si>
+    <t>1140-331K-RC</t>
+  </si>
+  <si>
+    <t>RES-00730</t>
+  </si>
+  <si>
+    <t>CRCW1206330KFKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 330K OHM 1% 1/4W 1206 100ppm/°C</t>
+  </si>
+  <si>
+    <t>DIO-00087</t>
+  </si>
+  <si>
+    <t>Dio, SiC Schottky, 10A, 1.75V, 650V, DPAK</t>
+  </si>
+  <si>
+    <t>1.75V</t>
+  </si>
+  <si>
+    <t>650V</t>
+  </si>
+  <si>
+    <t>STPSC10H065B-TR</t>
+  </si>
+  <si>
+    <t>diode_sch_A3C2</t>
+  </si>
+  <si>
+    <t>DIO-00088</t>
+  </si>
+  <si>
+    <t>Dio, Schottky, 7A, 0.62V, 60V, PowerDI5</t>
+  </si>
+  <si>
+    <t>0.62V</t>
+  </si>
+  <si>
+    <t>PDS760-13</t>
+  </si>
+  <si>
+    <t>POWERDI5</t>
+  </si>
+  <si>
+    <t>SN74LVC2G07DBVR</t>
+  </si>
+  <si>
+    <t>2G07</t>
+  </si>
+  <si>
+    <t>LOGIC-00046</t>
+  </si>
+  <si>
+    <t>IC, Buffer Non-Inverting, Dual, Open-Drain Outputs, 1.65~5.5V, SOT-23-6</t>
+  </si>
+  <si>
+    <t>IFACE-00034</t>
+  </si>
+  <si>
+    <t>IC, High-Speed USB 2.0 Switch, DPDT, 10-MSOP</t>
+  </si>
+  <si>
+    <t>FSUSB42MUX</t>
+  </si>
+  <si>
+    <t>MSOP-10</t>
+  </si>
+  <si>
+    <t>MAG-00134</t>
+  </si>
+  <si>
+    <t>7.2uH</t>
+  </si>
+  <si>
+    <t>7.9A</t>
+  </si>
+  <si>
+    <t>12.8mOhm</t>
+  </si>
+  <si>
+    <t>Ind, 7.2uH, 7.9A (6A sat.), 0.0128 Ohm</t>
+  </si>
+  <si>
+    <t>WURTH_7447798720</t>
+  </si>
+  <si>
+    <t>CL31A476MPHNNNE</t>
+  </si>
+  <si>
+    <t>CAP-00589</t>
   </si>
 </sst>
 </file>
@@ -21175,7 +21472,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -21211,6 +21508,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -21229,11 +21534,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -21255,9 +21561,11 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -21538,8 +21846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J839"/>
   <sheetViews>
-    <sheetView topLeftCell="A700" workbookViewId="0">
-      <selection activeCell="K709" sqref="K709"/>
+    <sheetView topLeftCell="A709" workbookViewId="0">
+      <selection activeCell="B733" sqref="B733"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42349,16 +42657,100 @@
       </c>
     </row>
     <row r="730" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C730"/>
-      <c r="D730"/>
+      <c r="A730" t="s">
+        <v>7051</v>
+      </c>
+      <c r="B730" t="s">
+        <v>7053</v>
+      </c>
+      <c r="C730">
+        <v>1</v>
+      </c>
+      <c r="D730" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="E730" s="12" t="s">
+        <v>5250</v>
+      </c>
+      <c r="F730" t="s">
+        <v>2439</v>
+      </c>
+      <c r="G730" t="s">
+        <v>7052</v>
+      </c>
+      <c r="H730" t="s">
+        <v>1471</v>
+      </c>
+      <c r="I730" t="s">
+        <v>12</v>
+      </c>
+      <c r="J730" s="8">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="731" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C731"/>
-      <c r="D731"/>
+      <c r="A731" t="s">
+        <v>7054</v>
+      </c>
+      <c r="B731" t="s">
+        <v>7055</v>
+      </c>
+      <c r="C731">
+        <v>2.1</v>
+      </c>
+      <c r="D731" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="E731" s="12" t="s">
+        <v>5250</v>
+      </c>
+      <c r="F731" t="s">
+        <v>2439</v>
+      </c>
+      <c r="G731" t="s">
+        <v>7056</v>
+      </c>
+      <c r="H731" t="s">
+        <v>1471</v>
+      </c>
+      <c r="I731" t="s">
+        <v>12</v>
+      </c>
+      <c r="J731" s="8">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="732" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C732"/>
-      <c r="D732"/>
+      <c r="A732" t="s">
+        <v>7114</v>
+      </c>
+      <c r="B732" t="s">
+        <v>7116</v>
+      </c>
+      <c r="C732" t="s">
+        <v>786</v>
+      </c>
+      <c r="D732" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="E732" s="12" t="s">
+        <v>5250</v>
+      </c>
+      <c r="F732" t="s">
+        <v>2439</v>
+      </c>
+      <c r="G732" t="s">
+        <v>7115</v>
+      </c>
+      <c r="H732" t="s">
+        <v>1471</v>
+      </c>
+      <c r="I732" t="s">
+        <v>12</v>
+      </c>
+      <c r="J732" s="8">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="733" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C733"/>
@@ -42796,10 +43188,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42812,7 +43204,7 @@
     <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -42838,7 +43230,7 @@
         <v>5483</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2369</v>
       </c>
@@ -42858,8 +43250,9 @@
         <v>2371</v>
       </c>
       <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2463</v>
       </c>
@@ -42880,7 +43273,7 @@
       </c>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2709</v>
       </c>
@@ -42895,7 +43288,7 @@
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2901</v>
       </c>
@@ -42916,7 +43309,7 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2926</v>
       </c>
@@ -42937,7 +43330,7 @@
       </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2976</v>
       </c>
@@ -42963,7 +43356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4233</v>
       </c>
@@ -42986,7 +43379,7 @@
         <v>26.62</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4260</v>
       </c>
@@ -43007,7 +43400,7 @@
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4264</v>
       </c>
@@ -43030,7 +43423,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4474</v>
       </c>
@@ -43056,7 +43449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4554</v>
       </c>
@@ -43079,7 +43472,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4582</v>
       </c>
@@ -43102,7 +43495,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4592</v>
       </c>
@@ -43125,7 +43518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4620</v>
       </c>
@@ -43148,7 +43541,7 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4638</v>
       </c>
@@ -44202,6 +44595,23 @@
       </c>
       <c r="G63" s="8">
         <v>0.10489999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>7065</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7066</v>
+      </c>
+      <c r="E64" t="s">
+        <v>7067</v>
+      </c>
+      <c r="F64" t="s">
+        <v>7068</v>
+      </c>
+      <c r="G64" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -46163,10 +46573,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46182,7 +46592,7 @@
     <col min="9" max="9" width="13.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
@@ -49192,6 +49602,149 @@
       </c>
       <c r="M86" s="8">
         <v>0.18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>7045</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>7046</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>7047</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>2944</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>2433</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>2496</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>7048</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>7049</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>7050</v>
+      </c>
+      <c r="L87" s="2" t="s">
+        <v>2501</v>
+      </c>
+      <c r="M87" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>7077</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>7080</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>4544</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>7079</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>4853</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>2091</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>7078</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>2126</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>4855</v>
+      </c>
+      <c r="M88" s="8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>7117</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>7118</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>7119</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>7120</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>4903</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>2092</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>7121</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>2413</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>7122</v>
+      </c>
+      <c r="M89" s="8">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>7123</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>7124</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>7125</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>2120</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>4921</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>2092</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>2091</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>7126</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>7127</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>5461</v>
+      </c>
+      <c r="M90" s="8">
+        <v>1.02</v>
       </c>
     </row>
   </sheetData>
@@ -49203,10 +49756,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L114"/>
+  <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K115" sqref="K115"/>
+    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52798,7 +53351,7 @@
         <v>7017</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>7002</v>
       </c>
@@ -52827,7 +53380,7 @@
         <v>7018</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>7003</v>
       </c>
@@ -52854,6 +53407,73 @@
       </c>
       <c r="J114" t="s">
         <v>7019</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>7063</v>
+      </c>
+      <c r="B115" t="s">
+        <v>7064</v>
+      </c>
+      <c r="C115" t="s">
+        <v>6678</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="G115" t="s">
+        <v>2388</v>
+      </c>
+      <c r="H115">
+        <v>733910060</v>
+      </c>
+      <c r="I115" t="s">
+        <v>7062</v>
+      </c>
+      <c r="J115" t="s">
+        <v>4740</v>
+      </c>
+      <c r="K115" s="8">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>7092</v>
+      </c>
+      <c r="B116" t="s">
+        <v>7093</v>
+      </c>
+      <c r="C116" t="s">
+        <v>5395</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116" t="s">
+        <v>4660</v>
+      </c>
+      <c r="G116" t="s">
+        <v>5393</v>
+      </c>
+      <c r="H116">
+        <v>1299</v>
+      </c>
+      <c r="I116" t="s">
+        <v>7094</v>
+      </c>
+      <c r="J116" t="s">
+        <v>2963</v>
+      </c>
+      <c r="K116" s="8">
+        <v>0.93</v>
       </c>
     </row>
   </sheetData>
@@ -52864,10 +53484,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K590"/>
+  <dimension ref="A1:K591"/>
   <sheetViews>
-    <sheetView topLeftCell="A581" workbookViewId="0">
-      <selection activeCell="B591" sqref="B591"/>
+    <sheetView tabSelected="1" topLeftCell="A581" workbookViewId="0">
+      <selection activeCell="B592" sqref="B592"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72465,6 +73085,42 @@
         <v>0.71</v>
       </c>
     </row>
+    <row r="591" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A591" t="s">
+        <v>7143</v>
+      </c>
+      <c r="B591" t="str">
+        <f>CONCATENATE("CAP",", ",C591,", ",D591,", ",E591,", ",F591,", 1206")</f>
+        <v>CAP, 47uF, ±20%, 10V, X5R, 1206</v>
+      </c>
+      <c r="C591" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D591" t="s">
+        <v>4327</v>
+      </c>
+      <c r="E591" t="s">
+        <v>947</v>
+      </c>
+      <c r="F591" t="s">
+        <v>4326</v>
+      </c>
+      <c r="G591" t="s">
+        <v>5112</v>
+      </c>
+      <c r="H591" t="s">
+        <v>7142</v>
+      </c>
+      <c r="I591" t="s">
+        <v>1471</v>
+      </c>
+      <c r="J591" t="s">
+        <v>23</v>
+      </c>
+      <c r="K591" s="8">
+        <v>0.48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -72473,10 +73129,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N134"/>
+  <dimension ref="A1:N136"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="J137" sqref="J137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -77052,6 +77708,76 @@
       </c>
       <c r="M134" s="8">
         <v>2.4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>7108</v>
+      </c>
+      <c r="B135" t="s">
+        <v>7109</v>
+      </c>
+      <c r="C135" t="s">
+        <v>7110</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="E135" t="s">
+        <v>5663</v>
+      </c>
+      <c r="H135" t="s">
+        <v>7111</v>
+      </c>
+      <c r="I135" t="s">
+        <v>4889</v>
+      </c>
+      <c r="J135" t="s">
+        <v>7113</v>
+      </c>
+      <c r="K135" t="s">
+        <v>7112</v>
+      </c>
+      <c r="L135" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M135" s="8">
+        <v>10.039999999999999</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>7136</v>
+      </c>
+      <c r="B136" t="s">
+        <v>7140</v>
+      </c>
+      <c r="C136" t="s">
+        <v>7137</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>5833</v>
+      </c>
+      <c r="E136" t="s">
+        <v>7138</v>
+      </c>
+      <c r="H136" t="s">
+        <v>7139</v>
+      </c>
+      <c r="I136" t="s">
+        <v>2420</v>
+      </c>
+      <c r="J136">
+        <v>7447798720</v>
+      </c>
+      <c r="K136" t="s">
+        <v>7141</v>
+      </c>
+      <c r="L136" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M136" s="8">
+        <v>3.34</v>
       </c>
     </row>
   </sheetData>
@@ -77354,10 +78080,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -78130,6 +78856,52 @@
         <v>14.03</v>
       </c>
     </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>7081</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7082</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7083</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7085</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7086</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7084</v>
+      </c>
+      <c r="G35" s="8">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>7132</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7133</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2091</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7134</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7135</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7134</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0.64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -78140,8 +78912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -78498,10 +79270,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -80899,6 +81671,149 @@
         <v>3.71</v>
       </c>
     </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>7069</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7070</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5719</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2170</v>
+      </c>
+      <c r="E68" t="s">
+        <v>1238</v>
+      </c>
+      <c r="G68" t="s">
+        <v>5071</v>
+      </c>
+      <c r="H68" t="s">
+        <v>2519</v>
+      </c>
+      <c r="I68" t="s">
+        <v>6519</v>
+      </c>
+      <c r="J68" t="s">
+        <v>7071</v>
+      </c>
+      <c r="K68" t="s">
+        <v>7072</v>
+      </c>
+      <c r="L68" t="s">
+        <v>7073</v>
+      </c>
+      <c r="M68" s="8">
+        <v>8.66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>7074</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7075</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5719</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2944</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G69" t="s">
+        <v>5071</v>
+      </c>
+      <c r="H69" t="s">
+        <v>2519</v>
+      </c>
+      <c r="I69" t="s">
+        <v>6519</v>
+      </c>
+      <c r="J69" t="s">
+        <v>7076</v>
+      </c>
+      <c r="K69" t="s">
+        <v>7072</v>
+      </c>
+      <c r="L69" t="s">
+        <v>7073</v>
+      </c>
+      <c r="M69" s="8">
+        <v>8.66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>7087</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7088</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6518</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2944</v>
+      </c>
+      <c r="E70" t="s">
+        <v>2953</v>
+      </c>
+      <c r="G70" t="s">
+        <v>5071</v>
+      </c>
+      <c r="H70" t="s">
+        <v>2519</v>
+      </c>
+      <c r="I70" t="s">
+        <v>6519</v>
+      </c>
+      <c r="J70" t="s">
+        <v>7091</v>
+      </c>
+      <c r="K70" t="s">
+        <v>7090</v>
+      </c>
+      <c r="L70" t="s">
+        <v>7089</v>
+      </c>
+      <c r="M70" s="8">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>7103</v>
+      </c>
+      <c r="B71" t="s">
+        <v>7104</v>
+      </c>
+      <c r="G71" t="s">
+        <v>7105</v>
+      </c>
+      <c r="H71" t="s">
+        <v>73</v>
+      </c>
+      <c r="I71" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J71" t="s">
+        <v>7107</v>
+      </c>
+      <c r="K71" t="s">
+        <v>4469</v>
+      </c>
+      <c r="L71" t="s">
+        <v>7106</v>
+      </c>
+      <c r="M71" s="8">
+        <v>1.39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -80907,10 +81822,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -82797,6 +83712,52 @@
         <v>2.92</v>
       </c>
     </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>7057</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7058</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4313</v>
+      </c>
+      <c r="D84" t="s">
+        <v>7059</v>
+      </c>
+      <c r="E84" t="s">
+        <v>7060</v>
+      </c>
+      <c r="F84" t="s">
+        <v>7061</v>
+      </c>
+      <c r="G84" s="8">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>7099</v>
+      </c>
+      <c r="B85" t="s">
+        <v>7100</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D85" t="s">
+        <v>7101</v>
+      </c>
+      <c r="E85" t="s">
+        <v>4485</v>
+      </c>
+      <c r="F85" t="s">
+        <v>7102</v>
+      </c>
+      <c r="G85" s="8">
+        <v>2.95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -82805,10 +83766,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -83817,6 +84778,52 @@
         <v>0.3</v>
       </c>
     </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>7095</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7096</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7097</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2558</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7098</v>
+      </c>
+      <c r="G47" s="8">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>7130</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7131</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7128</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2558</v>
+      </c>
+      <c r="F48" t="s">
+        <v>7129</v>
+      </c>
+      <c r="G48" s="8">
+        <v>0.43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add vertical gigabit ethernet mag-jack, and a few small updates
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17306" uniqueCount="7144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17323" uniqueCount="7152">
   <si>
     <t>Part Number</t>
   </si>
@@ -21463,6 +21463,30 @@
   </si>
   <si>
     <t>CAP-00589</t>
+  </si>
+  <si>
+    <t>PWREG-00070</t>
+  </si>
+  <si>
+    <t>TPS2066CDR</t>
+  </si>
+  <si>
+    <t>IC, Power Switch 1:2 N-Channel 1A, 8-SOIC, TPS2066</t>
+  </si>
+  <si>
+    <t>CONN-00115</t>
+  </si>
+  <si>
+    <t>RJ45 Modular Mag-jack, 8P8C, 1000 Base-T, Vertical</t>
+  </si>
+  <si>
+    <t>pulse-JXD2-0015NL</t>
+  </si>
+  <si>
+    <t>JXD2-0015NL</t>
+  </si>
+  <si>
+    <t>PULSE_JXD2-0015NL</t>
   </si>
 </sst>
 </file>
@@ -49756,10 +49780,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L116"/>
+  <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K118" sqref="K118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53476,6 +53500,38 @@
         <v>0.93</v>
       </c>
     </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>7147</v>
+      </c>
+      <c r="B117" t="s">
+        <v>7148</v>
+      </c>
+      <c r="C117" t="s">
+        <v>5800</v>
+      </c>
+      <c r="D117">
+        <v>8</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="G117" t="s">
+        <v>6448</v>
+      </c>
+      <c r="H117" t="s">
+        <v>7150</v>
+      </c>
+      <c r="I117" t="s">
+        <v>7151</v>
+      </c>
+      <c r="J117" t="s">
+        <v>7149</v>
+      </c>
+      <c r="K117" s="8">
+        <v>7.63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -53486,7 +53542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K591"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A581" workbookViewId="0">
+    <sheetView topLeftCell="A581" workbookViewId="0">
       <selection activeCell="B592" sqref="B592"/>
     </sheetView>
   </sheetViews>
@@ -79270,10 +79326,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N71"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -81812,6 +81868,41 @@
       </c>
       <c r="M71" s="8">
         <v>1.39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>7144</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7146</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6469</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6469</v>
+      </c>
+      <c r="E72" t="s">
+        <v>70</v>
+      </c>
+      <c r="G72" t="s">
+        <v>6470</v>
+      </c>
+      <c r="I72" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J72" t="s">
+        <v>7145</v>
+      </c>
+      <c r="K72" t="s">
+        <v>4469</v>
+      </c>
+      <c r="L72" t="s">
+        <v>6473</v>
+      </c>
+      <c r="M72" s="8">
+        <v>1.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various parts for ROV
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17340" uniqueCount="7164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17377" uniqueCount="7187">
   <si>
     <t>Part Number</t>
   </si>
@@ -21523,6 +21523,75 @@
   </si>
   <si>
     <t>WSON_8</t>
+  </si>
+  <si>
+    <t>PWREG-00072</t>
+  </si>
+  <si>
+    <t>IC, Power On Reset (POR) Voltage Monitor, 0.9V</t>
+  </si>
+  <si>
+    <t>TPS3106E09DBVR</t>
+  </si>
+  <si>
+    <t>TPS3106</t>
+  </si>
+  <si>
+    <t>POR</t>
+  </si>
+  <si>
+    <t>0.9 ~ 3.6V</t>
+  </si>
+  <si>
+    <t>CONN-00116</t>
+  </si>
+  <si>
+    <t>JST XH 4-Pos, 2.5mm Pitch, THT</t>
+  </si>
+  <si>
+    <t>JST_XH_4_0</t>
+  </si>
+  <si>
+    <t>Distributor Link</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B4B-XH-A-LF-SN/1651047</t>
+  </si>
+  <si>
+    <t>B4B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>DIO-00089</t>
+  </si>
+  <si>
+    <t>Dio, Schottky, 0.5A, 0.385V, 20V, SOD-123</t>
+  </si>
+  <si>
+    <t>0.385V</t>
+  </si>
+  <si>
+    <t>MBR0520LT1G</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-semiconductor/MBR0520LT1G/918574</t>
+  </si>
+  <si>
+    <t>CONN-00117</t>
+  </si>
+  <si>
+    <t>Header, 14x1, 0.1"</t>
+  </si>
+  <si>
+    <t>TSW-114-07-L-S</t>
+  </si>
+  <si>
+    <t>HDDR_14x1_0</t>
+  </si>
+  <si>
+    <t>conn-14x1_0</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/TSW-114-07-L-S/1101413</t>
   </si>
 </sst>
 </file>
@@ -46633,10 +46702,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView topLeftCell="C79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N92" sqref="N92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46656,7 +46725,7 @@
     <col min="13" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -46696,8 +46765,11 @@
       <c r="M1" s="2" t="s">
         <v>4494</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" s="2" t="s">
+        <v>7173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2095</v>
       </c>
@@ -46730,7 +46802,7 @@
       </c>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2103</v>
       </c>
@@ -46763,7 +46835,7 @@
       </c>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2109</v>
       </c>
@@ -46796,7 +46868,7 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2113</v>
       </c>
@@ -46829,7 +46901,7 @@
       </c>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2116</v>
       </c>
@@ -46862,7 +46934,7 @@
       </c>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2123</v>
       </c>
@@ -46895,7 +46967,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2134</v>
       </c>
@@ -46931,7 +47003,7 @@
       </c>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2184</v>
       </c>
@@ -46967,7 +47039,7 @@
       </c>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2185</v>
       </c>
@@ -47003,7 +47075,7 @@
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>2186</v>
       </c>
@@ -47039,7 +47111,7 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2187</v>
       </c>
@@ -47075,7 +47147,7 @@
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2188</v>
       </c>
@@ -47111,7 +47183,7 @@
       </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2189</v>
       </c>
@@ -47147,7 +47219,7 @@
       </c>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>2190</v>
       </c>
@@ -47183,7 +47255,7 @@
       </c>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>2191</v>
       </c>
@@ -49451,7 +49523,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>6825</v>
       </c>
@@ -49486,7 +49558,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>6868</v>
       </c>
@@ -49515,7 +49587,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>6930</v>
       </c>
@@ -49550,7 +49622,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>6937</v>
       </c>
@@ -49591,7 +49663,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>6952</v>
       </c>
@@ -49629,7 +49701,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>6968</v>
       </c>
@@ -49664,7 +49736,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>7045</v>
       </c>
@@ -49702,7 +49774,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>7077</v>
       </c>
@@ -49737,7 +49809,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>7117</v>
       </c>
@@ -49772,7 +49844,7 @@
         <v>3.31</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>7123</v>
       </c>
@@ -49805,6 +49877,44 @@
       </c>
       <c r="M90" s="8">
         <v>1.02</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>7176</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>7177</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>7178</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>2175</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>2092</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>2091</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>7179</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>2104</v>
+      </c>
+      <c r="L91" s="2" t="s">
+        <v>2097</v>
+      </c>
+      <c r="M91" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="N91" s="2" t="s">
+        <v>7180</v>
       </c>
     </row>
   </sheetData>
@@ -49816,10 +49926,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L117"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K118" sqref="K118"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H121" sqref="H121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49835,7 +49945,7 @@
     <col min="10" max="10" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -49872,8 +49982,11 @@
       <c r="L1" t="s">
         <v>5483</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>7173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2379</v>
       </c>
@@ -49908,7 +50021,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2385</v>
       </c>
@@ -49946,7 +50059,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2395</v>
       </c>
@@ -49981,7 +50094,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2442</v>
       </c>
@@ -50002,7 +50115,7 @@
       </c>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2447</v>
       </c>
@@ -50023,7 +50136,7 @@
       </c>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2448</v>
       </c>
@@ -50044,7 +50157,7 @@
       </c>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2469</v>
       </c>
@@ -50077,7 +50190,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2508</v>
       </c>
@@ -50101,7 +50214,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2575</v>
       </c>
@@ -50122,7 +50235,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2887</v>
       </c>
@@ -50155,7 +50268,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2888</v>
       </c>
@@ -50188,7 +50301,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2905</v>
       </c>
@@ -50221,7 +50334,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2959</v>
       </c>
@@ -50245,7 +50358,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2960</v>
       </c>
@@ -50269,7 +50382,7 @@
       </c>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2975</v>
       </c>
@@ -53411,7 +53524,7 @@
         <v>7017</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>7002</v>
       </c>
@@ -53440,7 +53553,7 @@
         <v>7018</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>7003</v>
       </c>
@@ -53469,7 +53582,7 @@
         <v>7019</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>7063</v>
       </c>
@@ -53501,7 +53614,7 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>7092</v>
       </c>
@@ -53536,7 +53649,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>7146</v>
       </c>
@@ -53566,6 +53679,79 @@
       </c>
       <c r="K117" s="8">
         <v>7.63</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>7170</v>
+      </c>
+      <c r="B118" t="s">
+        <v>7171</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2510</v>
+      </c>
+      <c r="D118">
+        <v>4</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>3</v>
+      </c>
+      <c r="G118" t="s">
+        <v>2471</v>
+      </c>
+      <c r="H118" t="s">
+        <v>7175</v>
+      </c>
+      <c r="I118" t="s">
+        <v>7172</v>
+      </c>
+      <c r="J118" t="s">
+        <v>2956</v>
+      </c>
+      <c r="K118" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="M118" t="s">
+        <v>7174</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>7181</v>
+      </c>
+      <c r="B119" t="s">
+        <v>7182</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D119">
+        <v>14</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="G119" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H119" t="s">
+        <v>7183</v>
+      </c>
+      <c r="I119" t="s">
+        <v>7184</v>
+      </c>
+      <c r="J119" t="s">
+        <v>7185</v>
+      </c>
+      <c r="K119" s="8">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="M119" t="s">
+        <v>7186</v>
       </c>
     </row>
   </sheetData>
@@ -79385,10 +79571,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -82000,6 +82186,35 @@
       </c>
       <c r="M73" s="8">
         <v>0.98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>7164</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7165</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7169</v>
+      </c>
+      <c r="G74" t="s">
+        <v>7168</v>
+      </c>
+      <c r="I74" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J74" t="s">
+        <v>7166</v>
+      </c>
+      <c r="K74" t="s">
+        <v>2558</v>
+      </c>
+      <c r="L74" t="s">
+        <v>7167</v>
+      </c>
+      <c r="M74" s="8">
+        <v>2.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Hirose connector for ROV
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17377" uniqueCount="7187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17386" uniqueCount="7191">
   <si>
     <t>Part Number</t>
   </si>
@@ -21592,6 +21592,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/samtec-inc/TSW-114-07-L-S/1101413</t>
+  </si>
+  <si>
+    <t>CONN-00118</t>
+  </si>
+  <si>
+    <t>HIROSE_DF13-4P-1-25DSA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/DF13-4P-1.25DSA/H2193-ND/241767</t>
+  </si>
+  <si>
+    <t>Header, 4-Pos, Shrouded, 1.25mm Pitch, Vertical, Thru-Hole</t>
   </si>
 </sst>
 </file>
@@ -49926,10 +49938,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M119"/>
+  <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H121" sqref="H121"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53752,6 +53764,44 @@
       </c>
       <c r="M119" t="s">
         <v>7186</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>7187</v>
+      </c>
+      <c r="B120" t="s">
+        <v>7190</v>
+      </c>
+      <c r="C120" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D120">
+        <v>4</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120" t="s">
+        <v>70</v>
+      </c>
+      <c r="G120" t="s">
+        <v>5994</v>
+      </c>
+      <c r="H120" t="s">
+        <v>5993</v>
+      </c>
+      <c r="I120" t="s">
+        <v>7188</v>
+      </c>
+      <c r="J120" t="s">
+        <v>2956</v>
+      </c>
+      <c r="K120" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="M120" t="s">
+        <v>7189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add PCA9685 plus a 10uF ceramic cap
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17386" uniqueCount="7191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17405" uniqueCount="7200">
   <si>
     <t>Part Number</t>
   </si>
@@ -21604,6 +21604,33 @@
   </si>
   <si>
     <t>Header, 4-Pos, Shrouded, 1.25mm Pitch, Vertical, Thru-Hole</t>
+  </si>
+  <si>
+    <t>MISC-00063</t>
+  </si>
+  <si>
+    <t>IC, 16-Channel PWM LED Controller, I2C, TSSOP28</t>
+  </si>
+  <si>
+    <t>TSSOP-28_1</t>
+  </si>
+  <si>
+    <t>PCA9685PW,112</t>
+  </si>
+  <si>
+    <t>PCA9685</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nxp-usa-inc/PCA9685PW112/2034324</t>
+  </si>
+  <si>
+    <t>CAP-00590</t>
+  </si>
+  <si>
+    <t>CGA6P1X7R1N106K250AC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tdk-corporation/CGA6P1X7R1N106K250AC/10240635</t>
   </si>
 </sst>
 </file>
@@ -43329,10 +43356,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43370,6 +43397,9 @@
       <c r="H1" t="s">
         <v>5483</v>
       </c>
+      <c r="I1" t="s">
+        <v>7173</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -44753,6 +44783,32 @@
       </c>
       <c r="G64" s="8">
         <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>7191</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7192</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2331</v>
+      </c>
+      <c r="D65" t="s">
+        <v>7194</v>
+      </c>
+      <c r="E65" t="s">
+        <v>7193</v>
+      </c>
+      <c r="F65" t="s">
+        <v>7195</v>
+      </c>
+      <c r="G65" s="8">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="I65" t="s">
+        <v>7196</v>
       </c>
     </row>
   </sheetData>
@@ -49940,7 +49996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
@@ -53812,10 +53868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K591"/>
+  <dimension ref="A1:L592"/>
   <sheetViews>
-    <sheetView topLeftCell="A581" workbookViewId="0">
-      <selection activeCell="B592" sqref="B592"/>
+    <sheetView tabSelected="1" topLeftCell="A577" workbookViewId="0">
+      <selection activeCell="B593" sqref="B593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53833,7 +53889,7 @@
     <col min="11" max="11" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -53867,8 +53923,11 @@
       <c r="K1" s="8" t="s">
         <v>4494</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>7173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -53901,7 +53960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -53934,7 +53993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -53967,7 +54026,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1085</v>
       </c>
@@ -54000,7 +54059,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1086</v>
       </c>
@@ -54033,7 +54092,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1087</v>
       </c>
@@ -54066,7 +54125,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1088</v>
       </c>
@@ -54099,7 +54158,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1089</v>
       </c>
@@ -54132,7 +54191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1090</v>
       </c>
@@ -54165,7 +54224,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1091</v>
       </c>
@@ -54198,7 +54257,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1092</v>
       </c>
@@ -54231,7 +54290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1093</v>
       </c>
@@ -54264,7 +54323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1094</v>
       </c>
@@ -54297,7 +54356,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1095</v>
       </c>
@@ -54330,7 +54389,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1096</v>
       </c>
@@ -72909,7 +72968,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="577" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>6812</v>
       </c>
@@ -72945,7 +73004,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="578" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>6814</v>
       </c>
@@ -72981,7 +73040,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="579" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
         <v>6817</v>
       </c>
@@ -73017,7 +73076,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="580" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>6820</v>
       </c>
@@ -73053,7 +73112,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="581" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>6839</v>
       </c>
@@ -73089,7 +73148,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="582" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>6845</v>
       </c>
@@ -73125,7 +73184,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="583" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>6852</v>
       </c>
@@ -73161,7 +73220,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="584" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>6865</v>
       </c>
@@ -73197,7 +73256,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="585" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>6898</v>
       </c>
@@ -73233,7 +73292,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="586" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
         <v>6902</v>
       </c>
@@ -73269,7 +73328,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="587" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>6958</v>
       </c>
@@ -73305,7 +73364,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="588" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
         <v>6969</v>
       </c>
@@ -73341,7 +73400,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="589" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>7020</v>
       </c>
@@ -73377,7 +73436,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="590" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
         <v>7030</v>
       </c>
@@ -73413,7 +73472,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="591" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
         <v>7143</v>
       </c>
@@ -73447,6 +73506,45 @@
       </c>
       <c r="K591" s="8">
         <v>0.48</v>
+      </c>
+    </row>
+    <row r="592" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A592" t="s">
+        <v>7197</v>
+      </c>
+      <c r="B592" t="str">
+        <f>CONCATENATE("CAP",", ",C592,", ",D592,", ",E592,", ",F592,", 1210")</f>
+        <v>CAP, 10uF, ±10%, 75V, X7R, 1210</v>
+      </c>
+      <c r="C592" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D592" t="s">
+        <v>4344</v>
+      </c>
+      <c r="E592" t="s">
+        <v>4852</v>
+      </c>
+      <c r="F592" t="s">
+        <v>20</v>
+      </c>
+      <c r="G592" t="s">
+        <v>1381</v>
+      </c>
+      <c r="H592" t="s">
+        <v>7198</v>
+      </c>
+      <c r="I592" t="s">
+        <v>4325</v>
+      </c>
+      <c r="J592" t="s">
+        <v>23</v>
+      </c>
+      <c r="K592" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="L592" t="s">
+        <v>7199</v>
       </c>
     </row>
   </sheetData>
@@ -78410,7 +78508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -84221,7 +84319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
A few connectors and a ferrite bead
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17405" uniqueCount="7200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17424" uniqueCount="7211">
   <si>
     <t>Part Number</t>
   </si>
@@ -21631,6 +21631,39 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/tdk-corporation/CGA6P1X7R1N106K250AC/10240635</t>
+  </si>
+  <si>
+    <t>BLM18KG221SN1D</t>
+  </si>
+  <si>
+    <t>50mOhm</t>
+  </si>
+  <si>
+    <t>Fe Bead, 220 @ 100MHz, 2.2A, 0603</t>
+  </si>
+  <si>
+    <t>MAG-00135</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/BLM18KG221SN1D/1982763</t>
+  </si>
+  <si>
+    <t>CONN-00119</t>
+  </si>
+  <si>
+    <t>Header, 8x3, 0.1", 24-Pos, Right-Angle</t>
+  </si>
+  <si>
+    <t>conn-8x3_0</t>
+  </si>
+  <si>
+    <t>HDDR_8x3_RA</t>
+  </si>
+  <si>
+    <t>TSW-108-08-L-T-RA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/TSW-108-08-L-T-RA/7869092</t>
   </si>
 </sst>
 </file>
@@ -49994,10 +50027,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M120"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53860,6 +53893,41 @@
         <v>7189</v>
       </c>
     </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>7205</v>
+      </c>
+      <c r="B121" t="s">
+        <v>7206</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D121">
+        <v>8</v>
+      </c>
+      <c r="E121">
+        <v>3</v>
+      </c>
+      <c r="G121" t="s">
+        <v>4737</v>
+      </c>
+      <c r="H121" t="s">
+        <v>7209</v>
+      </c>
+      <c r="I121" t="s">
+        <v>7208</v>
+      </c>
+      <c r="J121" t="s">
+        <v>7207</v>
+      </c>
+      <c r="K121" s="8">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="M121" t="s">
+        <v>7210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -53870,7 +53938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L592"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A577" workbookViewId="0">
+    <sheetView topLeftCell="A577" workbookViewId="0">
       <selection activeCell="B593" sqref="B593"/>
     </sheetView>
   </sheetViews>
@@ -73555,10 +73623,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N136"/>
+  <dimension ref="A1:O137"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="J137" sqref="J137"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -73577,7 +73645,7 @@
     <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -73620,8 +73688,11 @@
       <c r="N1" t="s">
         <v>5483</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>7173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -73650,7 +73721,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1383</v>
       </c>
@@ -73684,7 +73755,7 @@
       </c>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1384</v>
       </c>
@@ -73718,7 +73789,7 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1385</v>
       </c>
@@ -73752,7 +73823,7 @@
       </c>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1386</v>
       </c>
@@ -73786,7 +73857,7 @@
       </c>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1387</v>
       </c>
@@ -73820,7 +73891,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1388</v>
       </c>
@@ -73854,7 +73925,7 @@
       </c>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1389</v>
       </c>
@@ -73888,7 +73959,7 @@
       </c>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1390</v>
       </c>
@@ -73922,7 +73993,7 @@
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1391</v>
       </c>
@@ -73956,7 +74027,7 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1392</v>
       </c>
@@ -73990,7 +74061,7 @@
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1393</v>
       </c>
@@ -74024,7 +74095,7 @@
       </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1394</v>
       </c>
@@ -74058,7 +74129,7 @@
       </c>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1395</v>
       </c>
@@ -74092,7 +74163,7 @@
       </c>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1396</v>
       </c>
@@ -77932,7 +78003,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>6635</v>
       </c>
@@ -77967,7 +78038,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>6640</v>
       </c>
@@ -78002,7 +78073,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>6734</v>
       </c>
@@ -78037,7 +78108,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>6764</v>
       </c>
@@ -78072,7 +78143,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>6773</v>
       </c>
@@ -78104,7 +78175,7 @@
         <v>4.18</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>6939</v>
       </c>
@@ -78136,7 +78207,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>7108</v>
       </c>
@@ -78171,7 +78242,7 @@
         <v>10.039999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>7136</v>
       </c>
@@ -78204,6 +78275,44 @@
       </c>
       <c r="M136" s="8">
         <v>3.34</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>7203</v>
+      </c>
+      <c r="B137" t="s">
+        <v>7202</v>
+      </c>
+      <c r="E137" t="s">
+        <v>2264</v>
+      </c>
+      <c r="F137">
+        <v>220</v>
+      </c>
+      <c r="G137" t="s">
+        <v>37</v>
+      </c>
+      <c r="H137" t="s">
+        <v>7201</v>
+      </c>
+      <c r="I137" t="s">
+        <v>21</v>
+      </c>
+      <c r="J137" t="s">
+        <v>7200</v>
+      </c>
+      <c r="K137" t="s">
+        <v>6633</v>
+      </c>
+      <c r="L137" t="s">
+        <v>36</v>
+      </c>
+      <c r="M137" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="O137" t="s">
+        <v>7204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various additions, add links for some parts too
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21935" uniqueCount="8869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22026" uniqueCount="8922">
   <si>
     <t>Part Number</t>
   </si>
@@ -26638,6 +26638,165 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/vishay-dale/CRCW060333K2FKEA/1174840</t>
+  </si>
+  <si>
+    <t>MAG-00136</t>
+  </si>
+  <si>
+    <t>SRP1265A-330M</t>
+  </si>
+  <si>
+    <t>58mOhm</t>
+  </si>
+  <si>
+    <t>Ind, 33uH, 8A (11A sat.), 0.058 Ohm, Bourns SRP1265A</t>
+  </si>
+  <si>
+    <t>DIO-00090</t>
+  </si>
+  <si>
+    <t>TVS, 28V, 45.5V@66A, 3kW 66A Peak, Bidirectional, DO-214AC</t>
+  </si>
+  <si>
+    <t>SMC30J28CA</t>
+  </si>
+  <si>
+    <t>66A</t>
+  </si>
+  <si>
+    <t>3000W</t>
+  </si>
+  <si>
+    <t>31.1V</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/SMC30J28CA/2826980</t>
+  </si>
+  <si>
+    <t>CAP-00591</t>
+  </si>
+  <si>
+    <t>CP_RADIAL_D10.0_P5.0_H20.0</t>
+  </si>
+  <si>
+    <t>UPW1J221MPD</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nichicon/UPW1J221MPD/589683</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/mpd-memory-protection-devices/BU2032SM-JJ-GTR/1596664</t>
+  </si>
+  <si>
+    <t>CAP-00592</t>
+  </si>
+  <si>
+    <t>CL10B104KB8NNNL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10B104KB8NNNL/3894274</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL31B106KAHNNNE/3887462</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/GRM21BR71C105KA01K/2546959</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/taiyo-yuden/LMK325B7476MM-TR/2573870</t>
+  </si>
+  <si>
+    <t>LMK325B7476MM-TR</t>
+  </si>
+  <si>
+    <t>CAP-00593</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-general-semiconductor-diodes-division/SS5P6-M3-86A/2048208</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/DLPT05-7-F/808520</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-semiconductor/MBR140SFT1G/918583</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kingbright/APT1608LVBC-D/5177434</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/eaton-electronics-division/PTS12066V050/2639136</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/littelfuse-inc/1210L150-16WR/3997172</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-amp-connectors/1-1393644-6/2268175</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-amp-connectors/3-1827253-6/2188003</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/pulse-electronics-network/J0G-0003NL/2264761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cnc-tech/1003-004-01010/3466939</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/UJ2-ADH-1-TH/6187916</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/10029449-111RLF/2785386</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/1040310811/2370379</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-commercial-products/RJMG1BD3B8K1ANR/5359794</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-amp-connectors/1932638-3/4731612</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/IHLP3232DZER100M01/2657466</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/LQM21PN1R0MGHL/4864857</t>
+  </si>
+  <si>
+    <t>LQM21PN1R0MGHL</t>
+  </si>
+  <si>
+    <t>1.7A</t>
+  </si>
+  <si>
+    <t>MAG-00137</t>
+  </si>
+  <si>
+    <t>Ind, 1uH, 1.7A (1.1A sat.), 0.1 Ohm, 0805</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/SRN5040-3R3M/4867711</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/pulse-electronics-network/PE-0805PFB600ST/5050552</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74LVC2G04DBVT/1592245</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/TPD4E02B04DQAR/5880125</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74LVC1G126DBVR/385722</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74LVC1G11DBVR/637182</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/USBLC6-2SC6Y/2819177</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/TPS2066DGNR/684822</t>
   </si>
 </sst>
 </file>
@@ -27021,7 +27180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1204" workbookViewId="0">
+    <sheetView topLeftCell="A1204" workbookViewId="0">
       <selection activeCell="K1234" sqref="K1234"/>
     </sheetView>
   </sheetViews>
@@ -63975,8 +64134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -64210,6 +64369,9 @@
       <c r="G10" s="8">
         <v>0.3</v>
       </c>
+      <c r="I10" t="s">
+        <v>8897</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -65040,7 +65202,7 @@
         <v>12.23</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6223</v>
       </c>
@@ -65063,7 +65225,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>6233</v>
       </c>
@@ -65086,7 +65248,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>6258</v>
       </c>
@@ -65109,7 +65271,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>6289</v>
       </c>
@@ -65132,7 +65294,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6324</v>
       </c>
@@ -65155,7 +65317,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6340</v>
       </c>
@@ -65178,7 +65340,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>6378</v>
       </c>
@@ -65201,7 +65363,7 @@
         <v>13.68</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>6492</v>
       </c>
@@ -65224,7 +65386,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6585</v>
       </c>
@@ -65247,7 +65409,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>6621</v>
       </c>
@@ -65269,8 +65431,11 @@
       <c r="G58" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I58" t="s">
+        <v>8898</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>6702</v>
       </c>
@@ -65293,7 +65458,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>6782</v>
       </c>
@@ -65316,7 +65481,7 @@
         <v>6.32</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>6855</v>
       </c>
@@ -65339,7 +65504,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>6907</v>
       </c>
@@ -65362,7 +65527,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>6977</v>
       </c>
@@ -65385,7 +65550,7 @@
         <v>0.10489999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>7065</v>
       </c>
@@ -67387,10 +67552,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView topLeftCell="C79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N92" sqref="N92"/>
+    <sheetView topLeftCell="C55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67519,6 +67684,9 @@
         <v>2097</v>
       </c>
       <c r="M3" s="8"/>
+      <c r="N3" s="2" t="s">
+        <v>8895</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -69094,7 +69262,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>5010</v>
       </c>
@@ -69132,7 +69300,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>5160</v>
       </c>
@@ -69167,7 +69335,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>5161</v>
       </c>
@@ -69204,8 +69372,11 @@
       <c r="M51" s="8">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N51" s="2" t="s">
+        <v>8896</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>5162</v>
       </c>
@@ -69243,7 +69414,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>5205</v>
       </c>
@@ -69278,7 +69449,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>5374</v>
       </c>
@@ -69316,7 +69487,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>5406</v>
       </c>
@@ -69345,7 +69516,7 @@
         <v>4855</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>5455</v>
       </c>
@@ -69380,7 +69551,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>5723</v>
       </c>
@@ -69412,7 +69583,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>5724</v>
       </c>
@@ -69447,7 +69618,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>5836</v>
       </c>
@@ -69475,8 +69646,11 @@
       <c r="M59" s="8">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N59" s="2" t="s">
+        <v>8894</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>5919</v>
       </c>
@@ -69511,7 +69685,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>5997</v>
       </c>
@@ -69546,7 +69720,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>6045</v>
       </c>
@@ -69581,7 +69755,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>6049</v>
       </c>
@@ -69616,7 +69790,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>6072</v>
       </c>
@@ -69651,7 +69825,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>6077</v>
       </c>
@@ -69689,7 +69863,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>6131</v>
       </c>
@@ -69727,7 +69901,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>6147</v>
       </c>
@@ -69765,7 +69939,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>6247</v>
       </c>
@@ -69800,7 +69974,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>6366</v>
       </c>
@@ -69835,7 +70009,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>6413</v>
       </c>
@@ -69866,8 +70040,11 @@
       <c r="M70" s="8">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N70" s="2" t="s">
+        <v>8917</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>6428</v>
       </c>
@@ -69901,8 +70078,11 @@
       <c r="M71" s="8">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N71" s="2" t="s">
+        <v>8920</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>6475</v>
       </c>
@@ -69940,7 +70120,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>6508</v>
       </c>
@@ -69975,7 +70155,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>6556</v>
       </c>
@@ -70016,7 +70196,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>6603</v>
       </c>
@@ -70051,7 +70231,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>6607</v>
       </c>
@@ -70085,8 +70265,11 @@
       <c r="M76" s="8">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N76" s="2" t="s">
+        <v>8893</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>6709</v>
       </c>
@@ -70118,7 +70301,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>6735</v>
       </c>
@@ -70153,7 +70336,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>6804</v>
       </c>
@@ -70188,7 +70371,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>6823</v>
       </c>
@@ -70600,6 +70783,44 @@
       </c>
       <c r="N91" s="2" t="s">
         <v>7180</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>8873</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>8874</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>8878</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>8877</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>8876</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>2943</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>8875</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>2115</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>2942</v>
+      </c>
+      <c r="M92" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N92" s="2" t="s">
+        <v>8879</v>
       </c>
     </row>
   </sheetData>
@@ -70613,8 +70834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72113,7 +72334,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>5490</v>
       </c>
@@ -72148,7 +72369,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>5494</v>
       </c>
@@ -72183,7 +72404,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>5509</v>
       </c>
@@ -72215,7 +72436,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>5621</v>
       </c>
@@ -72247,7 +72468,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>5625</v>
       </c>
@@ -72282,7 +72503,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>5645</v>
       </c>
@@ -72317,7 +72538,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>5707</v>
       </c>
@@ -72352,7 +72573,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>5750</v>
       </c>
@@ -72387,7 +72608,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>5761</v>
       </c>
@@ -72419,7 +72640,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>5765</v>
       </c>
@@ -72451,7 +72672,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>5799</v>
       </c>
@@ -72476,8 +72697,11 @@
       <c r="K59" s="8">
         <v>3.92</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M59" t="s">
+        <v>8906</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>5805</v>
       </c>
@@ -72511,8 +72735,11 @@
       <c r="K60" s="8">
         <v>1.52</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M60" t="s">
+        <v>8907</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>5841</v>
       </c>
@@ -72547,7 +72774,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>5845</v>
       </c>
@@ -72576,7 +72803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>5854</v>
       </c>
@@ -72611,7 +72838,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>5864</v>
       </c>
@@ -72646,7 +72873,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>5865</v>
       </c>
@@ -72669,7 +72896,7 @@
         <v>5767</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>5870</v>
       </c>
@@ -72692,7 +72919,7 @@
         <v>5767</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>5876</v>
       </c>
@@ -72724,7 +72951,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>5933</v>
       </c>
@@ -72759,7 +72986,7 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>5995</v>
       </c>
@@ -72794,7 +73021,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>6017</v>
       </c>
@@ -72828,8 +73055,11 @@
       <c r="K70" s="8">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M70" t="s">
+        <v>8903</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>6031</v>
       </c>
@@ -72864,7 +73094,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>6036</v>
       </c>
@@ -72896,7 +73126,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>6057</v>
       </c>
@@ -72928,7 +73158,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>6106</v>
       </c>
@@ -72963,7 +73193,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>6146</v>
       </c>
@@ -72998,7 +73228,7 @@
         <v>2.5099999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>6216</v>
       </c>
@@ -73033,7 +73263,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>6252</v>
       </c>
@@ -73068,7 +73298,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>6299</v>
       </c>
@@ -73103,7 +73333,7 @@
         <v>6.67</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>6306</v>
       </c>
@@ -73134,8 +73364,11 @@
       <c r="K79" s="8">
         <v>2.76</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M79" t="s">
+        <v>8884</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>6313</v>
       </c>
@@ -73166,8 +73399,11 @@
       <c r="K80" s="8">
         <v>18.989999999999998</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M80" t="s">
+        <v>8900</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>6318</v>
       </c>
@@ -73199,10 +73435,13 @@
         <v>6322</v>
       </c>
       <c r="K81" s="8">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3.95</v>
+      </c>
+      <c r="M81" t="s">
+        <v>8902</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>6332</v>
       </c>
@@ -73236,8 +73475,11 @@
       <c r="K82" s="8">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M82" t="s">
+        <v>8904</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>6437</v>
       </c>
@@ -73272,7 +73514,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>6446</v>
       </c>
@@ -73303,8 +73545,11 @@
       <c r="K84" s="8">
         <v>10.26</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M84" t="s">
+        <v>8901</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>6487</v>
       </c>
@@ -73327,7 +73572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>6533</v>
       </c>
@@ -73361,8 +73606,11 @@
       <c r="K86" s="8">
         <v>7.49</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M86" t="s">
+        <v>8899</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>6538</v>
       </c>
@@ -73397,7 +73645,7 @@
         <v>5.17</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>6581</v>
       </c>
@@ -73423,7 +73671,7 @@
         <v>3.78</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>6613</v>
       </c>
@@ -73455,7 +73703,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>6615</v>
       </c>
@@ -73481,7 +73729,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>6645</v>
       </c>
@@ -73516,7 +73764,7 @@
         <v>13.14</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>6653</v>
       </c>
@@ -73551,7 +73799,7 @@
         <v>7.35</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>6671</v>
       </c>
@@ -73582,8 +73830,11 @@
       <c r="K93" s="8">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M93" t="s">
+        <v>8905</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>6676</v>
       </c>
@@ -73618,7 +73869,7 @@
         <v>11.45</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>6687</v>
       </c>
@@ -73653,7 +73904,7 @@
         <v>11.68</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>6717</v>
       </c>
@@ -74520,10 +74771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L592"/>
+  <dimension ref="A1:L595"/>
   <sheetViews>
-    <sheetView topLeftCell="A577" workbookViewId="0">
-      <selection activeCell="B593" sqref="B593"/>
+    <sheetView topLeftCell="A576" workbookViewId="0">
+      <selection activeCell="B596" sqref="B596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -77714,7 +77965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>1177</v>
       </c>
@@ -77747,7 +77998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>1178</v>
       </c>
@@ -77780,7 +78031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>1179</v>
       </c>
@@ -77813,7 +78064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>1180</v>
       </c>
@@ -77846,7 +78097,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>1181</v>
       </c>
@@ -77879,7 +78130,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>1182</v>
       </c>
@@ -77912,7 +78163,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>1183</v>
       </c>
@@ -77945,7 +78196,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>1184</v>
       </c>
@@ -77978,7 +78229,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>1185</v>
       </c>
@@ -78011,7 +78262,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>1186</v>
       </c>
@@ -78044,7 +78295,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>1187</v>
       </c>
@@ -78077,7 +78328,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>1188</v>
       </c>
@@ -78110,7 +78361,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>1189</v>
       </c>
@@ -78143,7 +78394,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>1190</v>
       </c>
@@ -78176,7 +78427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>1191</v>
       </c>
@@ -78209,7 +78460,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>1192</v>
       </c>
@@ -78241,6 +78492,9 @@
       <c r="J112" t="s">
         <v>23</v>
       </c>
+      <c r="L112" t="s">
+        <v>8889</v>
+      </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
@@ -91970,7 +92224,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="529" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
         <v>4458</v>
       </c>
@@ -92003,7 +92257,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="530" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
         <v>4459</v>
       </c>
@@ -92036,7 +92290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="531" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>4460</v>
       </c>
@@ -92069,7 +92323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="532" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>4461</v>
       </c>
@@ -92102,7 +92356,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="533" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>4462</v>
       </c>
@@ -92135,7 +92389,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="534" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
         <v>4463</v>
       </c>
@@ -92168,7 +92422,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="535" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>4464</v>
       </c>
@@ -92201,7 +92455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="536" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
         <v>4488</v>
       </c>
@@ -92237,7 +92491,7 @@
         <v>0.187</v>
       </c>
     </row>
-    <row r="537" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>4495</v>
       </c>
@@ -92273,7 +92527,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="538" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
         <v>4680</v>
       </c>
@@ -92309,7 +92563,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="539" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>4702</v>
       </c>
@@ -92336,7 +92590,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="540" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>4762</v>
       </c>
@@ -92363,7 +92617,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="541" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>4801</v>
       </c>
@@ -92395,8 +92649,11 @@
       <c r="J541" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="542" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L541" t="s">
+        <v>8888</v>
+      </c>
+    </row>
+    <row r="542" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
         <v>4803</v>
       </c>
@@ -92429,7 +92686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="543" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
         <v>4809</v>
       </c>
@@ -92462,7 +92719,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="544" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
         <v>4851</v>
       </c>
@@ -94197,6 +94454,123 @@
       </c>
       <c r="L592" t="s">
         <v>7199</v>
+      </c>
+    </row>
+    <row r="593" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A593" t="s">
+        <v>8880</v>
+      </c>
+      <c r="B593" t="str">
+        <f>CONCATENATE("CAP",", ",C593,", ",D593,", ",E593,", ",F593,", 5000hrs @ 105°C")</f>
+        <v>CAP, 220uF, ±20%, 63V, Al, 5000hrs @ 105°C</v>
+      </c>
+      <c r="C593" t="s">
+        <v>1823</v>
+      </c>
+      <c r="D593" t="s">
+        <v>4327</v>
+      </c>
+      <c r="E593" t="s">
+        <v>1841</v>
+      </c>
+      <c r="F593" t="s">
+        <v>1842</v>
+      </c>
+      <c r="G593" t="s">
+        <v>1555</v>
+      </c>
+      <c r="H593" t="s">
+        <v>8882</v>
+      </c>
+      <c r="I593" t="s">
+        <v>8881</v>
+      </c>
+      <c r="J593" t="s">
+        <v>2079</v>
+      </c>
+      <c r="K593" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="L593" t="s">
+        <v>8883</v>
+      </c>
+    </row>
+    <row r="594" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A594" t="s">
+        <v>8885</v>
+      </c>
+      <c r="B594" t="str">
+        <f>CONCATENATE("CAP",", ",C594,", ",D594,", ",E594,", ",F594,", 0603")</f>
+        <v>CAP, 0.1uF, ±10%, 50V, X7R, 0603</v>
+      </c>
+      <c r="C594" t="s">
+        <v>4663</v>
+      </c>
+      <c r="D594" t="s">
+        <v>4344</v>
+      </c>
+      <c r="E594" t="s">
+        <v>943</v>
+      </c>
+      <c r="F594" t="s">
+        <v>20</v>
+      </c>
+      <c r="G594" t="s">
+        <v>5112</v>
+      </c>
+      <c r="H594" t="s">
+        <v>8886</v>
+      </c>
+      <c r="I594" t="s">
+        <v>35</v>
+      </c>
+      <c r="J594" t="s">
+        <v>23</v>
+      </c>
+      <c r="K594" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="L594" t="s">
+        <v>8887</v>
+      </c>
+    </row>
+    <row r="595" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A595" t="s">
+        <v>8892</v>
+      </c>
+      <c r="B595" t="str">
+        <f>CONCATENATE("CAP",", ",C595,", ",D595,", ",E595,", ",F595,", 1210")</f>
+        <v>CAP, 47uF, ±20%, 10V, X7R, 1210</v>
+      </c>
+      <c r="C595" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D595" t="s">
+        <v>4327</v>
+      </c>
+      <c r="E595" t="s">
+        <v>947</v>
+      </c>
+      <c r="F595" t="s">
+        <v>20</v>
+      </c>
+      <c r="G595" t="s">
+        <v>4329</v>
+      </c>
+      <c r="H595" t="s">
+        <v>8891</v>
+      </c>
+      <c r="I595" t="s">
+        <v>4325</v>
+      </c>
+      <c r="J595" t="s">
+        <v>23</v>
+      </c>
+      <c r="K595" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="L595" t="s">
+        <v>8890</v>
       </c>
     </row>
   </sheetData>
@@ -94207,10 +94581,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O137"/>
+  <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+    <sheetView topLeftCell="C104" workbookViewId="0">
+      <selection activeCell="O125" sqref="O125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -97491,7 +97865,7 @@
         <v>8.85</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>4598</v>
       </c>
@@ -97526,7 +97900,7 @@
         <v>6.08</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>4657</v>
       </c>
@@ -97561,7 +97935,7 @@
         <v>9.5299999999999994</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>4665</v>
       </c>
@@ -97596,7 +97970,7 @@
         <v>9.5299999999999994</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>4682</v>
       </c>
@@ -97631,7 +98005,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>4887</v>
       </c>
@@ -97666,7 +98040,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>4897</v>
       </c>
@@ -97698,7 +98072,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>4917</v>
       </c>
@@ -97733,7 +98107,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>5027</v>
       </c>
@@ -97771,7 +98145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>5367</v>
       </c>
@@ -97800,7 +98174,7 @@
         <v>4.62</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>5385</v>
       </c>
@@ -97832,7 +98206,7 @@
         <v>1.97</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>5412</v>
       </c>
@@ -97858,7 +98232,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>5564</v>
       </c>
@@ -97890,10 +98264,13 @@
         <v>1382</v>
       </c>
       <c r="M108" s="8">
-        <v>1.65</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1.4</v>
+      </c>
+      <c r="O108" t="s">
+        <v>8908</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>5570</v>
       </c>
@@ -97928,7 +98305,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>5582</v>
       </c>
@@ -97963,7 +98340,7 @@
         <v>5.35</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>5684</v>
       </c>
@@ -97998,7 +98375,7 @@
         <v>8.91</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>5810</v>
       </c>
@@ -98033,7 +98410,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>5824</v>
       </c>
@@ -98067,8 +98444,11 @@
       <c r="M113" s="8">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O113" t="s">
+        <v>8914</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>5834</v>
       </c>
@@ -98100,7 +98480,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>5905</v>
       </c>
@@ -98132,7 +98512,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>5920</v>
       </c>
@@ -98167,7 +98547,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>5958</v>
       </c>
@@ -98202,7 +98582,7 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>5959</v>
       </c>
@@ -98237,7 +98617,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>6101</v>
       </c>
@@ -98272,7 +98652,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>6163</v>
       </c>
@@ -98307,7 +98687,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>6393</v>
       </c>
@@ -98342,7 +98722,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>6399</v>
       </c>
@@ -98377,7 +98757,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>6451</v>
       </c>
@@ -98409,7 +98789,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>6479</v>
       </c>
@@ -98444,7 +98824,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>6522</v>
       </c>
@@ -98479,7 +98859,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>6590</v>
       </c>
@@ -98517,7 +98897,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>6624</v>
       </c>
@@ -98551,8 +98931,11 @@
       <c r="M127" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O127" t="s">
+        <v>8915</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>6630</v>
       </c>
@@ -98897,6 +99280,79 @@
       </c>
       <c r="O137" t="s">
         <v>7204</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>8869</v>
+      </c>
+      <c r="B138" t="s">
+        <v>8872</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E138" t="s">
+        <v>6647</v>
+      </c>
+      <c r="H138" t="s">
+        <v>8871</v>
+      </c>
+      <c r="I138" t="s">
+        <v>4889</v>
+      </c>
+      <c r="J138" t="s">
+        <v>8870</v>
+      </c>
+      <c r="K138" t="s">
+        <v>5573</v>
+      </c>
+      <c r="L138" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M138" s="8">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>8912</v>
+      </c>
+      <c r="B139" t="s">
+        <v>8913</v>
+      </c>
+      <c r="C139" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E139" t="s">
+        <v>8911</v>
+      </c>
+      <c r="H139" t="s">
+        <v>5388</v>
+      </c>
+      <c r="I139" t="s">
+        <v>21</v>
+      </c>
+      <c r="J139" t="s">
+        <v>8910</v>
+      </c>
+      <c r="K139" t="s">
+        <v>6402</v>
+      </c>
+      <c r="L139" t="s">
+        <v>2418</v>
+      </c>
+      <c r="M139" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="O139" t="s">
+        <v>8909</v>
       </c>
     </row>
   </sheetData>
@@ -100412,10 +100868,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -100434,7 +100890,7 @@
     <col min="12" max="12" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -100477,8 +100933,11 @@
       <c r="N1" t="s">
         <v>5483</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>7173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -100517,7 +100976,7 @@
       </c>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2281</v>
       </c>
@@ -100553,7 +101012,7 @@
       </c>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2345</v>
       </c>
@@ -100583,7 +101042,7 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2411</v>
       </c>
@@ -100616,7 +101075,7 @@
       </c>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2428</v>
       </c>
@@ -100646,7 +101105,7 @@
       </c>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2513</v>
       </c>
@@ -100682,7 +101141,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2532</v>
       </c>
@@ -100709,7 +101168,7 @@
       </c>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2553</v>
       </c>
@@ -100739,7 +101198,7 @@
       </c>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2561</v>
       </c>
@@ -100760,7 +101219,7 @@
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2595</v>
       </c>
@@ -100790,7 +101249,7 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2604</v>
       </c>
@@ -100820,7 +101279,7 @@
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2892</v>
       </c>
@@ -100850,7 +101309,7 @@
       </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4276</v>
       </c>
@@ -100886,7 +101345,7 @@
       </c>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4308</v>
       </c>
@@ -100927,7 +101386,7 @@
         <v>11.15</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4511</v>
       </c>
@@ -102133,7 +102592,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6200</v>
       </c>
@@ -102171,7 +102630,7 @@
         <v>10.220000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>6275</v>
       </c>
@@ -102206,7 +102665,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>6387</v>
       </c>
@@ -102244,7 +102703,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>6418</v>
       </c>
@@ -102267,7 +102726,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6438</v>
       </c>
@@ -102305,7 +102764,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6467</v>
       </c>
@@ -102339,8 +102798,11 @@
       <c r="M54" s="8">
         <v>1.56</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O54" t="s">
+        <v>8921</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>6488</v>
       </c>
@@ -102369,7 +102831,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>6496</v>
       </c>
@@ -102404,7 +102866,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6502</v>
       </c>
@@ -102442,7 +102904,7 @@
         <v>4.3099999999999996</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>6516</v>
       </c>
@@ -102480,7 +102942,7 @@
         <v>5.71</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>6532</v>
       </c>
@@ -102518,7 +102980,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>6551</v>
       </c>
@@ -102556,7 +103018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>6574</v>
       </c>
@@ -102594,7 +103056,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>6749</v>
       </c>
@@ -102632,7 +103094,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>6750</v>
       </c>
@@ -102670,7 +103132,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>6785</v>
       </c>
@@ -105010,10 +105472,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -105027,7 +105489,7 @@
     <col min="7" max="7" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -105049,8 +105511,11 @@
       <c r="G1" s="8" t="s">
         <v>4494</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>7173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2565</v>
       </c>
@@ -105070,7 +105535,7 @@
         <v>2563</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2568</v>
       </c>
@@ -105089,8 +105554,14 @@
       <c r="F3" t="s">
         <v>2566</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="8">
+        <v>1.01</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8916</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2571</v>
       </c>
@@ -105110,7 +105581,7 @@
         <v>2569</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2577</v>
       </c>
@@ -105130,7 +105601,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2967</v>
       </c>
@@ -105150,7 +105621,7 @@
         <v>4317</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4293</v>
       </c>
@@ -105170,7 +105641,7 @@
         <v>4304</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4296</v>
       </c>
@@ -105190,7 +105661,7 @@
         <v>4304</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4300</v>
       </c>
@@ -105210,7 +105681,7 @@
         <v>4303</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4305</v>
       </c>
@@ -105230,7 +105701,7 @@
         <v>4303</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4335</v>
       </c>
@@ -105253,7 +105724,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4338</v>
       </c>
@@ -105273,7 +105744,7 @@
         <v>4337</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4506</v>
       </c>
@@ -105296,7 +105767,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4574</v>
       </c>
@@ -105319,7 +105790,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4707</v>
       </c>
@@ -105342,7 +105813,7 @@
         <v>2.87</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4828</v>
       </c>
@@ -105712,7 +106183,7 @@
         <v>40106</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>5886</v>
       </c>
@@ -105732,7 +106203,7 @@
         <v>4518</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5887</v>
       </c>
@@ -105752,7 +106223,7 @@
         <v>4018</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5888</v>
       </c>
@@ -105772,7 +106243,7 @@
         <v>4001</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5942</v>
       </c>
@@ -105792,7 +106263,7 @@
         <v>5940</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>5944</v>
       </c>
@@ -105815,7 +106286,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>6125</v>
       </c>
@@ -105838,7 +106309,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>6175</v>
       </c>
@@ -105861,7 +106332,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6284</v>
       </c>
@@ -105884,7 +106355,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>6407</v>
       </c>
@@ -105907,7 +106378,7 @@
         <v>8.19</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>6512</v>
       </c>
@@ -105929,8 +106400,11 @@
       <c r="G42" s="8">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>8918</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6552</v>
       </c>
@@ -105953,7 +106427,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6594</v>
       </c>
@@ -105975,8 +106449,11 @@
       <c r="G44" s="8">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" t="s">
+        <v>8919</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>6841</v>
       </c>
@@ -105999,7 +106476,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>7026</v>
       </c>
@@ -106022,7 +106499,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>7095</v>
       </c>
@@ -106045,7 +106522,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>7130</v>
       </c>

</xml_diff>

<commit_message>
Add chunky inductor for ROV
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="763" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28116" windowHeight="16440" tabRatio="763" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22026" uniqueCount="8922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22045" uniqueCount="8937">
   <si>
     <t>Part Number</t>
   </si>
@@ -26797,6 +26806,51 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/texas-instruments/TPS2066DGNR/684822</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nichicon/UVR2A101MPD/588889</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nichicon/UVR1V471MPD/588825</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-semiconductor/MM3Z16VST1G/1481864</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-semiconductor/FSV15150V/5306664?s=N4IgTCBcDaIGIGUBqBGArOgDEkBdAvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/phoenix-contact/1991095/2527261?s=N4IgTCBcDaIIwE4FwAwIKwgLoF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/IHLP3232DZERR33M01/2657475?s=N4IgTCBcDaIJIAkAyAFAzGDARAWgUQCUC00BZABgEYQBdAXyA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-siliconix/SUM90140E-GE3/6708888?s=N4IgTCBcDaIMoFUCyBOADARgCxoKIFoBxXAZhAF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-semiconductor/2SC6017-TL-E/2797038</t>
+  </si>
+  <si>
+    <t>MAG-00138</t>
+  </si>
+  <si>
+    <t>EPCOS</t>
+  </si>
+  <si>
+    <t>B82559A7682A024</t>
+  </si>
+  <si>
+    <t>EPCOS_B82559AXA024</t>
+  </si>
+  <si>
+    <t>1.45mOhm</t>
+  </si>
+  <si>
+    <t>Ind, 6.8uH, 35A (37.9A sat.), 1.45mOhm, EPCOS - TDK</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/epcos-tdk-electronics/B82559A7682A024/13165559</t>
   </si>
 </sst>
 </file>
@@ -64145,7 +64199,7 @@
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -65601,10 +65655,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -66787,7 +66841,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>5431</v>
       </c>
@@ -66825,7 +66879,7 @@
         <v>2.84</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5577</v>
       </c>
@@ -66862,8 +66916,11 @@
       <c r="L34" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" t="s">
+        <v>8928</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5655</v>
       </c>
@@ -66898,7 +66955,7 @@
         <v>5660</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5661</v>
       </c>
@@ -66936,7 +66993,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>5690</v>
       </c>
@@ -66973,8 +67030,11 @@
       <c r="L37" s="8">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" t="s">
+        <v>8929</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>5776</v>
       </c>
@@ -67012,7 +67072,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>6120</v>
       </c>
@@ -67050,7 +67110,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6132</v>
       </c>
@@ -67088,7 +67148,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>6213</v>
       </c>
@@ -67126,7 +67186,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>6266</v>
       </c>
@@ -67164,7 +67224,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6351</v>
       </c>
@@ -67202,7 +67262,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6356</v>
       </c>
@@ -67240,7 +67300,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>6362</v>
       </c>
@@ -67278,7 +67338,7 @@
         <v>7.91</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>6692</v>
       </c>
@@ -67316,7 +67376,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6696</v>
       </c>
@@ -67354,7 +67414,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>6708</v>
       </c>
@@ -67554,8 +67614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView topLeftCell="C55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N74" sqref="N74"/>
+    <sheetView topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68144,7 +68204,7 @@
       </c>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2192</v>
       </c>
@@ -68180,7 +68240,7 @@
       </c>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2193</v>
       </c>
@@ -68216,7 +68276,7 @@
       </c>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>2194</v>
       </c>
@@ -68252,7 +68312,7 @@
       </c>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>2195</v>
       </c>
@@ -68288,7 +68348,7 @@
       </c>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>2196</v>
       </c>
@@ -68324,7 +68384,7 @@
       </c>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>2197</v>
       </c>
@@ -68360,7 +68420,7 @@
       </c>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2198</v>
       </c>
@@ -68396,7 +68456,7 @@
       </c>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>2199</v>
       </c>
@@ -68432,7 +68492,7 @@
       </c>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>2200</v>
       </c>
@@ -68468,7 +68528,7 @@
       </c>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>2201</v>
       </c>
@@ -68504,7 +68564,7 @@
       </c>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>2202</v>
       </c>
@@ -68538,9 +68598,11 @@
       <c r="L27" s="2" t="s">
         <v>2129</v>
       </c>
-      <c r="M27" s="8"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N27" s="8" t="s">
+        <v>8924</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2203</v>
       </c>
@@ -68576,7 +68638,7 @@
       </c>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>2204</v>
       </c>
@@ -68612,7 +68674,7 @@
       </c>
       <c r="M29" s="8"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>2205</v>
       </c>
@@ -68648,7 +68710,7 @@
       </c>
       <c r="M30" s="8"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>2206</v>
       </c>
@@ -68684,7 +68746,7 @@
       </c>
       <c r="M31" s="8"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>2207</v>
       </c>
@@ -69549,6 +69611,9 @@
       </c>
       <c r="M56" s="8">
         <v>0.82</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>8925</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
@@ -70835,7 +70900,7 @@
   <dimension ref="A1:M121"/>
   <sheetViews>
     <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M63" sqref="M63"/>
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72572,6 +72637,9 @@
       <c r="K55" s="8">
         <v>1.23</v>
       </c>
+      <c r="M55" t="s">
+        <v>8926</v>
+      </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -74773,8 +74841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L595"/>
   <sheetViews>
-    <sheetView topLeftCell="A576" workbookViewId="0">
-      <selection activeCell="B596" sqref="B596"/>
+    <sheetView topLeftCell="A269" workbookViewId="0">
+      <selection activeCell="K285" sqref="K285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -82720,7 +82788,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>1946</v>
       </c>
@@ -82753,7 +82821,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>1947</v>
       </c>
@@ -82786,7 +82854,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>1948</v>
       </c>
@@ -82819,7 +82887,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>1949</v>
       </c>
@@ -82852,7 +82920,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>1950</v>
       </c>
@@ -82884,8 +82952,11 @@
       <c r="J245" t="s">
         <v>2079</v>
       </c>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K245" s="8" t="s">
+        <v>8922</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>1951</v>
       </c>
@@ -82918,7 +82989,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>1952</v>
       </c>
@@ -82951,7 +83022,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>1953</v>
       </c>
@@ -82984,7 +83055,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>1954</v>
       </c>
@@ -83017,7 +83088,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>1955</v>
       </c>
@@ -83050,7 +83121,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>1956</v>
       </c>
@@ -83083,7 +83154,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>1957</v>
       </c>
@@ -83116,7 +83187,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>1958</v>
       </c>
@@ -83149,7 +83220,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>1959</v>
       </c>
@@ -83182,7 +83253,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>1960</v>
       </c>
@@ -83215,7 +83286,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>1961</v>
       </c>
@@ -84304,7 +84375,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>1994</v>
       </c>
@@ -84336,8 +84407,11 @@
       <c r="J289" t="s">
         <v>2079</v>
       </c>
-    </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K289" s="8" t="s">
+        <v>8923</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>1995</v>
       </c>
@@ -84370,7 +84444,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>1996</v>
       </c>
@@ -84403,7 +84477,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>1997</v>
       </c>
@@ -84436,7 +84510,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>1998</v>
       </c>
@@ -84469,7 +84543,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>1999</v>
       </c>
@@ -84502,7 +84576,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>2000</v>
       </c>
@@ -84535,7 +84609,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>2001</v>
       </c>
@@ -84568,7 +84642,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>2002</v>
       </c>
@@ -84601,7 +84675,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>2003</v>
       </c>
@@ -84634,7 +84708,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>2004</v>
       </c>
@@ -84667,7 +84741,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>2005</v>
       </c>
@@ -84700,7 +84774,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>2006</v>
       </c>
@@ -84733,7 +84807,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>2007</v>
       </c>
@@ -84766,7 +84840,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>2008</v>
       </c>
@@ -84799,7 +84873,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>2009</v>
       </c>
@@ -94581,16 +94655,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O139"/>
+  <dimension ref="A1:O140"/>
   <sheetViews>
-    <sheetView topLeftCell="C104" workbookViewId="0">
-      <selection activeCell="O125" sqref="O125"/>
+    <sheetView tabSelected="1" topLeftCell="C128" workbookViewId="0">
+      <selection activeCell="O141" sqref="O141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -98004,6 +98078,9 @@
       <c r="M100" s="8">
         <v>1.65</v>
       </c>
+      <c r="O100" t="s">
+        <v>8927</v>
+      </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
@@ -99353,6 +99430,44 @@
       </c>
       <c r="O139" t="s">
         <v>8909</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>8930</v>
+      </c>
+      <c r="B140" t="s">
+        <v>8935</v>
+      </c>
+      <c r="C140" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="E140" t="s">
+        <v>4548</v>
+      </c>
+      <c r="H140" t="s">
+        <v>8934</v>
+      </c>
+      <c r="I140" t="s">
+        <v>8931</v>
+      </c>
+      <c r="J140" t="s">
+        <v>8932</v>
+      </c>
+      <c r="K140" t="s">
+        <v>8933</v>
+      </c>
+      <c r="L140" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M140" s="8">
+        <v>8.19</v>
+      </c>
+      <c r="O140" t="s">
+        <v>8936</v>
       </c>
     </row>
   </sheetData>
@@ -99372,7 +99487,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -100870,14 +100985,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B19" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.21875" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
@@ -100885,7 +101000,7 @@
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.44140625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Add 1.87k 0603 resistor and a few ceramic capacitors
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28116" windowHeight="16440" tabRatio="763" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28116" windowHeight="16440" tabRatio="763" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22045" uniqueCount="8937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22075" uniqueCount="8949">
   <si>
     <t>Part Number</t>
   </si>
@@ -26851,6 +26851,42 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/epcos-tdk-electronics/B82559A7682A024/13165559</t>
+  </si>
+  <si>
+    <t>RES-01232</t>
+  </si>
+  <si>
+    <t>1.87k</t>
+  </si>
+  <si>
+    <t>RC0603FR-071K87L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603FR-071K87L/726876</t>
+  </si>
+  <si>
+    <t>RES SMD 1.87K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CAP-00594</t>
+  </si>
+  <si>
+    <t>CL31B225KCHSNNE</t>
+  </si>
+  <si>
+    <t>can_single_np</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL31B225KCHSNNE/3888796</t>
+  </si>
+  <si>
+    <t>CL32A476KOJNNNE</t>
+  </si>
+  <si>
+    <t>CAP-00595</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL32A476KOJNNNE/3889034</t>
   </si>
 </sst>
 </file>
@@ -27232,10 +27268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1233"/>
+  <dimension ref="A1:K1234"/>
   <sheetViews>
-    <sheetView topLeftCell="A1204" workbookViewId="0">
-      <selection activeCell="K1234" sqref="K1234"/>
+    <sheetView topLeftCell="A1225" workbookViewId="0">
+      <selection activeCell="B1235" sqref="B1235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -64176,6 +64212,41 @@
       </c>
       <c r="K1233" t="s">
         <v>8868</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1234" t="s">
+        <v>8937</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>8941</v>
+      </c>
+      <c r="C1234" s="1" t="s">
+        <v>8938</v>
+      </c>
+      <c r="D1234" t="s">
+        <v>2818</v>
+      </c>
+      <c r="E1234" t="s">
+        <v>5814</v>
+      </c>
+      <c r="F1234" t="s">
+        <v>2611</v>
+      </c>
+      <c r="G1234" t="s">
+        <v>8939</v>
+      </c>
+      <c r="H1234" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1234" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1234" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="K1234" t="s">
+        <v>8940</v>
       </c>
     </row>
   </sheetData>
@@ -74839,10 +74910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L595"/>
+  <dimension ref="A1:L597"/>
   <sheetViews>
-    <sheetView topLeftCell="A269" workbookViewId="0">
-      <selection activeCell="K285" sqref="K285"/>
+    <sheetView tabSelected="1" topLeftCell="A580" workbookViewId="0">
+      <selection activeCell="L598" sqref="L598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -94647,6 +94718,84 @@
         <v>8890</v>
       </c>
     </row>
+    <row r="596" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A596" t="s">
+        <v>8942</v>
+      </c>
+      <c r="B596" t="str">
+        <f>CONCATENATE("CAP",", ",C596,", ",D596,", ",E596,", ",F596,", 1206")</f>
+        <v>CAP, 2.2uF, ±10%, 100V, X7R, 1206</v>
+      </c>
+      <c r="C596" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D596" t="s">
+        <v>4344</v>
+      </c>
+      <c r="E596" t="s">
+        <v>944</v>
+      </c>
+      <c r="F596" t="s">
+        <v>20</v>
+      </c>
+      <c r="G596" t="s">
+        <v>5112</v>
+      </c>
+      <c r="H596" t="s">
+        <v>8943</v>
+      </c>
+      <c r="I596" t="s">
+        <v>1471</v>
+      </c>
+      <c r="J596" t="s">
+        <v>8944</v>
+      </c>
+      <c r="K596" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L596" t="s">
+        <v>8945</v>
+      </c>
+    </row>
+    <row r="597" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A597" t="s">
+        <v>8947</v>
+      </c>
+      <c r="B597" t="str">
+        <f>CONCATENATE("CAP",", ",C597,", ",D597,", ",E597,", ",F597,", 1210")</f>
+        <v>CAP, 47uF, ±10%, 16V, X5R, 1210</v>
+      </c>
+      <c r="C597" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D597" t="s">
+        <v>4344</v>
+      </c>
+      <c r="E597" t="s">
+        <v>19</v>
+      </c>
+      <c r="F597" t="s">
+        <v>4326</v>
+      </c>
+      <c r="G597" t="s">
+        <v>5112</v>
+      </c>
+      <c r="H597" t="s">
+        <v>8946</v>
+      </c>
+      <c r="I597" t="s">
+        <v>4325</v>
+      </c>
+      <c r="J597" t="s">
+        <v>8944</v>
+      </c>
+      <c r="K597" s="8">
+        <v>0.81</v>
+      </c>
+      <c r="L597" t="s">
+        <v>8948</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -94657,8 +94806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C128" workbookViewId="0">
-      <selection activeCell="O141" sqref="O141"/>
+    <sheetView topLeftCell="C128" workbookViewId="0">
+      <selection activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix Capacitor library errors, add a few nice 1008 power inductors
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28116" windowHeight="16440" tabRatio="763" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28116" windowHeight="16440" tabRatio="763" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22075" uniqueCount="8949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22119" uniqueCount="8969">
   <si>
     <t>Part Number</t>
   </si>
@@ -26874,9 +26874,6 @@
     <t>CL31B225KCHSNNE</t>
   </si>
   <si>
-    <t>can_single_np</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL31B225KCHSNNE/3888796</t>
   </si>
   <si>
@@ -26887,6 +26884,69 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL32A476KOJNNNE/3889034</t>
+  </si>
+  <si>
+    <t>MAG-00139</t>
+  </si>
+  <si>
+    <t>MAG-00140</t>
+  </si>
+  <si>
+    <t>MAG-00141</t>
+  </si>
+  <si>
+    <t>MAG-00142</t>
+  </si>
+  <si>
+    <t>Ind, 2.2uH, 2.2A (3A sat.), 84mOhm, 1008</t>
+  </si>
+  <si>
+    <t>84mOhm</t>
+  </si>
+  <si>
+    <t>DFE252012P-2R2M=P2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/DFE252012P-2R2M=P2/5247260</t>
+  </si>
+  <si>
+    <t>Ind, 1uH, 4.3A, 42mOhm, 1008</t>
+  </si>
+  <si>
+    <t>4.3A</t>
+  </si>
+  <si>
+    <t>42mOhm</t>
+  </si>
+  <si>
+    <t>DFE252012P-1R0M=P2</t>
+  </si>
+  <si>
+    <t>Ind, 3.3uH, 2.3A, 140mOhm, 1008</t>
+  </si>
+  <si>
+    <t>140mOhm</t>
+  </si>
+  <si>
+    <t>DFE252012P-3R3M=P2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/DFE252012P-3R3M=P2/5247261</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/DFE252012P-1R0M=P2/5247258</t>
+  </si>
+  <si>
+    <t>60mOhm</t>
+  </si>
+  <si>
+    <t>DFE252012P-1R5M=P2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/DFE252012P-1R5M=P2/5247259</t>
+  </si>
+  <si>
+    <t>Ind, 1.5uH, 3.5A, 60mOhm, 1008</t>
   </si>
 </sst>
 </file>
@@ -74912,8 +74972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A580" workbookViewId="0">
-      <selection activeCell="L598" sqref="L598"/>
+    <sheetView topLeftCell="H576" workbookViewId="0">
+      <selection activeCell="J598" sqref="J598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -94748,18 +94808,18 @@
         <v>1471</v>
       </c>
       <c r="J596" t="s">
-        <v>8944</v>
+        <v>23</v>
       </c>
       <c r="K596" s="8">
         <v>0.55000000000000004</v>
       </c>
       <c r="L596" t="s">
-        <v>8945</v>
+        <v>8944</v>
       </c>
     </row>
     <row r="597" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
-        <v>8947</v>
+        <v>8946</v>
       </c>
       <c r="B597" t="str">
         <f>CONCATENATE("CAP",", ",C597,", ",D597,", ",E597,", ",F597,", 1210")</f>
@@ -94781,19 +94841,19 @@
         <v>5112</v>
       </c>
       <c r="H597" t="s">
-        <v>8946</v>
+        <v>8945</v>
       </c>
       <c r="I597" t="s">
         <v>4325</v>
       </c>
       <c r="J597" t="s">
-        <v>8944</v>
+        <v>23</v>
       </c>
       <c r="K597" s="8">
         <v>0.81</v>
       </c>
       <c r="L597" t="s">
-        <v>8948</v>
+        <v>8947</v>
       </c>
     </row>
   </sheetData>
@@ -94804,10 +94864,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O140"/>
+  <dimension ref="A1:O144"/>
   <sheetViews>
-    <sheetView topLeftCell="C128" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+    <sheetView tabSelected="1" topLeftCell="C127" workbookViewId="0">
+      <selection activeCell="K145" sqref="K145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -99617,6 +99677,158 @@
       </c>
       <c r="O140" t="s">
         <v>8936</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>8948</v>
+      </c>
+      <c r="B141" t="s">
+        <v>8952</v>
+      </c>
+      <c r="C141" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E141" t="s">
+        <v>2264</v>
+      </c>
+      <c r="H141" t="s">
+        <v>8953</v>
+      </c>
+      <c r="I141" t="s">
+        <v>21</v>
+      </c>
+      <c r="J141" t="s">
+        <v>8954</v>
+      </c>
+      <c r="K141" t="s">
+        <v>6397</v>
+      </c>
+      <c r="L141" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M141" s="8">
+        <v>0.38</v>
+      </c>
+      <c r="O141" t="s">
+        <v>8955</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>8949</v>
+      </c>
+      <c r="B142" t="s">
+        <v>8956</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E142" t="s">
+        <v>8957</v>
+      </c>
+      <c r="H142" t="s">
+        <v>8958</v>
+      </c>
+      <c r="I142" t="s">
+        <v>21</v>
+      </c>
+      <c r="J142" t="s">
+        <v>8959</v>
+      </c>
+      <c r="K142" t="s">
+        <v>6397</v>
+      </c>
+      <c r="L142" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M142" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="O142" t="s">
+        <v>8964</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>8950</v>
+      </c>
+      <c r="B143" t="s">
+        <v>8960</v>
+      </c>
+      <c r="C143" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E143" t="s">
+        <v>6165</v>
+      </c>
+      <c r="H143" t="s">
+        <v>8961</v>
+      </c>
+      <c r="I143" t="s">
+        <v>21</v>
+      </c>
+      <c r="J143" t="s">
+        <v>8962</v>
+      </c>
+      <c r="K143" t="s">
+        <v>6397</v>
+      </c>
+      <c r="L143" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M143" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="O143" t="s">
+        <v>8963</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>8951</v>
+      </c>
+      <c r="B144" t="s">
+        <v>8968</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E144" t="s">
+        <v>5832</v>
+      </c>
+      <c r="H144" t="s">
+        <v>8965</v>
+      </c>
+      <c r="I144" t="s">
+        <v>21</v>
+      </c>
+      <c r="J144" t="s">
+        <v>8966</v>
+      </c>
+      <c r="K144" t="s">
+        <v>6397</v>
+      </c>
+      <c r="L144" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M144" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="O144" t="s">
+        <v>8967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>